<commit_message>
Update legal_questions_answers.xlsx with new or modified data
</commit_message>
<xml_diff>
--- a/query/legal_questions_answers.xlsx
+++ b/query/legal_questions_answers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,1749 +473,1966 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jak mogę ubiegać się o tymczasowe zezwolenie na pobyt w Dolnośląskiem?</t>
+          <t>Jakie mam prawa jako zagraniczny pracownik w Polskim?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-czasowy/pobyt-czasowy-i-praca/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00214</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Kto składa wniosek?
-Kiedy powinienem / powinnam złożyć wniosek?
-Jak mogę złożyć wniosek?
-Jakie dokumenty muszę złożyć?
-Jakie są opłaty?</t>
+          <t>Niezależnie od tego, czy zatrudniasz cudzoziemca w Polsce czy też delegujesz go do świadczenia usług na terytorium Polski, jako podmiot powierzający wykonanie pracy musisz zapewnić warunki zatrudnienia, które są zgodne z polskimi przepisami. Jeśli cudzoziemiec jest zatrudniony/delegowany do Polski i wykonuje pracę na podstawie umowy o pracę, to zasadą jest, że jego warunki zatrudnienia nie mogą być mniej korzystne niż te, które gwarantują polskie przepisy prawa pracy . norm i wymiaru czasu pracy oraz okresów odpoczynku dobowego i tygodniowego,</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-czasowy/zezwolenie-na-pobyt-czasowy-w-celu-wykonywania-pracy-przez-cudzoziemca-w-ramach-przeniesienie-wewnatrz-przedsiebiorstwa/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00198</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Kto składa wniosek?
-Kiedy powinienem / powinnam złożyć wniosek?
-Jak mogę złożyć wniosek?
-Jakie dokumenty muszę złożyć?
-Jakie są opłaty?</t>
+          <t>Obowiązki pracodawcy delegującego pracownika z kraju trzeciego Pracodawca delegujący z siedzibą w kraju trzecim zobowiązany jest przestrzegać: wszystkich przepisów związanych z delegowaniem pracownika na terytorium Polski</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://pro4work.pl/zlozenie-wniosku-na-karte-pobytu-krok-po-kroku/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/004330</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Złożenie wniosku na kartę pobytu w Dolnośląskim Urzędzie Wojewódzkim we Wrocławiu w celu legalizacji pobytu i pracy jest obecnie dużym problemem dla Cudzoziemca. Na ten moment jedyną możliwością, aby złożyć wniosek na kartę pobytu w Dolnośląskim Urzędzie Wojewódzkim jest rejestracja poprzez “SYSTEM REZERWACJI WIZYT DOLNOŚLĄSKIEGO URZĘDU WOJEWÓDZKIEGO”.
-Cudzoziemcy nie mogą już składać wniosku na kartę pobytu udając się do Urzędu i pobierając odpowiedni bilet z biletomatu, tak jak miało to miejsce kilka miesięcy temu. Pamiętajmy, że wniosek legalizujący pobyt składa się w trakcie legalnego pobytu cudzoziemca w Polsce.
-Pierwszym etapem w celu rozpoczęcia procedury złożenia wniosku o wydanie decyzji na pobyt czasowy (karta pobytu) jest rejestracja konta użytkownika na stronie:
-https://rezerwacje.duw.pl/reservations/pol/login
-</t>
+          <t>Cudzoziemiec, który jest obywatelem państwa spoza Unii Europejskiej , Europejskiego Obszaru Gospodarczego lub Szwajcarii może legalnie pracować w Polsce, pod warunkiem że łącznie spełnia następujące warunki: legalnie przebywa na terytorium Polski, to znaczy posiada odpowiednie dokumenty pobytowe jeżeli nie jest zwolniony z obowiązku posiadania zezwolenia na pracę, to: uzyska zezwolenie na pobyt czasowy i pracę albo pracodawca uzyska dla niego zezwolenie na pracę, zezwolenie na pracę sezonową lub złoży oświadczenie o powierzeniu pracy cudzoziemcowi dokumenty pobytowe pozwalają mu na wykonywanie pracy jego praca odbywa się na warunkach oraz stanowisku, które zostały określone w zezwoleniu na pracę, oświadczeniu o powierzeniu pracy lub zezwoleniu na pobyt czasowy i pracę .</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Jakie są wymagania dotyczące stałego pobytu w Dolnośląskiem?</t>
+          <t>Jakie usługi są dostępne w urzędzie dla cudzoziemców?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-staly/</t>
+          <t>https://www.gov.pl/web/udsc/rodzaje-przyznawanej-pomocy</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Kto składa wniosek?
-Kiedy powinienem / powinnam złożyć wniosek?
-Jak mogę złożyć wniosek?
-Jakie dokumenty muszę złożyć?
-Jakie są opłaty?</t>
+          <t>zwrot kosztów za przejazdy środkami komunikacji publicznej w określonych przypadkach tj. związanych z postępowaniem o nadanie statusu uchodźcy, stawieniem się na badania lekarskie lub szczepienia ochronne czy w innych uzasadnionych przypadkach; stałą pomoc pieniężną na zakup środków higieny osobistej – 20 PLN miesięcznie oraz tzw. „kieszonkowe” – 50 PLN miesięcznie; zapewnienie jednorazowej pomocy pieniężnej na zakup odzieży i obuwia – 140 PLN;</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://firmadlakazdego.pl/jak-uzyskac-karte-stalego-pobytu-w-polsce/</t>
+          <t>https://www.gov.pl/web/udsc/zadania-realizowane-przez-urzad-do-spraw-cudzoziemcow</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>17 października 2024
-Proces uzyskania karty stałego pobytu
-Wymagania do karty stałego pobytu
-Dokumenty potrzebne do karty stałego pobytu</t>
+          <t>Szef Urzędu do Spraw Cudzoziemców, jako centralny organ administracji rządowej, realizuje następujące zadania: rozpatruje odwołania od decyzji wojewodów w sprawach legalizacji pobytu - zezwoleń na pobyt dla cudzoziemców, wiz i zaproszeń, rejestracji pobytu i prawa stałego pobytu obywateli Unii Europejskiej oraz członków ich rodzin, a także kontroluje wojewodów w tym zakresie; prowadzi konsultacje wizowe oraz dokonuje wymiany danych pomiędzy państwami członkowskimi na temat wiz;</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://migrant.wsc.mazowieckie.pl/pl/procedury/wydanie-karty-pobytu-na-wniosek</t>
+          <t>https://www.katowice.uw.gov.pl/usluga/cudzoziemcy</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Przejdź do menu głównego
-Przejdź do treści
-Dostępność
-Strona główna
-Procedury</t>
+          <t>"ŚLĄSKIE DLA CUDZOZIEMCÓW" Projekt FAMI.02.01-IZ.00-0002/24 dofinansowany ze środków Funduszu Azylu, Migracji i Integracji na lata 2021-2027 Pobyt czasowy, stały, rezydenta długoterminowego UE, wizy, świadczenia pieniężne dla posiadaczy Karty Polaka TRYB SKŁADANIA WNIOSKÓW POBYTOWYCH - REZERWACJA INTERNETOWA</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Czy mogę pracować w Dolnośląskiem na wizie studenckiej?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+          <t>Jakie są konsekwencje przekroczenia terminu ważności wizy w Polskim?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/attachment/c4067bab-e664-4072-8be5-6c90367ab4e3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Zobowiązanie cudzoziemca do powrotu - Rozdział 2 - ustawy Kontrola legalności pobytu cudzoziemców na terytorium ... Pouczenie dla cudzoziemca o zasadach i trybie postępowania ...</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://pckp.pl/baza-wiedzy/jak-legalnie-zatrudnic-cudzoziemca-bedacego-studentem-polskiej-uczelni/</t>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/ruch-cudzoziemcow-16868620</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Zgoda
-Szczegóły
-[#IABV2SETTINGS#]
-O plikach cookies
-Niezbędne  12 Niezbędne pliki cookie przyczyniają się do użyteczności strony poprzez umożliwianie podstawowych funkcji takich jak nawigacja na stronie i dostęp do bezpiecznych obszarów strony internetowej. Strona internetowa nie może funkcjonować poprawnie bez tych ciasteczek.Cookiebot1Dowiedz się więcej na temat tego dostawcyCookieConsentStores the user's cookie consent state for the current domainMaksymalny okres przechowywania: 1 rokRodzaj: Plik cookie HTTPGoogle4Dowiedz się więcej na temat tego dostawcyNiektóre dane gromadzone przez tego dostawcę służą do personalizacji i pomiaru skuteczności reklamy.test_cookieUsed to check if the user's browser supports cookies.Maksymalny okres przechowywania: 1 dzieńRodzaj: Plik cookie HTTPar_debugChecks whether a technical debugger-cookie is present. Maksymalny okres przechowywania: 3 miesięcyRodzaj: Plik cookie HTTPrc::aThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maksymalny okres przechowywania: StałeRodzaj: Lokalny magazyn HTMLrc::cThis cookie is used to distinguish between humans and bots. Maksymalny okres przechowywania: SesyjneRodzaj: Lokalny magazyn HTMLLinkedIn2Dowiedz się więcej na temat tego dostawcybcookieUsed in order to detect spam and improve the website's security. Maksymalny okres przechowywania: 1 rokRodzaj: Plik cookie HTTPli_gcStores the user's cookie consent state for the current domainMaksymalny okres przechowywania: 180 dniRodzaj: Plik cookie HTTPSales Manago1Dowiedz się więcej na temat tego dostawcySERVERIDThis cookie is used to assign the visitor to a specific server - this function is necessary for the functionality of the website.Maksymalny okres przechowywania: SesyjneRodzaj: Plik cookie HTTPVimeo2Dowiedz się więcej na temat tego dostawcy__cf_bmThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maksymalny okres przechowywania: 1 dzieńRodzaj: Plik cookie HTTP_cfuvidThis cookie is a part of the services provided by Cloudflare - Including load-balancing, deliverance of website content and serving DNS connection for website operators. Maksymalny okres przechowywania: SesyjneRodzaj: Plik cookie HTTPpckp.pl2storeApiNonceNecessary for the shopping cart functionality on the website.Maksymalny okres przechowywania: StałeRodzaj: Lokalny magazyn HTMLwpEmojiSettingsSupportsThis cookie is part of a bundle of cookies which serve the purpose of content delivery and presentation. The cookies keep the correct state of font, blog/picture sliders, color themes and other website settings.Maksymalny okres przechowywania: SesyjneRodzaj: Lokalny magazyn HTML</t>
+          <t>ROZPORZĄDZENIE MINISTRA SPRAW WEWNĘTRZNYCH z dnia 8 listopada 1929 r. o ruchu cudzoziemców, wydane co do §§ 1, 2, 3, 4, 5, 9, 10, 11, 13, 14, 15, 16, 17, 20, 21, 24, 38, 40, 41, 42, 43, 44, 47, 52 i 53 w porozumieniu z Ministrem Spraw Zagranicznych. Wiza pobytowa może uprawniać do wielokrotnego przekraczania granic Rzeczypospolitej. Wizy pobytowej do odwołania urząd konsularny udziela natomiast wówczas, gdy cel pobytu jest tego rodzaju, że czas, potrzebny dla osiągnięcia go, nie da się określić nawet w przybliżeniu.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://klubjagiellonski.pl/2025/03/18/w-polsce-jest-az-107-tys-studentow-z-zagranicy-to-szansa-czy-moze-zagrozenie/</t>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/cudzoziemcy-18053962/dz-8-roz-2</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>W Polsce rośnie liczba studentów zagranicznych – w minionym roku akademickim uczyło się ich już w naszym kraju ponad 107 tys. Studiują w równym stopniu na uczelniach prywatnych i publicznych, a najczęściej wybierane przez nich kierunki to zarządzanie, informatyka i kierunek lekarski. Czy wzrost liczby cudzoziemców studiujących na naszych uczelniach to pozytywne zjawisko i czy jako społeczeństwo możemy na tym skorzystać?
-Przegląd corocznych raportów Studenci zagraniczni w Polsce autorstwa fundacji Study in Poland współpracującej z magazynem Perspektywy nie pozostawia wątpliwości: liczba studentów zagranicznych w Polsce dynamicznie rośnie. Podczas gdy na początku tego stulecia w naszym kraju uczyło się nieco ponad 6,5 tys. obcokrajowców, w roku akademickim 2023/2024 ta liczba przekroczyła 107 tys. osób.
-Kwestia studentów zagranicznych na polskich uczelniach znalazła się w obiektywie opinii publicznej w związku z ogłoszeniem strategii migracyjnej na lata 2025-2030 przez rząd Donalda Tuska na jesieni zeszłego roku. Dokument ten zapowiada walkę z niekontrolowaną migracją spoza krajów OECD, co w perspektywie może rykoszetem dotknąć również te osoby, które do Polski chciałyby przyjechać w celu realizacji swoich pasji naukowych.
-Żyła złota dla uczelni?</t>
+          <t>Rozdział 2 - Zobowiązanie cudzoziemca do powrotu - Cudzoziemcy. - stała się ostateczna, a w przypadku wydania decyzji przez organ wyższego stopnia - od dnia, w którym decyzja została cudzoziemcowi doręczona; Organ prowadzący postępowanie w sprawie zobowiązania cudzoziemca do powrotu poucza cudzoziemca o możliwości złożenia wniosku o udzielenie ochrony międzynarodowej.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Jak długo mogę pozostać w Dolnośląskiem po wygaśnięciu wizy?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+          <t>Jak zgłosić narodziny dziecka w Polsce?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/zglos-urodzenie-dziecka</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Jeśli urodzi ci się dziecko, trzeba je zgłosić do odpowiedniego urzędu stanu cywilnego . Kierownik urzędu zarejestruje urodzenie dziecka, przekaże ci jego numer PESEL i zamelduje je. Sprawdź, jak zgłosić urodzenie dziecka –przez internet lub w urzędzie. Jeśli chcesz zgłosić urodzenie dziecka przez internet – potrzebujesz profilu zaufanego lub e-dowodu. Pozwalają one potwierdzić twoją tożsamość. Sprawdź, jak założyć profil zaufany lub jak skorzystać z e-dowodu.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/cyfryzacja/co-jest-potrzebne-by-zglosic-narodziny-dziecka-imie-i-internet</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Co jest potrzebne, by zgłosić narodziny dziecka? Imię i… internet! Jaś, Bożydar, Grześ, Kociemir – wybór imienia dla dziecka nie zawsze jest łatwy. Bardzo proste jest za to zgłoszenie narodzin nowego członka rodziny. Najłatwiej i najszybciej można to zrobić przez internet – na GOV.pl. Od dziś w telewizji i internecie możecie obejrzeć nasz najnowszy spot, w którym zachęcamy do skorzystania z tej możliwości. To kolejna odsłona naszej kampanii „e-Polak potrafi!”.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://archiwum.mswia.gov.pl/pl/sprawy-obywatelskie/rejestracja-stanu-cywi/12970,Jak-zarejestrowac-urodzenie-malzenstwo-zgon.html</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Formy zawarcia związku małżeńskiego Zawarcie małżeństwa przed kierownikiem urzędu stanu cywilnego ślub poza Urzędem Stanu Cywilnego Przed duchownym – małżeństwo wyznaniowe wywierające skutki cywilno-prawne przed konsulem Ślub poza urzędem stanu cywilnego​ Zawarcie małżeństwa przed kierownikiem urzędu stanu cywilnego ślub poza Urzędem Stanu Cywilnego Przed duchownym – małżeństwo wyznaniowe wywierające skutki cywilno-prawne przed konsulem</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Jakie są konsekwencje przekroczenia terminu ważności wizy w Dolnośląskiem?</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+          <t>Jak mogę ubiegać się o tymczasowe zezwolenie na pobyt w Polskim?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00210</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Procedura uzyskania zezwolenia na pobyt czasowy i pracę, czyli zezwolenie jednolite jest korzystna, bo wszystkie formalności legalizujące pobyt i zatrudnienie cudzoziemca odbywają się w ramach jednego postępowania administracyjnego - cudzoziemiec nie musi odrębnie ubiegać się o zezwolenie na pobyt , a pracodawca - o zezwolenie na pracę. Wojewoda, który udzielił jednolitego zezwolenia na pobyt czasowy i pracę na terytorium Polski, wydaje cudzoziemcowi z urzędu kartę pobytu. Karta pobytu, w okresie w którym jest ważna, potwierdza tożsamość cudzoziemca oraz uprawnia go, wraz z dokumentem podróży, do wielokrotnego przekraczania granicy bez konieczności uzyskania wizy.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://biznes.gov.pl/pl/portal/ou1613</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Uzyskaj zezwolenie na pobyt czasowy w celu wykonywania pracy w zawodzie wymagającym wysokich kwalifikacji Jesteś cudzoziemcem, posiadasz wysokie kwalifikacje zawodowe i chcesz pracować w Polsce? Dowiedz się jak uzyskać zezwolenie na pobyt czasowy w Polsce w celu wykonywania pracy wymagającej wysokich kwalifikacji. Co powinieneś wiedzieć i kto może skorzystać z usługi</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/uw-warminsko-mazurski/cudzoziemcy---zezwolenia-na-pobyt-czasowy-na-terytorium-rp</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Szczegółowe informacje znajdziesz na stronie Urzędu do Spraw Cudzoziemców w Module Obsługi Spraw pod linkiem: https://www.mos.cudzoziemcy.gov.pl/potrzebuje-informacji/pobyt-czas https://mos.cudzoziemcy.gov.pl/potrzebuje-informacji/szczegolne-okol</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Czy potrzebuję zezwolenia na pracę w Dolnośląskiem?</t>
+          <t>Czy mogę pracować w Polskim na wizie studenckiej?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-praca/zezwolenie-na-prace/</t>
+          <t>https://zielonalinia.gov.pl/-/student-cudzoziemiec-a-obowiazek-posiadania-zezwolenia-na-prace</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jakie dokumenty muszę złożyć (według typów zezwoleń)?
-Jak mogę złożyć wniosek?
-Jakie są opłaty?
-Co powinienem wiedzieć?
-</t>
+          <t>Kwestię zwolnienia z obowiązku posiadania przez cudzoziemca z kraju trzeciego zezwolenia na pracę regulują przepisy ustawy o promocji zatrudnienia i instytucjach rynku pracy oraz rozporządzenie Ministra Pracy i Polityki Społecznej w sprawie przypadków, w których powierzenie wykonywania pracy cudzoziemcowi na terytorium Rzeczypospolitej Polskiej jest dopuszczalne bez konieczności uzyskania zezwolenia na pracę. O studentach czytamy w § 1 pkt 10 ww. rozporządzenia. Zgodnie z tym przepisem powierzenie cudzoziemcowi wykonywania pracy na terytorium Rzeczypospolitej Polskiej bez konieczności uzyskania zezwolenia na pracę jest dopuszczalne w przypadku cudzoziemców będących studentami studiów stacjonarnych odbywanych w Rzeczypospolitej Polskiej lub uczestnikami stacjonarnych studiów doktoranckich odbywanych w Rzeczypospolitej Polskiej. Czytaj także: Podstawowy obowiązek pracodawcy, który chce zatrudnić cudzoziemca</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-czasowy/pobyt-czasowy-i-praca/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/004330</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Kto składa wniosek?
-Kiedy powinienem / powinnam złożyć wniosek?
-Jak mogę złożyć wniosek?
-Jakie dokumenty muszę złożyć?
-Jakie są opłaty?</t>
+          <t>Cudzoziemiec, który jest obywatelem państwa spoza Unii Europejskiej , Europejskiego Obszaru Gospodarczego lub Szwajcarii może legalnie pracować w Polsce, pod warunkiem że łącznie spełnia następujące warunki: legalnie przebywa na terytorium Polski, to znaczy posiada odpowiednie dokumenty pobytowe jeżeli nie jest zwolniony z obowiązku posiadania zezwolenia na pracę, to: uzyska zezwolenie na pobyt czasowy i pracę albo pracodawca uzyska dla niego zezwolenie na pracę, zezwolenie na pracę sezonową lub złoży oświadczenie o powierzeniu pracy cudzoziemcowi dokumenty pobytowe pozwalają mu na wykonywanie pracy jego praca odbywa się na warunkach oraz stanowisku, które zostały określone w zezwoleniu na pracę, oświadczeniu o powierzeniu pracy lub zezwoleniu na pobyt czasowy i pracę .</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://askor.waw.pl/zezwolenie-na-prace-wroclaw/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/004330#1</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Zezwolenie na pracę Wrocław – kogo dotyczy ?
-Jeśli zatrudniasz cudzoziemców spoza UE, EOG i Szwajcarii, będziesz potrzebował zezwolenia na pracę dla swoich pracowników.  Zezwolenie na pracę wydawane jest przez właściwego wojewodę. W związku z tym, wniosek o zezwolenie na pracę składa pracodawca do urzędu wojewódzkiego. Jeżeli siedziba lub miejsce zamieszkania pracodawcy znajduje się na terytorium województwa dolnośląskiego, wtedy bez wątpienia wniosek o zezwolenie można złożyć w Dolnośląskim Urzędzie Wojewódzkim. Wniosek o wydanie zezwolenia na pracę typ A dotyczy cudzoziemca wykonującego pracę na terytorium Polski na podstawie umowy z podmiotem. Zezwolenie to dotyczy pracy wykonywanej w tego konkretnego pracodawcy. Trzeba pamiętać, że nie jest ono ważne w przypadku zatrudnienia w innego pracodawcy. Jednocześnie, zatrudniając cudzoziemca trzeba wiedzieć jakiego zezwolenia na pracę potrzebujesz.
-Sprawdź rodzaje zezwoleń na pracę &gt;&gt;
-Wniosek o zezwolenie na pracę dla cudzoziemca należy złożyć przez Dolnośląski Urząd Wojewódzki we Wrocławiu. O zezwolenie na pracę Wrocław można starać się osobiście lub zamówić przez serwis internetowy online.
-Zezwolenia na pracę dla cudzoziemca || zamów &gt;&gt;</t>
+          <t>Cudzoziemiec, który jest obywatelem państwa spoza Unii Europejskiej , Europejskiego Obszaru Gospodarczego lub Szwajcarii może legalnie pracować w Polsce, pod warunkiem że łącznie spełnia następujące warunki: legalnie przebywa na terytorium Polski, to znaczy posiada odpowiednie dokumenty pobytowe jeżeli nie jest zwolniony z obowiązku posiadania zezwolenia na pracę, to: uzyska zezwolenie na pobyt czasowy i pracę albo pracodawca uzyska dla niego zezwolenie na pracę, zezwolenie na pracę sezonową lub złoży oświadczenie o powierzeniu pracy cudzoziemcowi dokumenty pobytowe pozwalają mu na wykonywanie pracy jego praca odbywa się na warunkach oraz stanowisku, które zostały określone w zezwoleniu na pracę, oświadczeniu o powierzeniu pracy lub zezwoleniu na pobyt czasowy i pracę .</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Jak mogę uzyskać zezwolenie na pracę jako obywatel spoza UE w Dolnośląskiem?</t>
+          <t>Czy cudzoziemiec może otworzyć firmę w Polskim?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://migrant.wsc.mazowieckie.pl/pl/faq/wydaniewymiana-karty-pobytu</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00806</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Przejdź do menu głównego
-Przejdź do treści
-Dostępność
-Strona główna
-zezwolenie na pobyt czasowy w celu połączenia się z rodziną, a w dniu złożenia wniosku o udzielenie tego zezwolenia przebywałeś poza granicami Rzeczypospolitej Polskiej,</t>
+          <t>Kto może prowadzić działalność gospodarczą w Polsce Obywatele państw członkowskich Unii Europejskiej oraz Europejskiego Obszaru Gospodarczego, którzy chcą wykonywać w Polsce działalność gospodarczą, mogą: założyć własną firmę jednoosobową lub dowolną spółkę handlową</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://infoopt.pl/ogolne-zasady-zatrudniania-cudzoziemcow-w-polsce/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/0613</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Zasady pobytu obywateli państw trzecich na terytorium RP określa ustawa z dnia 12 grudnia 2013 r. o cudzoziemcach, natomiast zasady ich zatrudnienia określają przepisy ustawy z 20 kwietnia 2004 r. o promocji zatrudnienia i instytucjach rynku pracy.
-przebywać legalnie na terytorium RP, czyli posiadać jeden z poniższych dokumentów, tj.:
-Ważną wizę*
-Zezwolenie na pobyt,
-Stempel w paszporcie potwierdzający fakt złożenia wniosku o pobyt czasowy,</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+          <t>Kto może prowadzić działalność gospodarczą w Polsce Polskie przepisy przewidują dużą swobodę prowadzenia działalności gospodarczej, co oznacza, że w większości wypadków możesz założyć firmę i prowadzić ją w wybranej przez siebie formie. Przeczytaj, kiedy trzeba spełnić dodatkowe warunki. Sprawdź, czy firmę może otworzyć cudzoziemiec, osoba niepełnoletnia lub emeryt. Firma cudzoziemca Zakładanie firmy jednoosobowej Polskie przepisy przewidują dużą swobodę prowadzenia działalności gospodarczej, co oznacza, że w większości wypadków możesz założyć firmę i prowadzić ją w wybranej przez siebie formie. Przeczytaj, kiedy trzeba spełnić dodatkowe warunki. Sprawdź, czy firmę może otworzyć cudzoziemiec, osoba niepełnoletnia lub emeryt. Jak delegować do Polski pracowników w ramach świadczenia usług Sprawdź na czym polega delegowanie w ramach świadczenia usług, jakie są zasady i obowiązki pracodawców delegujących, kiedy pracownik jest pracownikiem delegowanym. Firma cudzoziemca Delegowanie Obowiązki pracodawcy Zatrudnienie pracownika</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/001466</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Obywatel Ukrainy, który przebywa w Polsce legalnie i posiada numer PESEL, może założyć działalność gospodarczą na takich samych zasadach jak obywatel Polski w dowolnej formie. firmę jednoosobową – czyli działalność gospodarczą osoby fizycznej – i zarejestrować ją w CEIDG spółkę osobową lub kapitałową – w tym spółkę jawną i partnerską – i zarejestrować ją w KRS.</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Jakie mam prawa jako zagraniczny pracownik w Dolnośląskiem?</t>
+          <t>Jak przedłużyć wizę w Polsce?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/cudzoziemcy/pit-11-czy-ift-1r-jak-rozliczyc-cudzoziemca</t>
+          <t>https://migrant.poznan.uw.gov.pl/pl/procedury/przedluzenie-wizy-krajowej</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Styczeń to ważny miesiąc dla pracodawców. Mają oni obowiązek dostarczenia do Urzędu Skarbowego odpowiednich deklaracji podatkowych. Zatrudniając osoby z Polski, sprawa jest oczywista – pracodawca wystawia PIT-11. Wątpliwości pojawiają się natomiast w przypadku zatrudnienia obcokrajowców. Jak rozliczyć osoby fizyczne niemające miejsca zamieszkania w Polsce? Jaką deklarację roczną wystawić cudzoziemcowi zatrudnionemu na oświadczeniu o powierzeniu wykonywania pracy cudzoziemcowi lub na podstawie zezwolenia na pracę? Odpowiadamy w artykule.
-&gt;&gt; Przetestuj bezpłatnie system kadrowo – płacowy
-Zagadnienia poruszane w artykule:
-Pierwszym i najważniejszym krokiem jest ustalenie rezydencji podatkowej obcokrajowca. Określa ona, w którym kraju jako pierwszym powinien być odprowadzany podatek od dochodu.
-Dla celów podatkowych polski rezydent podatkowy to osoba, która mieszka w Polsce więcej niż 183 dni w roku lub osoba, która przebywa tu krócej, ale posiada w Polsce centrum interesów osobistych, życiowych i gospodarczych. Taka osoba podlega tzw. nieograniczonemu obowiązkowi podatkowemu.</t>
+          <t>Wniosek o przedłużenie wizy krajowej składasz najpóźniej w ostatnim dniu ważności wizy, którą posiadasz. Jeżeli złożysz wniosek w terminie i nie będzie w nim braków formalnych lub braki formalne uzupełnisz we wskazanym przez nas terminie, Twój pobyt będzie legalny od dnia złożenia wniosku do dnia, w którym decyzja w tej sprawie stanie się ostateczna. Przed złożeniem wniosku przeczytaj nasze wskazówki dotyczące wypełniania formularzy wniosków</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/pit-2-dla-cudzoziemca-co-warto-wiedziec</t>
+          <t>https://www.katowice.uw.gov.pl/usluga/cudzoziemcy/przedluzenie-wizy-schengen-lub-wizy-krajowej</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Autor
-Andrzej Tkaczuk
-Specjalista ds. legalizacji
-cudzoziemców</t>
+          <t>I Kto może starać się o przedłużenie wizy Jeżeli jesteś cudzoziemcem przebywającym na terytorium Rzeczypospolitej Polskiej możesz ubiegać się o przedłużenie okresu ważności wydanej przez organ polski wizy krajowej lub okresu pobytu objętego tą wizą. Jeżeli jesteś cudzoziemcem przebywającym na terytorium Rzeczypospolitej Polskiej, możesz ubiegać się o przedłużenie okresu ważności wydanej przez organ polski lub organ innego państwa obszaru Schengen wizy Schengen ważnej również na terytorium Polski lub długości pobytu objętego tą wizą. Jeżeli jesteś cudzoziemcem przebywającym na terytorium Rzeczypospolitej Polskiej możesz ubiegać się o przedłużenie okresu ważności wydanej przez organ polski wizy krajowej lub okresu pobytu objętego tą wizą. Jeżeli jesteś cudzoziemcem przebywającym na terytorium Rzeczypospolitej Polskiej, możesz ubiegać się o przedłużenie okresu ważności wydanej przez organ polski lub organ innego państwa obszaru Schengen wizy Schengen ważnej również na terytorium Polski lub długości pobytu objętego tą wizą. II Dokumenty Cudzoziemiec ubiegający się o przedłużenie wizy Schengen lub wizy krajowej obowiązany jest: złożyć wypełniony formularz wniosku o przedłużenie wizy Schengen lub wizy krajowej , przedstawić ważny dokument podróży, uzasadnić wniosek oraz dołączyć do wniosku: 1. aktualną fotografię – nieuszkodzoną, kolorową, o wymiarach 35 x 45 mm, wykonaną w ciągu ostatnich 6 miesięcy na jednolitym jasnym tle, mającą dobrą ostrość oraz pokazującą wyraźnie oczy i twarz od wierzchołka głowy do górnej części barków, tak aby twarz zajmowała 70-80 % fotografii; fotografia powinna przedstawiać osobę bez nakrycia głowy i okularów z ciemnymi szkłami, patrzącą na wprost z otwartymi oczami, nieprzesłoniętymi włosami, z naturalnym wyrazem twarzy i zamkniętymi ustami; ✸ Uwaga! Cudzoziemiec noszący nakrycie głowy zgodnie z zasadami swojego wyznania może dołączyć do wniosku fotografię przedstawiającą go w nakryciu głowy, o ile wizerunek twarzy jest w pełni widoczny. W takim przypadku do wniosku dołącza się oświadczenie cudzoziemca o przynależności do wspólnoty wyznaniowej. 2. dokumenty potwierdzające: - cel pobytu i konieczność przedłużenia wizy Schengen lub wizy krajowej, - posiadanie wystarczających środków finansowych na pokrycie kosztów utrzymania przez cały okres planowanego pobytu na terytorium Rzeczypospolitej Polskiej oraz na podróż powrotną do państwa pochodzenia lub zamieszkania albo na tranzyt do państwa trzeciego, które udzieli pozwolenia na wjazd, albo możliwość uzyskania takich środków zgodnie z prawem, - wiarygodność deklaracji o zamiarze opuszczenia terytorium Polski przed upływem terminu ważności wizy, - posiadanie ubezpieczenia zdrowotnego w rozumieniu ustawy z dnia 27 sierpnia 2004r. o świadczeniach opieki zdrowotnej finansowanych ze środków publicznych lub podróżnego ubezpieczenia medycznego o minimalnej kwocie ubezpieczenia w wysokości 30 000 euro, ważnego przez okres planowanego pobytu cudzoziemca na terytorium Rzeczypospolitej Polskiej, pokrywającego wszelkie wydatki, które mogą wyniknąć podczas pobytu na tym terytorium w związku z koniecznością powrotu z powodów medycznych, potrzebą pilnej pomocy medycznej, nagłym leczeniem szpitalnym lub ze śmiercią, w którym ubezpieczyciel zobowiązuje się do pokrycia kosztów udzielonych ubezpieczonemu świadczeń zdrowotnych bezpośrednio na rzecz podmiotu udzielającego takich świadczeń, na podstawie wystawionego przez ten podmiot rachunku - inne okoliczności podane we wniosku, - wykonanie obowiązku meldunkowego. Cudzoziemiec ubiegający się o przedłużenie wizy Schengen lub wizy krajowej przedstawia do wglądu dokument podróży spełniający kryteria: 1) jego okres ważności upłynie nie wcześniej niż po 3 miesiącach od upływu okresu ważności wizy, o którą się ubiega ; 2) zawiera przynajmniej dwie wolne strony; 3) został wydany w ciągu ostatnich 10 lat. Zał.1 - Formularz wniosku o przedłużenie wizy SchengenZał. 2 - Formularz wniosku o przedłużenie wizy krajowejZał. 3 - RODO Klauzula informacyjna Zał. 4 - RODO Klauzula informacyjna Szefa Urzędu ds. Cudzoziemców</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://centrumverte.pl/blog/rozliczenie-cudzoziemca-w-polsce-pit-11-czy-ift-1r/</t>
+          <t>https://www.gov.pl/web/uw-pomorski/przedluzenie-wizy-pobytowej</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Cenimy prywatność użytkowników
-Używamy plików cookie, aby poprawić jakość przeglądania, wyświetlać reklamy lub treści dostosowane do indywidualnych potrzeb użytkowników oraz analizować ruch na stronie. Kliknięcie przycisku „Akceptuj wszystkie” oznacza zgodę na wykorzystywanie przez nas plików cookie.
-Używamy plików cookie, aby pomóc użytkownikom w sprawnej nawigacji i wykonywaniu określonych funkcji. Szczegółowe informacje na temat wszystkich plików cookie odpowiadających poszczególnym kategoriom zgody znajdują się poniżej.
-Pliki cookie sklasyfikowane jako „niezbędne” są przechowywane w przeglądarce użytkownika, ponieważ są niezbędne do włączenia podstawowych funkcji witryny.... Pokaż więcej
-Niezbędne pliki cookie mają kluczowe znaczenie dla podstawowych funkcji witryny i witryna nie będzie działać w zamierzony sposób bez nich.Te pliki cookie nie przechowują żadnych danych umożliwiających identyfikację osoby.</t>
+          <t>Informacje zawarte w niniejszej karcie nie stanowią źródła prawa. Mają jedynie charakter ogólny i instrukcyjny. Wniosek o przedłużenie wizy krajowej należy złożyć najpóźniej w ostatnim dniu ważności wizy. Wizę krajową można przedłużyć jednokrotnie, przy czym okres pobytu na podstawie przedłużonej wizy krajowej nie może przekraczać okresu pobytu przewidzianego dla wizy krajowej, czyli 1 roku. Podstawa prawna: rozdział 2 działu IV ustawy z dnia 12 grudnia 2013 r. o cudzoziemcach oraz art. 33 rozporządzenia Parlamentu Europejskiego i Rady nr 810/2009 z dnia 13 lipca 2009 r. ustanawiającego Wspólnotowy Kodeks Wizowy.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Jak mogę zgłosić pracodawcę, który nie wypłaca mi wynagrodzenia w Dolnośląskiem?</t>
+          <t>Jak mogę zarejestrować narodziny mojego dziecka w Polskim?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.sdworx.pl/pl-pl/blog/place/nieterminowa-wyplata-wynagrodzenia</t>
+          <t>https://www.gov.pl/web/gov/zglos-urodzenie-dziecka</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Home&gt;
-Blog&gt;
-Płace&gt;
-Co, jeśli pracodawca spóźnia się z wypłatą? Skutki nieterminowej wypłaty wynagrodzenia
-Wynagrodzenie to priorytet dla 55% pracowników z całego świata. Niestety, niemal 30% kadry kierowniczej średniego i wyższego szczebla przyznaje, że często – lub zawsze! – otrzymuje zaniżoną płacę – wynika z raportu „People at Work 2024: A Global Workforce View” ADP Research Institute. Błędy na listach płac to jedne z wielu problemów, z którymi zmagają się pracownicy. PIP (Państwowa Inspekcja Pracy) otrzymała ok. 16 tysięcy skarg związanych z wypłatą wynagrodzenia oraz innych świadczeń w 2023 roku. Jakie działania może podjąć pracownik, gdy pracodawca spóźnia się z wypłatą? Sprawdź konsekwencje nieterminowej wypłaty wynagrodzenia na gruncie prawnym.</t>
+          <t>Jeśli urodzi ci się dziecko, trzeba je zgłosić do odpowiedniego urzędu stanu cywilnego . Kierownik urzędu zarejestruje urodzenie dziecka, przekaże ci jego numer PESEL i zamelduje je. Sprawdź, jak zgłosić urodzenie dziecka –przez internet lub w urzędzie. Jeśli chcesz zgłosić urodzenie dziecka przez internet – potrzebujesz profilu zaufanego lub e-dowodu. Pozwalają one potwierdzić twoją tożsamość. Sprawdź, jak założyć profil zaufany lub jak skorzystać z e-dowodu.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.gazetaprawna.pl/praca/artykuly/9722231,mobbing-w-polsce-najnowsze-dane-pip.html</t>
+          <t>https://www.gov.pl/web/cyfryzacja/rejestracja-narodzin-dziecka-online</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reklama
-Państwowa Inspekcja Pracy podsumowała najważniejsze dane dotyczące mobbingu. W 2024 roku udzielono 1367 porad prawnych w tym zakresie w porównaniu do 829 porad udzielonych w 2023 roku. O co najczęściej pytali pracownicy?
-Jak podano, wątpliwości zatrudnionych krążyły wokół problemów związanych z gromadzeniem dowodów potwierdzających jego występowanie w środowisku pracy czy procedurami wewnątrzzakładowymi. Pracownicy pytali również o możliwość uzyskania wsparcia inspektorów czy o kwestię dochodzenia roszczeń w tym zakresie przed sądem.
-Inspekcja, jak podano w komunikacie, wspiera ofiary mobbingu również wtedy, gdy zdecydują się na podjęcie kroków prawnych i chcą uzyskać odszkodowanie za doznane krzywdy.
-</t>
+          <t>Profil zaufany i kilka minut - to wszystko czego potrzeba, by zarejestrować narodziny dziecka online. Nowa usługa ruszyła 1 czerwca 2018 r. - to prezent na Dzień Dziecka od Ministerstwa Cyfryzacji. Na zarejestrowanie narodzin dziecka rodzice mają 21 dni od dnia wystawienia karty urodzenia. Do tej pory mieli tylko jedną opcję - wizyta w urzędzie. Od teraz będą mieli wybór - pędzić do urzędu czy spędzić ten czas z nowym członkiem rodziny. Prościej, szybciej i wygodniej - to najkrótszy opis uruchamianej usługi. Jak z niej skorzystać? Cały proces to 5 prostych kroków.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://poradnikpracownika.pl/-niewyplacone-wynagrodzenie-za-prace-czyli-jak-odzyskac-nalezna-wyplate</t>
+          <t>https://www.gov.pl/web/cyfryzacja/co-jest-potrzebne-by-zglosic-narodziny-dziecka-imie-i-internet</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>PoradnikPracownika
-ZAROBKI
-Wynagrodzenia
-Niewypłacone wynagrodzenie za pracę, czyli jak odzyskać należną wypłatę</t>
+          <t>Co jest potrzebne, by zgłosić narodziny dziecka? Imię i… internet! Jaś, Bożydar, Grześ, Kociemir – wybór imienia dla dziecka nie zawsze jest łatwy. Bardzo proste jest za to zgłoszenie narodzin nowego członka rodziny. Najłatwiej i najszybciej można to zrobić przez internet – na GOV.pl. Od dziś w telewizji i internecie możecie obejrzeć nasz najnowszy spot, w którym zachęcamy do skorzystania z tej możliwości. To kolejna odsłona naszej kampanii „e-Polak potrafi!”.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Co powinno być zawarte w mojej umowie o pracę w Dolnośląskiem?</t>
+          <t>Jak nostryfikować dyplom w Polsce?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.bankier.pl/wiadomosc/Umowa-o-prace-wszystko-co-powinienes-o-niej-wiedziec-700002.html</t>
+          <t>https://nawa.gov.pl/uznawalnosc/informacje-dla-uczelni/nostryfikacja-dyplomow</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Umowa o pracę zobowiązuje obie strony, czyli pracownika i pracodawcę do wypełniania względem siebie określonych obowiązków. Każdej ze stron umowy
-przysługują też pewne przywileje. Typy umów o pracę są zaś różne. Pracownik
-powinien dobrze zapoznać się z przepisami dotyczącymi zawierania stosunków
-pracy, aby uniknąć błędów i nieporozumień.
-Podpisując umowę o pracę,
-zobowiązujemy się do wykonywania określonego rodzaju pracy na rzecz pracodawcy
-i pod jego kierownictwem. Druga strona umowy, czyli pracodawca, zobowiązuje się
-zapewnić pracownikowi wynagrodzenie za pracę. Nie można jednak mówić o stosunku
-pracy, jeśli nie zaistniały określone przesłanki, takie jak podporządkowanie
-pracownika poleceniom pracodawcy, świadczenie pracy osobiście, wykonywanie
-pracy za wynagrodzeniem, w miejscu i czasie wyznaczonym przez pracodawcę.
-Istotnym czynnikiem jest również powtarzalność wykonywania pracy i obciążenie
-pracodawcy ryzykiem prowadzonej działalności i zatrudniania osób.
-Od 2016 roku w Kodeksie pracy wyróżnia się trzy rodzaje umów o pracę: umowę na okres próbny, na czas określony i na czas nieokreślony.
-Kodeks pracy wyróżnia też kilka
-typów umów o pracę. Pierwsza z nich to umowa
-na okres próbny, która ma na celu sprawdzić kwalifikacje pracownika w
-praktyce. Pracownik może dzięki niej zapoznać się z warunkami i organizacją
-pracy w danej firmie. Trzeba jednak pamiętać, że zatrudnienie na jej podstawie
-nie może trwać dłużej niż 3 miesiące. Drugim typem umowy o pracę, jest umowa na czas określony. Zmiany w zakresie podejmowania tego rodzaju umowy wprowadzono w 2016 roku. W wyniku zmian nie można zawierać dowolnie długie umowy na czas określony. Obecnie taki kontrakt nie może zostać zawarty na dłużej niż 33 miesiące pomiędzy tym samym pracodawcą i pracownikiem. Kolejną zmianą jest limit umów na czas określony - po 2016 roku można zawrzeć maksymalnie 3 takie umowy, w przypadku przekroczenia tego terminu uznaje się, że pracownik jest zatrudniony na czas nieokreślony. Wspomnianego limitu nie stosuje się do umów terminowych, o których mowa poniżej.
-Z
-punktu widzenia pracownika najkorzystniejsza jest jednak umowa na czas nieokreślony, która zapewnia największą ochronę przed
-zwolnieniem. Można ją wypowiedzieć bez zachowania okresu wypowiedzenia tylko z uzasadnionych przyczyn</t>
+          <t>1. Czym jest nostryfikacja Нострифікація дипломів про вищу освіту Nostryfikacja to procedura prowadząca do ustalenia polskiego odpowiednika zagranicznego dyplomu. Nostryfikacji podlega dyplom ukończenia studiów za granicą, który nie może być uznany za równoważny odpowiedniemu polskiemu dyplomowi i tytułowi zawodowemu na podstawie umowy międzynarodowej określającej równoważność . Postępowanie nostryfikacyjne odbywa się na podstawie rozporządzenia Ministra Nauki i Szkolnictwa Wyższego z dnia 28 września 2018 r. w sprawie nostryfikacji dyplomów ukończenia studiów za granicą oraz w sprawie potwierdzenia ukończenia studiów na określonym poziomie</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://poradnikprzedsiebiorcy.pl/-umowa-o-prace</t>
+          <t>https://www.gov.pl/web/zdrowie/uzyskaj-nostryfikacje-dyplomu-szkoly-wyzszej1</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Serwis Kadrowy
-Prawo pracy
-Umowa o pracę - poznaj podstawowe informacje
-umowa o pracę</t>
+          <t>Jeżeli masz dyplom ukończenia szkoły wyższej uzyskany w państwie spoza Unii Europejskiej, możesz go uznać za równorzędny z jego polskim odpowiednikiem. Nostryfikacją dyplomów, które potwierdzają kwalifikacje do wykonywania zawodów medycznych, zajmują się uczelnie medyczne – uprawnione do nadawania stopnia naukowego doktora nauk medycznych. Uwaga: Jeśli uzyskałeś za granicą dyplom potwierdzający ukończenie studiów wyższych, na które zostałeś skierowany zgodnie z obowiązującymi w tym zakresie przepisami, dyplom ten zostanie uznany bez postępowania nostryfikacyjnego.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/umowa-o-prace-wzor</t>
+          <t>https://nawa.gov.pl/uznawalnosc/podjecie-pracy-w-polsce/dyplom-z-innego-kraju</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Pracodawca, który zamierza zatrudnić pracownika na podstawie stosunku pracy, zobowiązany jest do podpisania z nim umowy o pracę. Powinny znaleźć się w niej informacje zarówno o pracodawcy (nazwa firmy, NIP, adres, osoba reprezentująca), jak i pracowniku (imię, nazwisko, miejsce zamieszkania). Umowę o pracę zawiera się na czas próbny, określony lub nieokreślony.
-Dane do umowy zbierane są najczęściej przy pomocy kwestionariusza osobowego. Najszybszym sposobem jest wysyłka ankiety do zatrudnienia przy pomocy systemu kadrowo – płacowego. Dzięki temu, przyszły pracownik sam uzupełni swoje dane do umowy. Stworzony zostanie profil pracownika, do którego automatycznie zaciągną się dane z ankiety. Podobnie z umową – nie ma potrzeby ręcznego przepisywania danych.
-Dodatkową zaletą zawierania umowy o pracę przy pomocy odpowiedniego systemu jest oszczędność czasu podczas przekazywania dokumentu do podpisu. Korzystając np. z podpisu elektronicznego możemy szybko nawiązać stosunek pracy, tym samym przyspieszając termin rozpoczęcia pracy.
-&gt;&gt; Przetestuj bezpłatnie system kadrowo – płacowy
-Zagadnienia poruszane w artykule:</t>
+          <t>Dyplom ukończenia studiów wyższych lub tytuł zawodowy uzyskany za granicą może być uznany za równoważny z polskim odpowiednikiem na podstawie umowy międzynarodowej, a w przypadku jej braku – w drodze nostryfikacji. Uzyskane za granicą dyplomy nie mogą zostać w Polsce uznane, jeśli: instytucje, które je wydały lub instytucje, w których prowadzone było kształcenie: nie były akredytowanymi uczelniami w dniu wydania dyplomu lub realizowały program studiów nieposiadający akredytacji w dniu wydania dyplomu; nie działają w systemie szkolnictwa wyższego żadnego państwa;</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Czy cudzoziemiec może otworzyć firmę w Dolnośląskiem?</t>
+          <t>Jak mogę uzyskać PESEL do celów podatkowych w Polskim?</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-czasowy/dzialalnosc-gospodarcza/</t>
+          <t>https://www.gov.pl/web/gov/uzyskaj-numer-pesel-dla-cudzoziemcow</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Kto składa wniosek?
-Kiedy powinienem / powinnam złożyć wniosek?
-Jak mogę złożyć wniosek?
-Jakie dokumenty muszę złożyć?
-Jakie są opłaty?</t>
+          <t>Jeśli jesteś cudzoziemcem, który mieszka w Polsce, możesz zameldować się – wtedy automatycznie dostaniesz numer PESEL. Jeśli nie możesz zameldować się, a jakiś urząd wymaga od ciebie numeru PESEL – złóż wniosek. Sprawdź, jak to zrobić. Rozwiń tekst Kto może uzyskać Dostaniesz numer PESEL z urzędu – jeśli zameldujesz się w Polsce na pobyt powyżej 30 dni. Złóż wniosek w dowolnym urzędzie gminy – jeśli nie możesz się zameldować, a potrzebujesz numeru PESEL. Dostaniesz numer PESEL z urzędu – jeśli zameldujesz się w Polsce na pobyt powyżej 30 dni.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.migrant.info.pl/pl/strona-glowna-2/dzialalnosc-gospodarcza/mozliwosc-prowadzenia-dzialalnosci-gospodarczej-przez-cudzoziemcow</t>
+          <t>https://www.podatki.gov.pl/abc-podatkow/wyjasnienia/od-1-maja-cudzoziemcy-moga-wystapic-o-nadanie-pesel-do-celow-podatkowych/</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Pragniemy zwrócić Państwa uwagę, że zamieszczone na niniejszej stronie informacje nie stanowią źródła prawa. Zapewniamy, że dołożyliśmy wszelkich starań, by były one zgodne z obowiązującymi regulacjami. Prosimy jednak pamiętać, że niniejsza strona służy wyłącznie celom informacyjnym, a informacje na niej zamieszczone nie mogą stanowić podstawy w sporach z organami administracji publicznej. W razie wątpliwości zalecamy skontaktowanie się z organem prowadzącym postępowanie administracyjne w danej sprawie oraz zapoznanie się z przepisami prawa, które mogą mieć decydujący wpływ na jej rozstrzygnięcie. Zapraszamy również do kontaktu z prowadzoną przez nas infolinią migrant.info - +48 22 490 20 44
-Pragniemy zwrócić Państwa uwagę, że zamieszczone na niniejszej stronie informacje nie stanowią źródła prawa. Zapewniamy, że dołożyliśmy wszelkich starań, by były one zgodne z obowiązującymi regulacjami. Prosimy jednak pamiętać, że niniejsza strona służy wyłącznie celom informacyjnym, a informacje na niej zamieszczone nie mogą stanowić podstawy w sporach z organami administracji publicznej. W razie wątpliwości zalecamy skontaktowanie się z organem prowadzącym postępowanie administracyjne w danej sprawie oraz zapoznanie się z przepisami prawa, które mogą mieć decydujący wpływ na jej rozstrzygnięcie. Zapraszamy również do kontaktu z prowadzoną przez nas infolinią migrant.info - +48 22 490 20 44</t>
+          <t>Od 1 czerwca cudzoziemcy mogą wystąpić o nadanie PESEL do celów podatkowych 1 czerwca 2021 r. wchodzi w życie zmiana ustawy o zasadach ewidencji i identyfikacji podatników i płatników w zakresie definicji podatników, których identyfikatorem podatkowym jest PESEL. Dzięki nowym przepisom urzędy gminy będą mogły nadawać numer PESEL cudzoziemcom na ich wniosek.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://symfonia.pl/blog/rozwoj-firmy/jdg/zakladanie-jednoosobowej-dzialalnosci-w-polsce/</t>
+          <t>https://www.gov.pl/web/uw-warminsko-mazurski/jestes-cudzoziemcem-potrzebujesz-pesel-lub-nip-do-zalatwienia-spraw-podatkowych</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Zgoda
-Szczegóły
-[#IABV2SETTINGS#]
-O plikach cookies
-Wykorzystujemy pliki cookie do spersonalizowania treści i reklam, aby oferować funkcje społecznościowe i analizować ruch w naszej witrynie. Informacje o tym, jak korzystasz z naszej witryny, udostępniamy partnerom społecznościowym, reklamowym i analitycznym. Partnerzy mogą połączyć te informacje z innymi danymi otrzymanymi od Ciebie lub uzyskanymi podczas korzystania z ich usług.</t>
+          <t>Jesteś cudzoziemcem? Potrzebujesz PESEL lub NIP do załatwienia spraw podatkowych Naczelnik Urzędu Skarbowego w Olsztynie przypomina o obowiązku posiadania przez cudzoziemców identyfikatora podatkowego tj. numeru PESEL lub NIP. Jak uzyskać takie dokumenty? O tym w dalszej części artykułu. Jeśli jesteś cudzoziemcem, który mieszka w Polsce, możesz zameldować się – wtedy automatycznie dostaniesz numer PESEL. Jeśli nie możesz zameldować się, a jakiś urząd wymaga od ciebie numeru PESEL – złóż wniosek. Sprawdź, jak to zrobić.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jakie są wymagania podatkowe dla samozatrudnionych cudzoziemców w Dolnośląskiem?</t>
+          <t>Jak otworzyć konto bankowe w Polsce?</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.ksiega-podatkowa.pl/akademia-skp/rozliczenie-wynagrodzenia-cudzoziemcow</t>
+          <t>https://sip.lex.pl/akty-prawne/mp-monitor-polski/ogolne-zasady-otwierania-i-prowadzenia-rachunkow-bankowych-16820548</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ostatnimi czasy na teren naszego kraju w celach zarobkowych przyjeżdża coraz więcej obywateli innych państw. Zatrudnienie ich może być korzystne dla polskich przedsiębiorców, z uwagi na ostatnie trudności znalezienia pracowników wśród obywateli naszego kraju, którzy sami również emigrują na terytoria innych państw. Jeżeli więc zatrudniasz lub zamierzasz zatrudnić obcokrajowców i chcesz prawidłowo rozliczyć ich wynagrodzenia oraz sporządzić niezbędną dokumentację, zapoznaj się koniecznie z poniższym artykułem.
-Zanim przystąpisz do ewidencji wynagrodzenia obcokrajowców, postępuj zgodnie z poniższymi krokami:
-1. sprawdź status rezydencji zatrudnionego cudzoziemca
-2. zapytaj go, czy posiada certyfikat rezydencji innego kraju niż Polska
-3. zweryfikuj istnienie umowy o unikaniu podwójnego opodatkowania z krajem, którego certyfikat rezydencji
-posiada dana osoba
-4. dobierz odpowiedni rodzaj umowy, wylicz odpowiednie wynagrodzenia i sporządź niezbędną dokumentację
-Więc po kolei…
-Kogo uznać za rezydenta?
-Rezydent to osoba, która przebywa w Polsce w danym roku podatkowym więcej niż 183 dni lub która ma w naszym kraju ośrodek interesów życiowych, np. mieszka tu ze swoją rodziną, tu dzieci chodzą do szkoły albo prowadzi działalność gospodarczą. Wystarczy, że jeden z tych warunków został spełniony by obcokrajowca można było uznać za rezydenta. Jeżeli więc zatrudniony przez nas cudzoziemiec przebywa w Polsce krótko lub posiada certyfikat rezydenta innego kraju, nie można go uznać za rezydenta.
-Posiadanie certyfikatu rezydencji
-Certyfikat rezydencji to w zasadzie potwierdzenie faktu miejsca zamieszkania podatnika. To, w jakim państwie uzyska certyfikat, w tym rozliczy swoje dochody. Sam bowiem decyduje, gdzie chce mieszkać i gdzie płacić podatki. Cudzoziemiec może również uzyskać polski certyfikat rezydencji. W tym celu musi się zwrócić do polskiego urzędu o jego wydanie, a urząd decyduje, czy uznać danego podatnika za rezydenta naszego kraju czy nie. Jeżeli więc nasz potencjalny pracownik przedstawi taki certyfikat, będzie wiązało się do z pewnymi konsekwencjami w wyliczaniu podatku dochodowego.</t>
+          <t>Ogólne zasady otwierania i prowadzenia rachunków bankowych. ZARZĄDZENIE PREZESA NARODOWEGO BANKU POLSKIEGO z dnia 10 grudnia 1982 r. w sprawie ogólnych zasad otwierania i prowadzenia rachunków bankowych. Jeżeli chcesz mieć dostęp do wszystkich dokumentów powiązanych, zaloguj się do LEX-a Nie korzystasz jeszcze z programów LEX? Zamów dostęp testowy »</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/cudzoziemcy/pit-11-czy-ift-1r-jak-rozliczyc-cudzoziemca</t>
+          <t>https://www.knf.gov.pl/dla_rynku/procesy_licencyjne/bankowy/banki/wstep</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Styczeń to ważny miesiąc dla pracodawców. Mają oni obowiązek dostarczenia do Urzędu Skarbowego odpowiednich deklaracji podatkowych. Zatrudniając osoby z Polski, sprawa jest oczywista – pracodawca wystawia PIT-11. Wątpliwości pojawiają się natomiast w przypadku zatrudnienia obcokrajowców. Jak rozliczyć osoby fizyczne niemające miejsca zamieszkania w Polsce? Jaką deklarację roczną wystawić cudzoziemcowi zatrudnionemu na oświadczeniu o powierzeniu wykonywania pracy cudzoziemcowi lub na podstawie zezwolenia na pracę? Odpowiadamy w artykule.
-&gt;&gt; Przetestuj bezpłatnie system kadrowo – płacowy
-Zagadnienia poruszane w artykule:
-Pierwszym i najważniejszym krokiem jest ustalenie rezydencji podatkowej obcokrajowca. Określa ona, w którym kraju jako pierwszym powinien być odprowadzany podatek od dochodu.
-Dla celów podatkowych polski rezydent podatkowy to osoba, która mieszka w Polsce więcej niż 183 dni w roku lub osoba, która przebywa tu krócej, ale posiada w Polsce centrum interesów osobistych, życiowych i gospodarczych. Taka osoba podlega tzw. nieograniczonemu obowiązkowi podatkowemu.</t>
+          <t>Czynności bankowe i inne rodzaje działalności dozwolone dla banków Formy działalności Bank państwowy Bank w formie spółki akcyjnej Bank spółdzielczy Bank hipoteczny Wymagania obowiązujące przy tworzeniu banku Wstęp Założyciele Kapitał założycielski Fundusze własne banku Osoby przewidziane do objęcia stanowisk Plan działalności banku Pomieszczenia przewidziane do prowadzenia działalności</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/pit-11-dla-cudzoziemca-jaki-urzad-skarbowy</t>
+          <t>https://www.knf.gov.pl/dla_rynku/procesy_licencyjne/bankowy/banki/wymagania_obowiazujace_przy_tworzeniu_banku</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Zagadnienia poruszane w artykule:
-Są dwa rozwiązania związane z rozliczeniem cudzoziemca w Polsce. Zależą one od tego, czy cudzoziemiec zatrudniony w Polsce posiada status rezydenta lub nierezydenta.
-W tym wypadku deklarację należy wysłać do urzędu skarbowego ds. cudzoziemców, a w adresie cudzoziemca należy wpisać jego zagraniczny adres.
-Deklarację cudzoziemca rezydenta należy wysłać do urzędu skarbowego zgodnego z miejscem jego zamieszkania. (W adresie cudzoziemca należy wpisać jego adres zamieszkania w Polsce. Jeżeli cudzoziemiec nie mieszka już w Polsce to deklarację należy wysłać na jego obecny, zagraniczny adres. Urzędy Skarbowe pozostają bez zmian.)
-Zapraszamy do naszego artykułu, w którym więcej o tym, jaką deklarację podatkową wystawić obcokrajowcom.</t>
+          <t>Wymagania obowiązujące przy tworzeniu banku - Komisja Nadzoru Finansowego Pomieszczenia przewidziane do prowadzenia działalności Aby ułatwić korzystanie z serwisu, mechanizm nim zarządzający wykorzystuje technologię cookies – informacje zapisywane są przez serwer Urzędu na komputerze użytkownika. Nie jest ona wykorzystywana do pozyskiwania jakichkolwiek danych o osobach odwiedzających serwis. Użytkownik może w każdej chwili wyłączyć w swojej przeglądarce internetowej opcję przyjmowania cookies. Może to spowodować pewne utrudnienia w korzystaniu z serwisu. Więcej informacji w zakładce Polityka prywatności. Polityka Prywatności</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Jak mogę zarejestrować firmę w Dolnośląskiem?</t>
+          <t>Jakie są wymagania podatkowe dla samozatrudnionych cudzoziemców w Polskim?</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://dc.biz.pl/wirtualne-biuro-wroclaw-gajowice-2/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00806</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Zgoda
-Szczegóły
-[#IABV2SETTINGS#]
-O plikach cookies
-Niezbędne  2 Niezbędne pliki cookie przyczyniają się do użyteczności strony poprzez umożliwianie podstawowych funkcji takich jak nawigacja na stronie i dostęp do bezpiecznych obszarów strony internetowej. Strona internetowa nie może funkcjonować poprawnie bez tych ciasteczek.Cookiebot1Dowiedz się więcej na temat tego dostawcyCookieConsentStores the user's cookie consent state for the current domainMaksymalny okres przechowywania: 1 rokRodzaj: Plik cookie HTTPGoogle1Dowiedz się więcej na temat tego dostawcyNiektóre dane gromadzone przez tego dostawcę służą do personalizacji i pomiaru skuteczności reklamy.test_cookieUsed to check if the user's browser supports cookies.Maksymalny okres przechowywania: 1 dzieńRodzaj: Plik cookie HTTP</t>
+          <t>Kto może prowadzić działalność gospodarczą w Polsce Obywatele państw członkowskich Unii Europejskiej oraz Europejskiego Obszaru Gospodarczego, którzy chcą wykonywać w Polsce działalność gospodarczą, mogą: założyć własną firmę jednoosobową lub dowolną spółkę handlową</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=9EnRI4hflKM</t>
+          <t>https://www.biznes.gov.pl/pl/portal/0613</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-New
-New
-</t>
+          <t>Kto może prowadzić działalność gospodarczą w Polsce Polskie przepisy przewidują dużą swobodę prowadzenia działalności gospodarczej, co oznacza, że w większości wypadków możesz założyć firmę i prowadzić ją w wybranej przez siebie formie. Przeczytaj, kiedy trzeba spełnić dodatkowe warunki. Sprawdź, czy firmę może otworzyć cudzoziemiec, osoba niepełnoletnia lub emeryt. Firma cudzoziemca Zakładanie firmy jednoosobowej Polskie przepisy przewidują dużą swobodę prowadzenia działalności gospodarczej, co oznacza, że w większości wypadków możesz założyć firmę i prowadzić ją w wybranej przez siebie formie. Przeczytaj, kiedy trzeba spełnić dodatkowe warunki. Sprawdź, czy firmę może otworzyć cudzoziemiec, osoba niepełnoletnia lub emeryt. Jak delegować do Polski pracowników w ramach świadczenia usług Sprawdź na czym polega delegowanie w ramach świadczenia usług, jakie są zasady i obowiązki pracodawców delegujących, kiedy pracownik jest pracownikiem delegowanym. Firma cudzoziemca Delegowanie Obowiązki pracodawcy Zatrudnienie pracownika</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.nieruchomosci-online.pl/porady/dzialalnosc-gospodarcza-w-mieszkaniu-lub-domu-30970.html</t>
+          <t>https://www.biznes.gov.pl/pl/portal/001466</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Zaloguj się
-Kupno
-Sprzedaż
-Wynajem</t>
+          <t>Obywatel Ukrainy, który przebywa w Polsce legalnie i posiada numer PESEL, może założyć działalność gospodarczą na takich samych zasadach jak obywatel Polski w dowolnej formie. firmę jednoosobową – czyli działalność gospodarczą osoby fizycznej – i zarejestrować ją w CEIDG spółkę osobową lub kapitałową – w tym spółkę jawną i partnerską – i zarejestrować ją w KRS.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Czy muszę płacić podatki w Dolnośląskiem, jeśli pracuję zdalnie dla zagranicznej firmy?</t>
+          <t>Czy muszę płacić podatki w Polskim, jeśli pracuję zdalnie dla zagranicznej firmy?</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.podatnik.info/publikacje/podatek-za-prace-za-granica-kiedy-nie-trzeba-wykazywac-dochodow-z-zagranicy,6164b0</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00399</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>We and our vendors (2) use cookies and similar technologies to read, store, and write information on your device. Essential cookies are necessary for our site to work properly. With your consent, we and our vendors may also use non-essential cookies to improve user experience, personalize advertisements, and analyze website traffic. For these reasons, we may process your personal data (such as IP address or browsing and interaction data).
-By clicking “Accept,” you agree to our website's data use as described in our “Cookie Policy.” You may change or withdraw your consent at any time by clicking the “Consent Preferences” link in the footer and accessing the categories, purposes, and vendors tabs.
-We process data for the following purposes and special features: Actively scan device characteristics for identification, Create profiles for personalised advertising, Create profiles to personalise content, Develop and improve services, Measure advertising performance, Measure content performance, Store and/or access information on a device, Understand audiences through statistics or combinations of data from different sources, Use limited data to select advertising, Use limited data to select content, Use profiles to select personalised advertising, Use profiles to select personalised content.
-DARMOWY PROGRAM DO PIT 2024/2025
-Praca za granicą często wiąże się z uzyskiwaniem wyższych dochodów niż w Polsce, co sprawia, że staje się atrakcyjną opcją dla wielu osób. Warto jednak pamiętać, że zarobki osiągane poza Polską mogą rodzić obowiązki podatkowe w kraju, w tym konieczność rozliczenia się z fiskusem zgodnie z polskimi przepisami. W tym artykule poruszamy często spotykane zagadnienie, jakim jest praca za granicą a podatek w Polsce. Zapraszamy do czytania.</t>
+          <t>Usługi transgraniczne to usługi świadczone dla odbiorców z innych państw UE. Usługi transgraniczne świadczysz, gdy: przemieszczasz się do innego państwa, aby wykonać usługę, na przykład remontujesz budynek we Francji przemieszczasz się do państwa członkowskiego A, by wykonać usługę dla podmiotu z państwa członkowskiego B, na przykład doradzasz przedsiębiorcy z Niemiec przy transakcji w Czechach</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://poradnikprzedsiebiorcy.pl/-skladanie-zeznan-podatkowych-przez-nierezydentow</t>
+          <t>https://biznes.gov.pl/pl/portal/00586</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Serwis Księgowy
-Sprawozdawczość
-Składanie zeznań podatkowych przez nierezydentów
-składanie zeznań podatkowych przez n...</t>
+          <t>Polacy, w ramach jednolitego rynku wewnętrznego Unii Europejskiej, korzystają ze swobodnego przepływu towarów, usług, kapitału i osób – mogą prowadzić wymianę handlową i działalność gospodarczą we wszystkich państwach członkowskich Unii Europejskiej i Europejskiego Obszaru Gospodarczego. Państwami członkowskimi Unii Europejskiej są: Austria, Belgia, Bułgaria, Chorwacja, Cypr, Czechy, Dania, Estonia, Finlandia, Francja, Grecja, Hiszpania, Holandia, Irlandia, Litwa, Luksemburg, Łotwa, Malta, Niemcy, Polska, Portugalia, Rumunia, Słowenia, Słowacja, Szwecja, Węgry, Włochy. Państwami członkowskimi Europejskiego Obszaru Gospodarczego, poza państwami należącymi do Unii Europejskiej, są: Norwegia, Islandia, Liechtenstein.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.podatki.biz/i91099/podatek-dochodowy-osob/podatek-dochodowy-osob.htm</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00229</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>mojepodatki.biz
-REJESTRACJA
-MENU
-Działy tematyczne
-Aktualności - podatki, rachunkowość, ZUS, gospodarkaABC - prawo i podatki dla początkującychAmortyzacja - środki trwałe i wartości niematerialne i prawneDla Czytelników podatki.bizDziałalność gospodarczaFakturowanie VATFormularze podatkowe i wzory dokumentówKasy fiskalneKoszty uzyskania przychodówLimity, parametry, wskaźnikiPodatek PCC, podatek od nieruchomości, pozostałe podatki i opłatyPodatek VAT i akcyza - zagadnienia ogólnePodatki dochodowe PIT i CIT - zagadnienia ogólnePracownicy: zatrudnianie, urlopy, zasiłki, świadczenia, ekwiwalentyRachunkowość: PKPiR | Pełna księgowość | Ewidencje podatkowe i księgoweRozliczenie roczne PITRyczałt od przychodów ewidencjonowanych i karta podatkowaSamochód w firmieSprawy codzienne: spadki i darowizny, najem prywatny, nieruchomości, kupno-sprzedażSzkolenia rozpoczynające się w najbliższych dniachSkładki ZUS: ubezpieczenia społeczne, zdrowotne, FP, FGŚPZobowiązania podatkowe, czyli jak płacić podatki
-Aktualności - podatki, rachunkowość, ZUS, gospodarka</t>
+          <t>O tym, gdzie płacić podatki, decyduje zasada rezydencji, czyli miejsce zamieszkania dla celów podatkowych. Osoby, które mają miejsce zamieszkania dla celów podatkowych w Polsce , mają nieograniczony obowiązek podatkowy. To znaczy, że rozliczają tu wszystkie dochody, zarówno osiągnięte w Polsce, jak i za granicą. Miejsce zamieszkania w Polsce ma osoba fizyczna, która spełnia przynajmniej jeden z dwóch warunków:</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jak mogę uzyskać PESEL do celów podatkowych w Dolnośląskiem?</t>
+          <t>Jak korzystać z publicznej służby zdrowia w Polsce?</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://poradnikprzedsiebiorcy.pl/-pit-11-za-cudzoziemca-wylacznie-z-numerem-pesel</t>
+          <t>http://pacjent.gov.pl/zasady-korzystania-z-systemu</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Zdaniem eksperta
-PIT-11 za cudzoziemca a identyfikator podatkowy
-pit-11 za cudzoziemca
-4.93/5
-(30)</t>
+          <t>Kiedy i na jakich zasadach możesz korzystać z systemu opieki zdrowotnej? Tutaj znajdziesz odpowiedzi</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/cudzoziemcy/pit-11-czy-ift-1r-jak-rozliczyc-cudzoziemca</t>
+          <t>http://pacjent.gov.pl/system-opieki-zdrowotnej</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Styczeń to ważny miesiąc dla pracodawców. Mają oni obowiązek dostarczenia do Urzędu Skarbowego odpowiednich deklaracji podatkowych. Zatrudniając osoby z Polski, sprawa jest oczywista – pracodawca wystawia PIT-11. Wątpliwości pojawiają się natomiast w przypadku zatrudnienia obcokrajowców. Jak rozliczyć osoby fizyczne niemające miejsca zamieszkania w Polsce? Jaką deklarację roczną wystawić cudzoziemcowi zatrudnionemu na oświadczeniu o powierzeniu wykonywania pracy cudzoziemcowi lub na podstawie zezwolenia na pracę? Odpowiadamy w artykule.
-&gt;&gt; Przetestuj bezpłatnie system kadrowo – płacowy
-Zagadnienia poruszane w artykule:
-Pierwszym i najważniejszym krokiem jest ustalenie rezydencji podatkowej obcokrajowca. Określa ona, w którym kraju jako pierwszym powinien być odprowadzany podatek od dochodu.
-Dla celów podatkowych polski rezydent podatkowy to osoba, która mieszka w Polsce więcej niż 183 dni w roku lub osoba, która przebywa tu krócej, ale posiada w Polsce centrum interesów osobistych, życiowych i gospodarczych. Taka osoba podlega tzw. nieograniczonemu obowiązkowi podatkowemu.</t>
+          <t>Najważniejsze ogniwa systemu opieki zdrowotnej w Polsce to praktyki lekarskie, pielęgniarek i położnych, przychodnie i szpitale. Do niektórych z nich możemy wybrać się bez skierowania, do innych potrzebujemy takiego dokumentu Dowiedz się, jak zorganizowana jest opieka zdrowotna w Polsce. Pierwszy szczebel, czyli podstawowa opieka zdrowotna</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://poradnikprzedsiebiorcy.pl/-oswiadczenie-cudzoziemca-o-rezydencji-podatkowej-wzor-do-pobrania</t>
+          <t>http://pacjent.gov.pl/aktualnosc/wiesz-jak-dziala-system-ochrony-zdrowia</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Pobierz
-Wzory pism
-Oświadczenie cudzoziemca o rezydencji podatkowej - wzór do pobrania
-oświadczenie cudzoziemca o rezydencj...</t>
+          <t>Poznaj zasady funkcjonowania systemu ochrony zdrowia, aby z niego korzystać Do systemowej opieki mają prawo osoby ubezpieczone obowiązkowo, dobrowolnie lub spełniające inne warunki, zapisane w ustawie. Jak wygląda status Twojego ubezpieczenia, sprawdzisz na Internetowym Koncie Pacjenta.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Jakie są składki na opiekę zdrowotną i ubezpieczenie społeczne dla cudzoziemców w Dolnośląskiem?</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+          <t>Jak mogę ubiegać się o polskie obywatelstwo w Polskim?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/mswia/uzyskaj-polskie-obywatelstwo</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Potwierdzenie posiadania lub utraty obywatelstwa polskiego Chcesz dostać polskie obywatelstwo? Utraciłeś polskie obywatelstwo i chcesz je odzyskać? Potrzebujesz urzędowego potwierdzenia, że masz polskie obywatelstwo? Tutaj znajdziesz wszystkie potrzebne informacje. Złóż wniosek do Prezydenta o nadanie polskiego obywatelstwa</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://poradnikpracownika.pl/-skladki-odprowadzane-od-wynagrodzenia</t>
+          <t>https://powroty.gov.pl/nabycie-obywatelstwa-polskiego-10000</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>PoradnikPracownika
-ZATRUDNIENIE
-Ubezpieczenia
-Składki odprowadzane od wynagrodzenia przez pracodawcę i pracownika w 2025 r.</t>
+          <t>Informacje zgodne ze stanem prawnym na dzień: 2024-09-11 Zagadnienia nabycia obywatelstwa polskiego i jego utraty reguluje ustawa z 2 kwietnia 2009 r. o obywatelstwie polskim. 1. Urodzenie z rodziców, z których co najmniej jedno ma obywatelstwo polskie – zasada krwi/Ius Sanguinis</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://tuz.pl/ekspert-radzi/ubezpieczenie-zdrowotne-dla-cudzoziemcow-w-polsce-wszystko-co-musisz-wiedziec-na-ten-temat/</t>
+          <t>https://archiwum.mswia.gov.pl/pl/bezpieczenstwo/obywatelstwo-i-repatri/cudzoziemcy/10169,SPOSOBY-NABYCIA-OBYWATELSTWA-POLSKIEGO.html</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Polska, jako członek Unii Europejskiej, oferuje szeroki zakres usług zdrowotnych dla swoich obywateli. Jednakże, dla cudzoziemców przebywających tymczasowo lub na stałe w Polsce, kwestie ubezpieczenia zdrowotnego mogą być nieco bardziej złożone. Dla tych, którzy przybywają do Polski, ważne jest zrozumienie zasad, rodzajów ubezpieczeń i procedur związanych z opieką zdrowotną. Poniżej znajdziesz wszystkie istotne informacje na ten temat.
-Ubezpieczenie kosztów leczenia obcokrajowca to dobrowolna polisa, która zapewnia ochronę finansową w przypadku nagłego zachorowania lub wypadku podczas pobytu na terytorium Polski. Jest to szczególnie ważne dla osób, które nie są objęte publicznym ubezpieczeniem zdrowotnym w Polsce, np. obywateli państw trzecich. Zakres ubezpieczenia kosztów leczenia obcokrajowca może się różnić w zależności od wybranej polisy, ale zazwyczaj obejmuje:
-koszty leczenia ambulatoryjnego i szpitalnego,
-koszty leków i opatrunków,
-koszty badań diagnostycznych i zabiegów operacyjnych,</t>
+          <t>Zagadnienia nabycia obywatelstwa polskiego i jego utraty reguluje ustawa z dnia 2 kwietnia 2009 roku o obywatelstwie polskim . Ustawa zawiera dwie podstawowe zasady dotyczące obywatelstwa polskiego. Wyrażona w art. 2 ustawy zasada ciągłości obywatelstwa polskiego gwarantuje trwałość obywatelstwa w czasie, począwszy od momentu jego nabycia, zgodnie z obowiązującymi w tym czasie przepisami, niezależnie od zmian, jakim podlega ustawodawstwo dotyczące obywatelstwa. Oznacza to, iż osoby, które nabyły obywatelstwo polskie na podstawie dawnych przepisów, następnie uchylonych lub zmienionych, jeśli obywatelstwa polskiego nie utraciły, zachowują je zgodnie z przepisami obowiązującymi w dacie jego nabycia. Zasada ta jest równocześnie dyrektywą dla właściwych organów administracji publicznej w postępowaniu o potwierdzenie posiadania lub utraty obywatelstwa polskiego. Natomiast wprowadzona przepisem art. 3 ustawy, zasada wyłączności obywatelstwa polskiego wiąże się ściśle z problemem podwójnego obywatelstwa, tworzy bowiem jasną dyrektywę kolizyjną w przypadku jego zaistnienia i pozwala na usuwanie jego niekorzystnych skutków. Projekt ustawy przyjmuje zasadę dopuszczalności wielości obywatelstw przy utrzymaniu bezwzględnego priorytetu obywatelstwa polskiego. Obywatel polski może posiadać równocześnie obywatelstwo polskie i obywatelstwo państwa obcego, ale nawet wówczas posiada wobec Rzeczypospolitej Polskiej takie same prawa i obowiązki, jak osoba posiadająca wyłącznie obywatelstwo polskie, tj. nie może wobec władz polskich powoływać się ze skutkiem prawnym na posiadane równocześnie obywatelstwo obce lub na wynikające z niego prawa i obowiązki. Urodzenie z rodziców, z których co najmniej jedno posiada obywatelstwo polskie – Zasada krwi/Ius Sanguinis</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Jakie mam prawa jako najemca w Dolnośląskiem?</t>
+          <t>Jakie podatki muszą płacić cudzoziemcy w Polsce?</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://gazetawroclawska.pl/stancja-wroclaw-jak-wynajac-mieszkanie-poradnik/ar/c3-969554</t>
+          <t>https://www.gov.pl/web/gruzja/srodki-finansowe-wymagane-od-cudzoziemca-wjezdzajacego-do-polski</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>This website is using a security service to protect itself from online attacks. The action you just performed triggered the security solution. There are several actions that could trigger this block including submitting a certain word or phrase, a SQL command or malformed data.
-You can email the site owner to let them know you were blocked. Please include what you were doing when this page came up and the Cloudflare Ray ID found at the bottom of this page.
-Cloudflare Ray ID: 92f5478f88e1c3fe
-•
-      Your IP:
-      Click to reveal
-83.27.101.111
-•
-Performance &amp; security by Cloudflare</t>
+          <t>Środki finansowe wymagane od cudzoziemca wjeżdżającego do Polski Zgodnie z Rozporządzeniem Ministra Spraw Wewnętrznych z dnia 23 lutego 2015 r. w sprawie środków finansowych wymaganych od cudzoziemca wjeżdżającego na terytorium Rzeczypospolitej Polskiej oraz dokumentów, które mogą potwierdzić możliwość uzyskania takich środków, a także cel i czas trwania planowanego pobytu na podstawie art. 26 ust. 1 ustawy z dnia 12 grudnia 2013 r. o cudzoziemcach , cudzoziemiec powinien posiadać środki finansowe na pokrycie kosztów: - utrzymania w trakcie jego pobytu na tym terytorium,</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.flatte.app/blog/obowiazki-wynajmujacego-mieszkanie</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00806</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Obowiązki wynajmującego mieszkanie mogą wynikać zarówno z mocy prawa, jak i postanowień umowy. Przy czym treść umowy najmu nie może naruszać przepisów prawa, ani sprzeciwiać się właściwości stosunku prawnego, ani zasadom współżycia społecznego. Co w przypadku, kiedy obowiązki właściciela nieruchomości wobec najemcy wyszczególnione w zawartej umowie najmu są sprzeczne z treścią ustawy? Zasadniczo obowiązuje zasada swobody umów, natomiast w przypadku sprzeczności postanowień z treścią obowiązującego prawa, w tym w szczególności ustawą o prawach lokatorów,  tego typu postanowienia zawarte w umowie są nieważne, czyli nie rodzą skutków prawnych.
-Prawo wynajmu mieszkania w Polsce, w tym obowiązki wynajmującego mieszkanie wynikające z przepisów prawa wymienione są przede wszystkim w dwóch aktach prawa. Pierwszym jest ustawa z 21 czerwca 2021 r. o ochronie praw lokatorów, mieszkaniowym zasobie gminy i o zmianie Kodeksu cywilnego. Drugim jest Kodeks cywilny, a dokładniej przepisy w dziale I. Znajomość wspomnianych powyżej aktów prawa jest niezbędna przy tworzeniu zgodnej z prawem umowy najmu.
-Bezsprzecznie podstawowym obowiązkiem wynajmującego mieszkanie jest wydanie lokalu najemcy. Mieszkanie musi być w stanie zgodnym z ustaleniami i gotowe do użytkowania. Wynajmujący zobowiązany jest również do umożliwienia najemcy korzystania z lokalu. W praktyce oznacza to obowiązek wydania kluczy do lokalu w umówionym terminie. Kolejnym obowiązkiem właściciela mieszkania jest określenie wysokości czynszu i dodatkowych opłat. Warto pamiętać, że do obowiązków inwestora należy także spisanie stanu liczników i protokołu zdawczo-odbiorczego. Kolejnym obowiązkiem wynajmującego mieszkanie, o którym wynajmujący często zapominają, jest okazanie najemcy świadectwa charakterystyki energetycznej lokalu.
-To nie jedyne obowiązki właściciela nieruchomości wobec najemcy. Zgodnie z prawem, obowiązki wynajmującego lokal mieszkalny obejmują również zapewnienie prawidłowego działania istniejących urządzeń i instalacji. W szczególności tych związanych z nieruchomością, które umożliwiają lokatorowi korzystanie z wody, energii elektrycznej oraz paliw gazowych i ciekłych, ciepła, dźwigów osobowych i innych instalacji oraz urządzeń stanowiących wyposażenie lokalu i budynku określone odrębnymi przepisami.
-Oczywistym jest, że zarówno sprzęty, jak i urządzenia ulegają awariom i zużyciu. Wiąże się to z koniecznością ich naprawy lub wymiany. O ile właściciel mieszkania jest równocześnie jego lokatorem, nie ma problemu z określeniem, kto jest odpowiedzialny za tego typu konserwacje i naprawy. Problem pojawia się w przypadku mieszkań wynajmowanych. Tam z jednej strony występuje właściciel mieszkania, a z drugiej – najemca, który zamieszkuje ów lokat. Kto zatem jest odpowiedzialny za remonty i naprawy w wynajmowanym mieszkaniu? Zgodnie z prawem obowiązek zapewnienia przez wynajmującego mieszkanie sprawnego działania urządzeń i instalacji związanych z mieszkaniem nie oznacza, że jest on odpowiedzialny za wszystkie naprawy. Za część napraw odpowiedzialny jest inwestor, a za pozostałe lokator. Zatem za jakie naprawy odpowiedzialny jest wynajmujący, a za jakie najemca?</t>
+          <t>Kto może prowadzić działalność gospodarczą w Polsce Obywatele państw członkowskich Unii Europejskiej oraz Europejskiego Obszaru Gospodarczego, którzy chcą wykonywać w Polsce działalność gospodarczą, mogą: założyć własną firmę jednoosobową lub dowolną spółkę handlową</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://skup.io/czy-lokator-moze-nie-wpuscic-wlasciciela/</t>
+          <t>https://www.gov.pl/web/armenia/srodki-finansowe-wymagane-od-cudzoziemcow-wjezdzajacych-do-polski</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Cenimy prywatność użytkowników
-Używamy plików cookie, aby poprawić jakość przeglądania, wyświetlać reklamy lub treści dostosowane do indywidualnych potrzeb użytkowników oraz analizować ruch na stronie. Kliknięcie przycisku „Akceptuj wszystkie” oznacza zgodę na wykorzystywanie przez nas plików cookie.
-Używamy plików cookie, aby pomóc użytkownikom w sprawnej nawigacji i wykonywaniu określonych funkcji. Szczegółowe informacje na temat wszystkich plików cookie odpowiadających poszczególnym kategoriom zgody znajdują się poniżej.
-Pliki cookie sklasyfikowane jako „niezbędne” są przechowywane w przeglądarce użytkownika, ponieważ są niezbędne do włączenia podstawowych funkcji witryny.... Pokaż więcej
-Więcej informacji na temat działania plików typu „cookie” od osób trzecich oraz na temat obsługi Twoich danych podajemy w:  Polityce prywatności firmy Google</t>
+          <t>Środki finansowe wymagane od cudzoziemców wjeżdżających do Polski Zgodnie z Rozporządzeniem Ministra Spraw Wewnętrznych z dnia 23 lutego 2015 r. w sprawie środków finansowych wymaganych od cudzoziemca wjeżdżającego na terytorium Rzeczypospolitej Polskiej oraz dokumentów, które mogą potwierdzić możliwość uzyskania takich środków, a także cel i czas trwania planowanego pobytu na podstawie art. 26 ust. 1 ustawy z dnia 12 grudnia 2013 r. o cudzoziemcach , każdy cudzoziemiec powinien posiadać środki finansowe na pokrycie kosztów: utrzymania w trakcie jego pobytu na tym terytorium;</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Czy wynajmujący może mnie eksmitować bez wypowiedzenia w Dolnośląskiem?</t>
+          <t>Jak zameldować się w Polsce?</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://gazetawroclawska.pl/najem-mieszkania-o-czym-nalezy-pamietac/ar/11984540</t>
+          <t>https://www.gov.pl/web/gov/zamelduj-sie-na-pobyt-staly-lub-czasowy-dluzszy-niz-3-miesiace</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>This website is using a security service to protect itself from online attacks. The action you just performed triggered the security solution. There are several actions that could trigger this block including submitting a certain word or phrase, a SQL command or malformed data.
-You can email the site owner to let them know you were blocked. Please include what you were doing when this page came up and the Cloudflare Ray ID found at the bottom of this page.
-Cloudflare Ray ID: 92f54809bf17c3fe
-•
-      Your IP:
-      Click to reveal
-83.27.101.111
-•
-Performance &amp; security by Cloudflare</t>
+          <t>Zamelduj się na pobyt stały lub czasowy dłuższy niż 3 miesiące Zmieniasz miejsce zamieszkania? A może wracasz z zagranicy i nie masz meldunku w Polsce? Pamiętaj, żeby się zameldować. Możesz to zrobić przez internet albo w urzędzie gminy. Jeśli jesteś obywatelem Polski i twoje dziecko urodziło się w Polsce – kierownik urzędu stanu cywilnego, który sporządził akt urodzenia, z urzędu zamelduje twoje dziecko.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://skup.io/kiedy-nie-mozna-wyrzucic-lokatora-z-mieszkania/</t>
+          <t>https://www.gov.pl/web/cyfryzacja/zamelduj-sie-wygodnie--przez-internet</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Cenimy prywatność użytkowników
-Używamy plików cookie, aby poprawić jakość przeglądania, wyświetlać reklamy lub treści dostosowane do indywidualnych potrzeb użytkowników oraz analizować ruch na stronie. Kliknięcie przycisku „Akceptuj wszystkie” oznacza zgodę na wykorzystywanie przez nas plików cookie.
-Używamy plików cookie, aby pomóc użytkownikom w sprawnej nawigacji i wykonywaniu określonych funkcji. Szczegółowe informacje na temat wszystkich plików cookie odpowiadających poszczególnym kategoriom zgody znajdują się poniżej.
-Pliki cookie sklasyfikowane jako „niezbędne” są przechowywane w przeglądarce użytkownika, ponieważ są niezbędne do włączenia podstawowych funkcji witryny.... Pokaż więcej
-Więcej informacji na temat działania plików typu „cookie” od osób trzecich oraz na temat obsługi Twoich danych podajemy w:  Polityce prywatności firmy Google</t>
+          <t>Zmieniasz miejsce zamieszkania? Jeśli tak, to z pewnością masz wiele na głowie, a wizyta w urzędzie jest ostatnim, o czym teraz myślisz. Mamy dobrą wiadomość – dzięki naszym e-usługom sprawy meldunkowe załatwisz z fotela, a nawet hamaka. To nie tylko wygodne, ale także popularne rozwiązanie. Tylko w maju Polacy skorzystali z e-usług meldunkowych 20 815 razy. Przez cały ubiegły rok zaś – ponad 180 tysięcy razy. Już teraz zameldowanie się przez internet jest proste. Wkrótce będzie jeszcze prostsze! A jak skorzystać z e-usług meldunkowych? Zacznijmy od tego, co będzie Ci potrzebne.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://pogorzelski.pl/eksmisja-z-mieszkania-czy-mozna-wyrzucic-lokatora-z-mieszkania/</t>
+          <t>https://www.gov.pl/web/gov/zamelduj-sie-na-pobyt-staly-dla-cudzoziemcow</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Cenimy prywatność użytkowników
-Używamy plików cookie, aby poprawić jakość przeglądania, wyświetlać reklamy lub treści dostosowane do indywidualnych potrzeb użytkowników oraz analizować ruch na stronie. Kliknięcie przycisku „Akceptuj wszystkie” oznacza zgodę na wykorzystywanie przez nas plików cookie.
-Używamy plików cookie, aby pomóc użytkownikom w sprawnej nawigacji i wykonywaniu określonych funkcji. Szczegółowe informacje na temat wszystkich plików cookie odpowiadających poszczególnym kategoriom zgody znajdują się poniżej.
-Pliki cookie sklasyfikowane jako „niezbędne” są przechowywane w przeglądarce użytkownika, ponieważ są niezbędne do włączenia podstawowych funkcji witryny.... Pokaż więcej
-Niezbędne pliki cookie mają kluczowe znaczenie dla podstawowych funkcji witryny i witryna nie będzie działać w zamierzony sposób bez nich. Te pliki cookie nie przechowują żadnych danych umożliwiających identyfikację osoby.</t>
+          <t>Zamelduj się na pobyt stały lub czasowy Aby sprawdzić, jak zameldować się na pobyt stały lub czasowy, odpowiedz na pytania poniżej. Jeśli mieszkasz w Polsce – zamelduj się na pobyt stały lub czasowy .</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Jak mogę odzyskać kaucję za wynajem w Dolnośląskiem?</t>
+          <t>Czy mogę otworzyć konto bankowe w Polskim jako cudzoziemiec?</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://ladek.pl/ogloszenie-o-ii-naborze-na-najem-w-ramach-sim-sudety-2-nabor/</t>
+          <t>http://bip.brpo.gov.pl/pl/content/k%C5%82opoty-cudzoziemca-z-kontem-w-polskim-banku</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Home
-AKTUALNOŚCI
-INFORMACJE
-...
-Ogłoszenie o II naborze na najem w ramach SIM SUDETY</t>
+          <t>Obywatel Iranu nie może założyć konta bankowego w Polsce, mimo że ma kartę pobytu czasowego na terenie Polski, od kilku studiuje i pracuje tu, a jego żona jest Polką. Swój problem przedstawił w Biurze Terenowym RPO we Wrocławiu. Pełnomocnik Rzecznika wystosował pismo w jego sprawie do Związku Banków Polskich i Urzędu Ochrony Konkurencji i Konsumentów, wskazując m.in., że mogło dojść do dyskryminacji. Problem ten został przedstawiony też: Komisji Nadzoru Finansowego i Rzecznikowi Finansowemu. Sprawą zajmował się również Narodowy Bank Polski, Komisja Nadzoru Finansowego oraz Generalny Inspektor Informacji Finansowej. Związek Banków Polskich uzasadnił: odmowa założenia rachunku bankowego wynika z konieczności respektowania szczególnych środków ograniczających i zapisów ustawy z dnia 16 listopada 2000 r. o praniu pieniędzy oraz finansowaniu terroryzmu. Z opinii Narodowego Banku Polskiego czy Generalnego Inspektora IF wynika jednak, że w przepisach prawa nie ma podstaw do odmowy założenia rachunku dla obywateli Iranu. Nawet przy uwzględnieniu wytycznych i rekomendacji uznających Islamską Republikę Iranu za kraj wysokiego ryzyka.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://bingowynajem.pl/kaucja-w-umowie-najmu-co-wynajmujacy-moze-potracic-z-kaucji/</t>
+          <t>https://www.prawo.pl/biznes/czy-polacy-moga-zakladac-konta-w-zagranicznych-bankach,514996.html</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Kaucja w umowie najmu mieszkania to zabezpieczenie dla właściciela wynajmowanej nieruchomości w sytuacji, gdy najemca zwleka z opłatami czynszowymi lub doprowadzi do zniszczenia wyposażenia, a nawet samego lokalu. Kiedy wynajmujący ma prawo nie zwrócić kaucji? Co zrobić, gdy wynajmujący nie chce oddać kaucji za mieszkanie bezpodstawnie? Na te oraz inne pytania znajdziesz odpowiedź w naszym dzisiejszym artykule.
-Spis treści
-Zgodnie z ustawą z dnia 21 czerwca 2001 r. o ochronie praw lokatorów, mieszkaniowym zasobie gminy i o zmianie Kodeksu cywilnego, kaucja podlega zwrotowi w ciągu miesiąca od dnia opróżnienia lokalu lub nabycia jego własności przez najemcę.
-Choć z założenia kaucja jest zwrotna, istnieje kilka sytuacji, w których wynajmujący ma prawo ją zatrzymać. Jeśli najemca ma zaległości w opłatach czynszowych czy rachunkach za media, które przekraczają wartość kaucji, z pewnością nie zostanie ona zwrócona. Sytuacje, w których wynajmujący może zatrzymać kaucję, powinny zostać ujęte w umowie. Innym powodem niezwrócenia pieniędzy może być uszkodzenia nieruchomości i wyposażenia. Stan mieszkania i przedmiotów w trakcie zdawania nieruchomości powinien pokrywać się ze stanem z protokołu zdawczo-odbiorczego. W przypadku zniszczeń, kaucja zostanie potrącona.
-Powyżej pisaliśmy o sytuacjach, kiedy wynajmujący ma prawo nie zwrócić kaucji najemcy. Czasami zwrot jest możliwy, jeśli zaległości czynszowe czy naprawy nie przekraczają wartości kaucji lub część zniszczeń została pokryta już wcześniej na koszt najemcy i zostało to udokumentowane.</t>
+          <t>Można trzymać pieniądze na koncie za granicą, ale nie wszędzie to proste Można trzymać pieniądze na koncie za granicą, ale nie wszędzie to proste Wojna za wschodnią granicą i słaby złoty skłaniają do rozglądania się za rachunkami w zagranicznych bankach. I choć obecnie o pieniądze w naszych bankach nie musimy się niepokoić, to konta za granicą stały się bardziej kuszące.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://rankomat.pl/nieruchomosci/kaucja-w-umowie-najmu-mieszkania</t>
+          <t>https://www.gov.pl/web/gruzja/srodki-finansowe-wymagane-od-cudzoziemca-wjezdzajacego-do-polski</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Zgoda
-Szczegóły
-[#IABV2SETTINGS#]
-O plikach cookies
-Używamy plików cookie i innych narzędzi śledzących (np. Pixel lub API), aby mierzyć wydajność, dostosowywać nasz marketing i zapewniać lepsze wrażenia z korzystania z naszej witryny.</t>
+          <t>Środki finansowe wymagane od cudzoziemca wjeżdżającego do Polski Zgodnie z Rozporządzeniem Ministra Spraw Wewnętrznych z dnia 23 lutego 2015 r. w sprawie środków finansowych wymaganych od cudzoziemca wjeżdżającego na terytorium Rzeczypospolitej Polskiej oraz dokumentów, które mogą potwierdzić możliwość uzyskania takich środków, a także cel i czas trwania planowanego pobytu na podstawie art. 26 ust. 1 ustawy z dnia 12 grudnia 2013 r. o cudzoziemcach , cudzoziemiec powinien posiadać środki finansowe na pokrycie kosztów: - utrzymania w trakcie jego pobytu na tym terytorium,</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Czy istnieją ograniczenia prawne dotyczące wynajmu mieszkania przez cudzoziemca w Dolnośląskiem?</t>
+          <t>Czy wynajmujący może mnie eksmitować bez wypowiedzenia w Polskim?</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://cudzoziemiec.eu/?q=obrot_cudzoziemcy</t>
+          <t>https://powroty.gov.pl/-/wypowiadanie-umow-najmu-przez-wynajmujacego-wlasciciela-nieruchomosci-wielka-brytania</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Kalkulator legalności pobytu
-cudzoziemcy
-kupno
-nieruchomości
-obrót nieruchomościami</t>
+          <t>Warto zaznaczyć, że niektóre zasady dotyczące długości wypowiedzenia uległy zmianie z powodu koronawirusa . Krótkoterminowe umowy najmu - Assured shorthold tenancies Właściciel wynajmowanej nieruchomości może wypowiedzieć umowę bez podania przyczyny jeśli:</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://sawastian-lipska.pl/blog/czy-cudzoziemiec-moze-kupic-nieruchomosc-w-polsce/</t>
+          <t>https://www.prawo.pl/prawo/kupno-oswiadczenia-o-mozliwosci-zamieszkania-najem-okazjonalny,520257.html</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>660 539 046
-kancelaria@sawastian-lipska.pl
-Wróć do poprzedniej strony
-4 sierpnia, 2024
-Brak komentarzy</t>
+          <t>Adres „do eksmisji” za 500 zł? Umowa najmu okazjonalnego nie taka bezpieczna Adres „do eksmisji” za 500 zł? Umowa najmu okazjonalnego nie taka bezpieczna Potrzebne do zawarcia umowy oświadczenie łatwo kupić w internecie – kosztuje ok. 400 – 500 zł. Podaje to pod wątpliwość cały sens instytucji najmu okazjonalnego, bo w razie sporu pomiędzy stronami umowy może być to problematyczne dla ich obu.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://kancelaria-skarbiec.pl/jak-cudzoziemiec-moze-kupic-nieruchomosc-w-polsce-luka-w-ustawie/</t>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kodeks-cywilny-16785996/ks-3-tyt-17-dz-1</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Cenimy prywatność użytkowników
-Używamy plików cookie, aby poprawić jakość przeglądania, wyświetlać reklamy lub treści dostosowane do indywidualnych potrzeb użytkowników oraz analizować ruch na stronie. Kliknięcie przycisku „Akceptuj wszystkie” oznacza zgodę na wykorzystywanie przez nas plików cookie.
-Używamy plików cookie, aby pomóc użytkownikom w sprawnej nawigacji i wykonywaniu określonych funkcji. Szczegółowe informacje na temat wszystkich plików cookie odpowiadających poszczególnym kategoriom zgody znajdują się poniżej.
-Pliki cookie sklasyfikowane jako „niezbędne” są przechowywane w przeglądarce użytkownika, ponieważ są niezbędne do włączenia podstawowych funkcji witryny.... Pokaż więcej
-Niezbędne pliki cookie mają kluczowe znaczenie dla podstawowych funkcji witryny i witryna nie będzie działać w zamierzony sposób bez nich.Te pliki cookie nie przechowują żadnych danych umożliwiających identyfikację osoby.</t>
+          <t>Umowa najmu nieruchomości lub pomieszczenia na czas dłuższy niż rok powinna być zawarta na piśmie. W razie niezachowania tej formy poczytuje się umowę za zawartą na czas nieoznaczony. Jeżeli w czasie trwania najmu rzecz wymaga napraw, które obciążają wynajmującego, a bez których rzecz nie jest przydatna do umówionego użytku, najemca może wyznaczyć wynajmującemu odpowiedni termin do wykonania napraw. Po bezskutecznym upływie wyznaczonego terminu najemca może dokonać koniecznych napraw na koszt wynajmującego. Jeżeli osoba trzecia dochodzi przeciwko najemcy roszczeń dotyczących rzeczy najętej, najemca powinien niezwłocznie zawiadomić o tym wynajmującego.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Jak mogę wziąć ślub w Dolnośląskiem jako cudzoziemiec?</t>
+          <t>Jak długo mogę pozostać w Polskim po wygaśnięciu wizy?</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://tvn24.pl/wroclaw/wroclaw-czekaja-na-legalizacje-w-polsce-rodza-im-sie-dzieci-umieraja-bliscy-st7781158</t>
+          <t>https://migrant.poznan.uw.gov.pl/pl/faq/przedluzenie-wizy</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TVN24 na żywo
-TVN24 BiS na żywo
-TVN24 po ukraińsku
-TVN24NajnowszeŚwiatPolskaBiznesMeteoPremiumSportZdrowieTechnologiaKultura i stylCiekawostki
-FaktyZobacz FaktyFakty po FaktachFakty o ŚwiecieFakty po PołudniuLudzie Faktów</t>
+          <t>Jeżeli planujesz pobyt w Polsce po upływie ważności posiadanej wizy przez okres dłuższy niż 3 miesiące, powinieneś złożyć wniosek o zezwolenie na pobyt czasowy. Co do zasady, możesz przebywać w Polsce w celu turystycznym na podstawie ruchu bezwizowego lub wizy. Twój całkowity pobyt na terytorium wszystkich państw członkowskich obszaru Schengen bez konieczności uzyskania wizy nie może przekroczyć 90 dni w ciągu każdego 180-dniowego okresu. Przebywam cel turystyczny - przedłużenie ruchu bezwizowego</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.olsztyn-adwokat.pl/proces-uzyskiwania-zezwolenia-na-staly-pobyt-dla-cudzoziemca-malzonka-obywatela-polski/</t>
+          <t>https://www.gov.pl/attachment/c4067bab-e664-4072-8be5-6c90367ab4e3</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>O Kancelarii
-Zespół
-Zakres usług►Sprawy rodzinne i opiekuńczeSpadki i darowiznyWindykacja należności ochrona dłużnikówOdszkodowania zadośćuczynienia i rentyPrawo rzeczowe ochrona własności i posiadaniaZobowiązania roszczenia z umów i prawo konsumenckiePrawo gospodarcze i handlowePrawo pracy i ubezpieczeń społecznychObsługa prawna przedsiębiorcówPrawo karne i wykroczeniowePrawo administracyjneCudzoziemcyMediacjeSłużby mundurowe i Korpus Służby Cywilnej
-Sprawy rodzinne i opiekuńcze
-Spadki i darowizny</t>
+          <t>Jeżeli planujesz pobyt w Polsce po upływie ważności posiadanej wizy przez okres dłuższy niż 3 miesiące, powinieneś złożyć wniosek o zezwolenie na pobyt czasowy. Co do zasady, możesz przebywać w Polsce w celu turystycznym na podstawie ruchu bezwizowego lub wizy. Twój całkowity pobyt na terytorium wszystkich państw członkowskich obszaru Schengen bez konieczności uzyskania wizy nie może przekroczyć 90 dni w ciągu każdego 180-dniowego okresu. Przebywam cel turystyczny - przedłużenie ruchu bezwizowego</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://migrant.wsc.mazowieckie.pl/pl/procedury/malzonek-ma-zezwolenie-na-pobyt</t>
+          <t>https://zielonalinia.gov.pl/-/ruch-bezwizowy-ktorych-krajow-dotyczy-</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Przejdź do menu głównego
-Przejdź do treści
-Dostępność
-Strona główna
-Procedury</t>
+          <t>Przepisów dotyczących obowiązku wizowego i ruchu bezwizowego przy wjeździe do któregoś z krajów członkowskich należy szukać przede wszystkim w rozporządzeniu Parlamentu Europejskiego i Rady 2018/1806 z dnia 14 listopada 2018 r. wymieniające państwa trzecie, których obywatele muszą posiadać wizy podczas przekraczania granic zewnętrznych, oraz te, których obywatele są zwolnieni z tego wymogu. W załącznikach I i II do tego dokumentu wymienione są państwa, których obywatele są objęci obowiązkiem wizowym przy przekraczaniu granic zewnętrznych państw członkowskich oraz państwa, których obywatele są zwolnieni z tego obowiązku, gdy ich całkowity pobyt nie przekracza 90 dni w ciągu każdego 180-dniowego okresu. W załączniku nr II ww. rozporządzenia znajduje się wykaz państw trzecich, których obywatele są zwolnieni z obowiązku posiadania wizy podczas przekraczania granic zewnętrznych państw członkowskich na pobyt nie dłuższy niż 90 dni w okresie 180 dni. Są to: Państwa: była jugosłowiańska republika Macedonii, Andora, Zjednoczone Emiraty Arabskie, Antigua i Barbuda, Albania, Argentyna, Australia, Bośnia i Hercegowina, Barbados, Brunei, Brazylia, Bahamy, Kanada, Chile, Kolumbia, Kostaryka, Dominika, Mikronezja, Grenada, Gruzja, Gwatemala, Honduras, Izrael, Japonia, Kiribati, Saint Kitts i Nevis, Korea Południowa, Saint Lucia, Monako, Mołdawia, Czarnogóra, Wyspy Marshalla, Mauritius, Meksyk, Malezja, Nikaragua, Nauru, Nowa Zelandia, Panama, Peru, Palau, Paragwaj, Serbia ), Wyspy Salomona, Seszele, Singapur, San Marino, Salwador, Timor Wschodni, Tonga, Trynidad i Tobago, Tuvalu, Ukraina, Zjednoczone Królestwo Wielkiej Brytanii i Irlandii Północnej, Stany Zjednoczone Ameryki, Urugwaj, Stolica Apostolska, Saint Vincent i Grenadyny, Wenezuela, Vanuatu, Samoa, Tajwan .</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Jakie są wymagania dotyczące wiz łączenia rodzin w Dolnośląskiem?</t>
+          <t>Jakie dokumenty są potrzebne do pracy w Polsce?</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-czasowy/polaczenie-z-rodzina/</t>
+          <t>https://wroclaw.praca.gov.pl/dla-bezrobotnych-i-poszukujacych-pracy/abc-bezrobotnego-i-poszukujacego-pracy/dokumenty-potrzebne-do-rejestracji-osoby-bezrobotnej</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Kto składa wniosek?
-Kiedy powinienem / powinnam złożyć wniosek?
-Jak mogę złożyć wniosek?
-Jakie dokumenty muszę złożyć?
-Jakie są opłaty?</t>
+          <t>dowód osobisty albo inny dokument tożsamości np. paszport; oświadczenie dotyczące miejsca zameldowania, przy czym w przypadku gdy wyżej wymienione oświadczenie wzbudzi uzasadnione wątpliwości organu, urząd może zawsze wezwać do przedłożenia zaświadczenia o meldunku wydanego przez organ meldunkowy; świadectwa ukończenia szkoły, dyplomy lub inne dokumenty potwierdzające kwalifikacje lub zaświadczenia o ukończeniu szkolenia;</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://help.unhcr.org/poland/pl/dostep-do-uslug-dla-uznanych-uchodzcow/laczenie-rodzin/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/ou1611</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>العربية
-English
-Kurdî
-Русский
-Українська</t>
+          <t>Wypełnij i wyślij elektroniczny wniosek na portalu praca.gov.pl. Podpiszesz go podpisem kwalifikowanym lub profilem zaufanym. Zezwolenie typu A lub B na pracę cudzoziemca na terytorium Polski Jesteś przedsiębiorcą, masz firmę w Polsce i chcesz zatrudnić cudzoziemca spoza UE, EOG lub Szwajcarii? Musisz najpierw uzyskać zezwolenie na wykonywanie przez niego pracy typu A lub B. Przeczytaj, czym różnią się te zezwolenia i jak je uzyskać.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.migrant.info.pl/pl/pobyt-w-polsce-czlonkow-rodziny-obywateli-panstw-trzecich</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00210</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Pragniemy zwrócić Państwa uwagę, że zamieszczone na niniejszej stronie informacje nie stanowią źródła prawa. Zapewniamy, że dołożyliśmy wszelkich starań, by były one zgodne z obowiązującymi regulacjami. Prosimy jednak pamiętać, że niniejsza strona służy wyłącznie celom informacyjnym, a informacje na niej zamieszczone nie mogą stanowić podstawy w sporach z organami administracji publicznej. W razie wątpliwości zalecamy skontaktowanie się z organem prowadzącym postępowanie administracyjne w danej sprawie oraz zapoznanie się z przepisami prawa, które mogą mieć decydujący wpływ na jej rozstrzygnięcie. Zapraszamy również do kontaktu z prowadzoną przez nas infolinią migrant.info - +48 22 490 20 44
-Pragniemy zwrócić Państwa uwagę, że zamieszczone na niniejszej stronie informacje nie stanowią źródła prawa. Zapewniamy, że dołożyliśmy wszelkich starań, by były one zgodne z obowiązującymi regulacjami. Prosimy jednak pamiętać, że niniejsza strona służy wyłącznie celom informacyjnym, a informacje na niej zamieszczone nie mogą stanowić podstawy w sporach z organami administracji publicznej. W razie wątpliwości zalecamy skontaktowanie się z organem prowadzącym postępowanie administracyjne w danej sprawie oraz zapoznanie się z przepisami prawa, które mogą mieć decydujący wpływ na jej rozstrzygnięcie. Zapraszamy również do kontaktu z prowadzoną przez nas infolinią migrant.info - +48 22 490 20 44</t>
+          <t>Procedura uzyskania zezwolenia na pobyt czasowy i pracę, czyli zezwolenie jednolite jest korzystna, bo wszystkie formalności legalizujące pobyt i zatrudnienie cudzoziemca odbywają się w ramach jednego postępowania administracyjnego - cudzoziemiec nie musi odrębnie ubiegać się o zezwolenie na pobyt , a pracodawca - o zezwolenie na pracę. Wojewoda, który udzielił jednolitego zezwolenia na pobyt czasowy i pracę na terytorium Polski, wydaje cudzoziemcowi z urzędu kartę pobytu. Karta pobytu, w okresie w którym jest ważna, potwierdza tożsamość cudzoziemca oraz uprawnia go, wraz z dokumentem podróży, do wielokrotnego przekraczania granicy bez konieczności uzyskania wizy.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Jak mogę zarejestrować narodziny mojego dziecka w Dolnośląskiem?</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>https://www.mops.wroclaw.pl/10-formy-pomocy?start=27</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Przejdź do treści Przejdź do wyszukiwarki
-Deklaracja dostępności   Wysoki kontrast A- A A+
-Strona Główna</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>https://narodziny-milosci.pl/niemowle/</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Mama biologiczna dziecka ma zaledwie 15 lat. Nie jest gotowa do opieki nad Maleństwem, nie ma też żadnego wsparcia ze strony najbliższej rodziny. Mama pozostaje pod opieką lekarza, ciąża rozwija się prawidłowo.
-Potrzebna jest rodzina zastępcza dla jej dziecka, które urodzi się z końcem sierpnia (Nie adopcyjna!). Rodzina musi być świadoma, że do ukończenia przez mamę 18 roku życia Sąd nie wyda decyzji o odebraniu praw rodzicielskich i do tego czasu nie będzie możliwa adopcja.
-Szukamy rodziny, która będzie przygotowana na ewentualne dwa scenariusze. Pierwszy to: na powrót dziecka do mamy biologicznej po uzyskaniu przez nią pełnoletności lub drugi na adopcję dziecka, jeśli mama biologiczna nie będzie w stanie sie nim zająć.
-Zależy nam na rodzinie, która spróbuje pomóc mamie odnaleźć się w nowej roli, która okaże jej wsparcie (wsparcie, na które nie może liczyć ze strony swoich najbliższych). Może dzięki temu będzie w stanie w przysłości zatrzymać swoje dziecko.
-Osoby, (przede wszystkim te, które ukończyły szkolenia na rz i mieszkają w woj. dolnośląskim lub wielkopolskim) i chciałyby dowiedzieć się więcej – zapraszam do kontaktu po szczegółowe informacje: dzieckoadopcyjne@gmail.com – tu zawsze najszybciej odpowiadamy (ewentualnie na priv na FB).</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>https://mops.wroclaw.pl/10-formy-pomocy?start=30</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Przejdź do treści Przejdź do wyszukiwarki
-Deklaracja dostępności   Wysoki kontrast A- A A+
-Strona Główna</t>
-        </is>
-      </c>
+          <t>Jak uzyskać PESEL w Polsce?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Czy mogę prowadzić pojazd w Dolnośląskiem na zagranicznym prawie jazdy?</t>
+          <t>Jakie są prawa pracownika w Polsce?</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.prawo.pl/ukraina/3,strona.html</t>
+          <t>https://www.gov.pl/attachment/26e5c093-83dd-4b1b-9dd8-a353e0bd18af</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ukraina
-</t>
+          <t>Obowiązki pracownika i pracodawcy - Kodeks Pracy - ZL Źródła prawa pracy - Ministerstwo Rodziny, Pracy i Polityki ... Art. 100. - Kodeks pracy. - Dz.U.2025.277 t.j. - OpenLEX</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.rynek-kolejowy.pl/wiadomosci/tylko-pesa-chce-sprzedac-dwa-spalinowe-zespoly-trakcyjne-kolejom-dolnoslaskim-97822.html</t>
+          <t>https://www.gov.pl/web/rodzina/podstawowe-informacje-z-zakresu-prawa-pracy</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>SERWISY PARTNERSKIE
-rynekinfrastruktury.pl
-transport-publiczny.pl
-rynek-lotniczy.pl
-tor-konferencje.pl
-zdgtor.pl
-Biznes
-Infrastruktura
-Pasażer
-Prawo</t>
+          <t>Praca zdalna Ustawa z dnia 1 grudnia 2022 r. o zmianie ustawy – Kodeks pracy oraz niektórych innych ustaw wprowadziła do Kodeksu pracy pracę zdalną, jednocześnie uchylając przepisy dot. telepracy. Nowe przepisy regulujące pracę zdalną weszły w życie z dniem 7 kwietnia 2023 r. Kontrola trzeźwości i kontrola na obecność środków działających podobnie do alkoholu Ustawa z dnia 1 grudnia 2022 r. o zmianie ustawy – Kodeks pracy oraz niektórych innych ustaw wprowadziła do Kodeksu pracy możliwość kontroli trzeźwości pracowników i kontroli na obecność środków działających podobnie do alkoholu. Nowe przepisy weszły w życie z dniem 21 lutego 2023 r. Czas pracy Czas pracy stanowi jeden z najistotniejszych przedmiotów regulacji prawa pracy. Wyznacza bowiem granice czasowe, w ramach których pracodawca może żądać od pracownika gotowości do świadczenia pracy.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://bip.um.wroc.pl/attachments/download/152367</t>
+          <t>https://www.gov.pl/web/rodzina/zrodla-prawa-pracy</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>SERWISY PARTNERSKIE
-rynekinfrastruktury.pl
-transport-publiczny.pl
-rynek-lotniczy.pl
-tor-konferencje.pl
-zdgtor.pl
-Biznes
-Infrastruktura
-Pasażer
-Prawo</t>
+          <t>Podstawowym źródłem prawa pracy jest ustawa z dnia 26 czerwca 1974 r. - Kodeks pracy oraz akty wykonawcze do Kodeksu pracy. rozporządzenie Ministra Rodziny i Polityki Społecznej z dnia 8 maja 2023 r. w sprawie wniosków dotyczących uprawnień pracowników związanych z rodzicielstwem oraz dokumentów dołączanych do takich wniosków , rozporządzenie Ministra Pracy i Polityki Socjalnej z 8 stycznia 1997 r. w sprawie szczegółowych zasad udzielania urlopu wypoczynkowego, ustalania i wypłacania wynagrodzenia za czas urlopu oraz ekwiwalentu pieniężnego za urlop ,</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Jak mogę wymienić moje prawo jazdy na polskie w Dolnośląskiem?</t>
+          <t>Jak mogę wziąć ślub w Polskim jako cudzoziemiec?</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://dord.dolnyslask.pl/</t>
+          <t>https://powroty.gov.pl/-/slub-z-cudzoziemcem-w-polsce</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Witaj na stronie Dolnośląskiego Ośrodka Ruchu Drogowego. Wybierz miasto, które Cię interesuje, aby uzyskać więcej informacji o danym oddziale DORD.
-Możesz się zapisać na Egzamin online, kliknij wtedy przycisk na górze strony.</t>
+          <t>Zgodnie z polskim prawem związek małżeński mogą zawrzeć osoby pełnoletnie, które nie są w związku małżeńskim, nie są ze sobą spokrewnione w linii prostej oraz nie są rodzeństwem , nie są ze sobą spowinowaceni w linii prostej i nie są w stosunku przysposobienia . WYJĄTEK! Jeśli kobieta jest niepełnoletnia, ale ukończyła 16 lat lub osoby są ze sobą spowinowacone – mogą wziąć ślub, jeżeli uzyskają na to zgodę sądu. Ponadto, jeśli osoba jest dotknięta chorobą psychiczną albo niedorozwojem umysłowym – może wziąć ślub, jeżeli uzyska na to zgodę sądu. Osoby całkowicie ubezwłasnowolnione nie mogą zawrzeć związku małżeńskiego.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://flowapps.pl/blog/jak-wymienic-ukrainskie-prawo-jazdy-na-polskie/</t>
+          <t>https://www.gov.pl/web/gov/wez-slub-cywilny</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Strona główna — Blog — Porady — Jak wymienić ukraińskie prawo jazdy na polskie?
-utworzone przez Piotr | mar 4, 2025 | Porady | 0 komentarzy
-Jeśli jesteś obywatelem Ukrainy i przebywasz w Polsce, z pewnością zastanawiasz się, jak wygląda kwestia wymiany ukraińskiego prawa jazdy na polskie. Dzięki wprowadzeniu tymczasowych regulacji Unii Europejskiej, proces ten został uproszczony. Zgodnie z Rozporządzeniem Parlamentu Europejskiego i Rady (UE) z 2022 roku, ukraińskie prawo jazdy jest uznawane na terytorium Unii Europejskiej dla osób objętych tymczasową ochroną, bez konieczności dostarczania tłumaczeń lub międzynarodowego prawa jazdy.
-Ale… jeżeli zamierzasz pracować jako kierowca taksówki, lub wykonywać usługi przewozu, MUSISZ POSIADAĆ POLSKIE PRAWO JAZDY – jest to wymóg niepodlegający dyskusji. Na wstępnie należy wspomnieć, że jeżeli boisz się tych formalności to stoimy za Tobą murem – a Flow Apps oferuje pełne wsparcie i pomoc w procesie legalizacji pobytu i pracy dla cudzoziemców. W tym artykule przybliżamy, jak wygląda proces wymiany ukraińskiego prawa jazdy na polskie.
-W ostatnich miesiącach pojawia się wiele pytań dotyczących wymiany prawa jazdy dla obywateli krajów spoza Unii Europejskiej, w szczególności z Ukrainy i Białorusi. Kierowcy z tych państw stanowią istotną grupę pracowników, zwłaszcza w sektorze międzynarodowych przewozów dla polskich firm transportowych. W związku z zakończeniem obowiązywania tymczasowych przepisów związanych z konfliktem w Ukrainie oraz wprowadzeniem wymogu posiadania polskiego prawa jazdy dla osób świadczących odpłatne usługi transportowe (np. taksówki, przewozy w aplikacjach do 9 osób – takich jak m.in. Uber, Bolt, FreeNow, Bliq), warto przypomnieć kluczowe zasady dotyczące wymiany prawa jazdy dla kierowców z krajów trzecich.</t>
+          <t>Jeśli zdecydowaliście się na ślub cywilny – udajcie się do urzędu stanu cywilnego . Tam złożycie tak zwane zapewnienie o braku okoliczności wyłączających zawarcie małżeństwa oraz ustalicie termin ślubu. Możecie też zdecydować, czy ślub odbędzie się w urzędzie czy poza nim, na przykład w plenerze. Poniżej znajdziecie jedynie ogólne informacje – o szczegóły zapytajcie kierownika USC. Rozwiń tekst Kto może wziąć Ślub możecie wziąć, jeśli: jesteście pełnoletni, nie jesteście w związku małżeńskim, nie jesteście ze sobą spokrewnieni w linii prostej oraz nie jesteście rodzeństwem , nie jesteście ze sobą spowinowaceni w linii prostej , nie jesteście w stosunku przysposobienia . Jeśli kobieta jest niepełnoletnia, ale ukończyła 16 lat – może wziąć ślub, jeżeli uzyska na to zgodę sądu. Jeśli osoby są ze sobą spowinowacone – mogą wziąć ślub, jeżeli uzyskają na to zgodę sądu. Jeśli osoba jest dotknięta chorobą psychiczną albo niedorozwojem umysłowym – może wziąć ślub, jeżeli uzyska na to zgodę sądu. Osoby całkowicie ubezwłasnowolnione nie mogą zawrzeć związku małżeńskiego.</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://karta-pobytu.pl/baza-wiedzy/wymiana-zagranicznego-prawa-jazdy-na-polskie/</t>
+          <t>http://bip.brpo.gov.pl/pl/content/rpo-cudzoziemiec-malzenstwo-zaswiadczenie-problemy-mswia</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>astanawiasz się nad wymianą zagranicznego prawa jazdy na polskie? To może być konieczne, jeśli planujesz osiedlić się w Polsce i prowadzić pojazd. Nie martw się, nasz przewodnik krok po kroku uczyni ten proces zaskakująco prostym! W artykule omówimy procedurę wymiany, wymagane dokumenty, szczegóły dotyczące różnych krajów oraz przydatne informacje dla cudzoziemców. Rozpocznij swoją przygodę na polskich drogach z pewnością siebie!
-Wymiana zagranicznego prawa jazdy na polskie może być konieczna dla osób, które zamierzają mieszkać i prowadzić pojazd w Polsce. Proces ten może wydawać się skomplikowany, jednak dzięki temu przewodnikowi dowiesz się, jak przejść przez niego krok po kroku. W kolejnych sekcjach artykułu omówimy procedurę wymiany, dokumenty potrzebne do ubiegania się o wymianę, specyfikę wymiany prawa jazdy z różnych krajów oraz informacje dla cudzoziemców dotyczące tego procesu.
-Należy pamiętać, że procedury mogą się różnić w zależności od Twojej sytuacji indywidualnej oraz kraju, z którego pochodzi zagraniczne prawo jazdy. Warto skorzystać z profesjonalnej pomocy kancelarii prawnej, aby proces przebiegł sprawnie i zgodnie z obowiązującymi przepisami.
-Proces wymiany prawa jazdy polega na zamianie zagranicznego dokumentu uprawniającego do kierowania pojazdami na polski odpowiednik. Wymiana jest konieczna dla osób, które zamierzają mieszkać i prowadzić pojazd w Polsce na stałe. Ogólne zasady wymiany obejmują m.in. spełnienie wymogów formalnych: zgłoszenie się do odpowiedniego wydziału komunikacji, przedłożenie wymaganych dokumentów oraz opłacenie stosownych opłat.
-Procedura wymiany zagranicznego prawa jazdy na polskie składa się z kilku kroków. Po pierwsze, należy zgłosić się do wydziału komunikacji właściwego dla miejsca zamieszkania. Następnie, trzeba przedłożyć wymagane dokumenty, takie jak zagraniczne prawo jazdy, paszport, a także zaświadczenie o zameldowaniu. W niektórych przypadkach konieczne może być również przedstawienie tłumaczenia prawa jazdy na język polski. Po spełnieniu wszystkich formalności, urząd wyda decyzję o wymianie prawa jazdy, a następnie przekaże nowy dokument.</t>
+          <t>Problemy z zaświadczeniem wymaganym do ślubu z cudzoziemcem. Odpowiedzi MSWiA Niektóre Urzędy Stanu Cywilnego nie uwzględniają zaświadczeń cudzoziemca o możności zawarcia małżeństwa według prawa jego kraju i w nim wydawanych - jeśli nie ma w nich danych drugiej osoby mającej zawrzeć to małżeństwo Z polskich przepisów nie wynika wprost, że takie zaświadczenie musi zawierać dane drugiego z nupturientów</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Jakie są zasady rejestracji zagranicznego pojazdu w Dolnośląskiem?</t>
+          <t>Jakie są wymagania dotyczące wiz łączenia rodzin w Polskim?</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.powiatwroclawski.pl/wydzial-komunikacji.html</t>
+          <t>https://www.gov.pl/attachment/59d481b9-ee0d-449a-b03f-9f0b8f114669</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Strona główna
-Starostwo
-Wydziały / Biura</t>
+          <t>Zezwolenie na pobyt czasowy w celu połączenia się z ... Rodzic ma wizę/pobyt czasowy - Wydział Spraw Cudzoziemców Zezwolenie na pobyt czasowy dla członków rodzin obywateli ...</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://mubi.pl/poradniki/rejestracja-samochodu-z-zagranicy/</t>
+          <t>https://www.mos.cudzoziemcy.gov.pl/informacje/zwiazek-mal</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Zgoda
-Szczegóły
-[#IABV2SETTINGS#]
-O plikach cookies
-Korzystamy z plików cookie, aby nasza porównywarka działała prawidłowo (niezbędne pliki cookie) oraz aby zapewnić Ci spersonalizowane oferty i usługi (cookies funkcjonalne, analityczne i marketingowe).</t>
+          <t>Temporary residence permit for the purpose of family reunification Select an area of interest or explore the full information regarding the permit The migration rules ensure that certain sponsors who are third-country nationals or stateless persons can exercise their right to family reunification, including:</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://bip.um.wroc.pl/attachments/download/152367</t>
+          <t>https://www.gov.pl/web/mswia/warunki-wjazdu-i-pobytu-cudzoziemcow-w-polsce</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Zgoda
-Szczegóły
-[#IABV2SETTINGS#]
-O plikach cookies
-Korzystamy z plików cookie, aby nasza porównywarka działała prawidłowo (niezbędne pliki cookie) oraz aby zapewnić Ci spersonalizowane oferty i usługi (cookies funkcjonalne, analityczne i marketingowe).</t>
+          <t>ważną wizę długoterminową lub ważne zezwolenie na pobyt wydane przez polskie władze; dokument potwierdzający posiadanie ubezpieczenia zdrowotnego w rozumieniu przepisów ustawy z dnia 27 sierpnia 2004 r. o świadczeniach opieki zdrowotnej finansowanych ze środków publicznych lub posiadanie podróżnego ubezpieczenia medycznego o minimalnej kwocie ubezpieczenia w wysokości 30 000 euro, ważnego przez okres planowanego pobytu cudzoziemca na terytorium Rzeczypospolitej Polskiej, pokrywającego wszelkie wydatki, które mogą wyniknąć podczas pobytu na tym terytorium w związku z koniecznością podróży powrotnej z powodów medycznych, potrzebą pilnej pomocy medycznej, nagłym leczeniem szpitalnym lub ze śmiercią, w którym ubezpieczyciel zobowiązuje się do pokrycia kosztów udzielonych ubezpieczonemu świadczeń zdrowotnych bezpośrednio na rzecz podmiotu udzielającego takich świadczeń, na podstawie wystawionego przez ten podmiot rachunku – w przypadku wjazdu na podstawie wizy długoterminowej. Informacje Ministra Spraw Zagranicznych na temat ubezpieczycieli i ubezpieczeń spełniających te warunki można znaleźć tutaj: https://www.gov.pl/web/dyplomacja/wizy; Wymóg posaidania ubezpieczenia medycznego, o którym mowa powyżej, można uznać za spełniony, jeżeli cudzoziemiec posiada odpowiednie ubezpieczenie w związku ze swoją sytuacją zawodową; środki finansowe wystarczające na pokrycie kosztów planowanego pobytu oraz podróży powrotnej do państwa pochodzenia lub zamieszkania lub kosztów tranzytu do państwa trzeciego, które udzieli pozwolenia na wjazd, albo dokument potwierdzający możliwość uzyskania takich środków zgodnie z prawem</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Jak mogę ubiegać się o polskie obywatelstwo w Dolnośląskiem?</t>
+          <t>Czy mogę mieć podwójne obywatelstwo w Polskim?</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://dudkowiak.pl/prawo-imigracyjne/jak-uzyskac-polskie-obywatelstwo/</t>
+          <t>https://bip.brpo.gov.pl/pl/content/rpo-podwojne-obywatelstwo-paszport-wyjazd-sg-odpowiedz</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Strefa inwestora
-Wróć
-Inwestuj w Polsce
-Wróć
-Inwestuj w Polsce
-Kontrola inwestycji zagranicznych w Polsce
-Outsourcing IT – przewodnik
-Rejestracja spółek
-Wróć
-Rejestracja spółek
-Spółka komandytowa
-Spółka jawna
-Spółka cywilna
-Przedstawicielstwo w Polsce
-Oddział w Polsce
-Spółka zależna/celowa
-Spółki gotowe (spółki szelfowe, shelf companies)
-Otwarcie konta bankowego
-Spółka z ograniczoną odpowiedzialnością
-Spółka akcyjna
-Prawo pracy
-Wróć
-Prawo pracy
-Praca zdalna
-Jak zatrudnić pracownika w Polsce?
-Ile kosztuje zatrudnienie pracownika?
-Kalkulator podatkowy
-Rozwiązanie umowy o pracę
-Świadczenia pracownicze
-Sygnaliści – whistleblowers
-Wzór umowy o pracę
-Czas pracy
-Związki zawodowe
-Pracownicze Plany Kapitałowe (PPK)
-HR / Agencja pośrednictwa pracy
-Postępowanie sądowe
-Wróć
-Postępowanie sądowe
-Prawo morskie
-Prawo ubezpieczeniowe
-Arbitraż
-Kary administracyjne
-Prawo podatkowe
-Wróć
-Prawo podatkowe
-Podatek dochodowy od osób prawnych (CIT)
-Przewodnik po VAT
-Rejestracja dla celów podatku VAT
-Zwrot podatku VAT
-Podatek od zysków kapitałowych
-Podatek u źródła (WHT)
-Opinia WHT
-Podatek od dywidendy
-Zakład Podatkowy w Polsce (PE)
-Ceny Transferowe
-Schematy podatkowe MDR 
-Strategia podatkowa
-Podatek od czynności cywilnoprawnych (PCC)
-Podatek od nieruchomości
-Interpretacje podatkowe i Wiążąca Informacja Stawkowa
-Uprzednie porozumienia cenowe (APA)
-Ogólna klauzula przeciwko unikaniu opodatkowania (GAAR)
-Klauzula przeciwko unikaniu opodatkowania (SAAR)
-Zwolnienie podatkowe dla dostawców armii amerykańskiej w Polsce
-Czym jest Polska Fundacja Rodzinna?
-Cło antydumpingowe – jak uniknąć? 
-Windykacja należności
-Wróć
-Windykacja należności
-Nakazy sądowe/nakazy zapłaty
-Zabezpieczenie wierzytelności/roszczeń
-Wykonywanie wyroków zagranicznych
-Postępowanie egzekucyjne
-Stawka odsetek za zwłokę
-Upadłość i restrukturyzacja
-Termin przedawnienia
-Prawo kontraktowe
-Wróć
-Prawo kontraktowe
-Kontrakt B2B
-Franczyza
-Zakup nieruchomości
-Wróć
-Zakup nieruchomości
-Kupno mieszkania
-Zakup domu
-Zakup gruntów rolnych
-Due Diligence nieruchomości
-Rejestr nieruchomości
-Hipoteka
-Zakup nieruchomości i podatki
-Zakup nieruchomości przez cudzoziemca
-Najem nieruchomości
-Prawo budowlane
-Znak towarowy
-Fintech
-Wróć
-Fintech
-Implementacja MiCA w Polsce
-Instytucje pożyczkowe w Polsce
-Licencja CASP w Polsce
-Mała instytucja płatnicza
-Instytucja pieniądza elektronicznego
-Licencja VASP w Polsce | Licencja na kryptowaluty
-Pożyczki B2B/kredyty
-AML/CFT
-Prawo korporacyjne
-Wróć
-Prawo korporacyjne
-Kapitał zakładowy w sp. z o.o.
-Zarząd spółki
-Odpowiedzialność zarządu sp. z o.o. za zobowiązania
-Reprezentacja w spółce z o.o.
-Nadzór w spółce – Rada Nadzorcza
-Prokurent
-Zgromadzenie wspólników
-Dokapitalizowanie spółki
-Sprawozdawczość NBP
-Opodatkowanie spółki
-Księgowość w spółce
-UBO/ostateczny beneficjent rzeczywisty
-Przekształcenie w spółkę akcyjną
-Likwidacja spółki
-Rejestracja fundacji
-M&amp;A (fuzje i przejęcia)
-Wróć
-M&amp;A (fuzje i przejęcia)
-Umowy NDA w Polsce
-Kontrola koncentracji
-Due Diligence
-Opodatkowanie transakcji na udziałach
-Nabycie udziałów w spółce
-Sprzedaż udziałów w spółce
-Działalność regulowana
-Wróć
-Działalność regulowana
-Koncesja MSWiA na broń i wyroby wojskowe – poradnik
-Regulacje CBD w Polsce i UE
-Prawo górnicze – koncesje wydobywcze
-Prawo hazardowe
-Elektromobilność
-Prawo ochrony środowiska
-Wróć
-Prawo ochrony środowiska
-Ochrona wód i gruntów
-Produkcja chemikaliów
-Redukcja Emisji Gazów i Efektywność Energetyczna
-Prawo odpadowe
-Greenwashing
-CBAM
-Regulacja Zanieczyszczenia Powietrza
-Prawo karne
-Wróć
-Prawo karne
-Pranie brudnych pieniędzy – na czym polega i jakie są kary
-Europejski nakaz aresztowania (ENA)
-Odpowiedzialność karna podmiotów zbiorowych za czyny zabronione
-Blokada konta bankowego
-Zniesławienie
-Cyberprzestępczość i oszustwa bankowe
-Prawo antymonopolowe/prawo konkurencji
-Wróć
-Prawo antymonopolowe/prawo konkurencji
-Nieuczciwa konkurencja
-Ochrona konsumenta
-Terminy płatności (opóźnienia)
-Prawo reklamy
-Prawo imigracyjne
-Wróć
-Prawo imigracyjne
-Zatrudnianie obywateli Wielkiej Brytanii
-Zezwolenie na pobyt czasowy
-Jak uzyskać wizę do Polski
-Polskie obywatelstwo za inwestycje
-Zezwolenie na pracę w Polsce
-Potwierdzenie posiadania obywatelstwa polskiego
-Jak uzyskać polskie obywatelstwo?
-Zakup samochodu w Polsce
-Zatrudnianie cudzoziemców w Polsce
-Prawo spadkowe
-Wróć
-Prawo spadkowe
-Dziedziczenie ustawowe
-Dziedziczenie testamentowe
-Podatek od spadku
-Dziedziczenie nieruchomości
-Prawo autorskie
-Wróć
-Inwestuj w Polsce
-Wróć
-Inwestuj w Polsce
-Kontrola inwestycji zagranicznych w Polsce
-Outsourcing IT – przewodnik
-Wróć
-Inwestuj w Polsce</t>
+          <t>Masz dwa obywatelstwa - przy wyjeździe z Polski musisz okazać paszport RP. Odpowiedź Straży Granicznej Straż Graniczna odmawia obywatelom polskim z podwójnym obywatelstwem przekroczenia granicy w celu wyjazdu z Polski na podstawie paszportu innego państwa Tymczasem przepisy przyznają prawo do posiadania paszportu, a nie obowiązek. Zamieszkały w Polsce pełnoletni obywatel RP ma tylko obowiązek posiadania dowodu osobistego</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.lexmotion.eu/blog/requirements-for-polish-passport/</t>
+          <t>https://www.prawo.pl/prawo/podwojne-obywatelstwo-kiedy-mozliwe,523539.html</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Before applying for a Polish passport, you must first confirm your Polish citizenship. In this article, you will learn about the conditions and criteria that need to be met to obtain a Polish passport and enjoy its benefits.
-In today’s globalized world, the ability to move freely and pursue personal development has become increasingly important.
-A Polish passport grants visa-free entry to 176 out of over 195 countries worldwide, making it one of the most valuable travel documents available.</t>
+          <t>Zatrzymany w Dubaju Sebastian M., posiadający obywatelstwo polskie i niemieckie, nie jest wyjątkiem. W coraz bardziej globalizującym się świecie po dwa, a nawet więcej paszportów w walizce ma legalnie coraz więcej osób, choć nie wszystkie państwa patrzą na to przychylnie. „Podwójne obywatelstwo służy zarówno jako polisa ubezpieczeniowa, jak i metoda otwierania nowych możliwości. Posiadanie drugiego paszportu to też plan B na wypadek, gdyby w twoim kraju wprowadzono jakieś dziwne, nieakceptowalne przepisy, albo rząd był niestabilny” - przekonuje Andrew Henderson z firmy Nomad Capitalist z Austin , która specjalizuje się w inwestycjach typu off shore i optymalizacji podatkowej. Nie zawsze jednak łatwo o podwójne obywatelstwo - ośmiu europejskich Japończyków wystąpiło z pozwem umożliwienie im posiadania podwójnego obywatelstwa z wyboru . Sąd Najwyższy w Tokio w wyroku z 28 września br. oddalił jednak ich roszczenia i uznał za zgodną z Konstytucją automatyczną utratę japońskiego obywatelstwa w razie dobrowolnego nabycia innego. „Podwójne obywatelstwo może spowodować konflikt w prawach i obowiązkach między krajami, a także między jednostką a państwem" – argumentują sędziowie japońskiego SN w uzasadnieniu. Wiele osób pochodzenia japońskiego mieszka np. w USA, Brazylii, Peru, w krajach Europy Zachodniej, na Filipinach. Japońska diaspora na całym świecie liczy nawet ok. 4 mln osób. Jeśli z jakichś powodów mają prawo do podwójnego obywatelstwa, to stają przed dylematem, które wybrać. Ministerstwo Sprawiedliwości w Tokio przypomina, że zgodnie z obowiązującymi od 1985 r. przepisami Japonia dopuszcza jedynie podwójne obywatelstwo osób młodszych niż 22 lata. Kończąc ten wiek należy zdecydować – czy zostaje się przy obywatelstwie japońskim, czy wybiera obce. Tak w 2019 r. zrobiła znana tenisistka Naomi Osaka, która oddała paszport USA. Odpowiednie oświadczenie w tej sprawie trzeba złożyć urzędnikom na Wyspach, a za granicą w konsulacie bądź ambasadzie Kraju Kwitnącej Wiśni. Natomiast ci, którzy podwójne obywatelstwo uzyskali po dwudziestych urodzinach, mają od tego momentu dwa lata czasu na wybór, który paszport chcą mieć w kieszeni. Japonia nie jest wyjątkiem - na liście państw pozbawiających automatycznie swojego obywatelstwa osoby, które nabędą inne, są także Indie, Chiny i Zjednoczone Emiraty Arabskie. Obywatelstwo Kraju Kwitnącej Wiśni należy też do tych, które najtrudniej zdobyć, nawet osobom z japońskimi korzeniami albo pracującymi w Japonii. „To skomplikowana droga, skupiamy się głównie na wnioskach Koreańczyków zatrudnionych u nas od wielu lat i mających tu osoby bliskie” – podkreśla Ikuko Maekawa, prawniczka mająca biuro w Osace.</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://migrant.wsc.mazowieckie.pl/pl/procedury/nadanie-obywatelstwa-polskiego</t>
+          <t>https://powroty.gov.pl/czy-obywatel-polski-z-podwojnym-obywatelstwem-moze-w-polsce-poslugiwac-sie-amerykanskimi-dokumentami-jako-obywatel-jakiego-kraju-bedzie-tra-24074</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Przejdź do menu głównego
-Przejdź do treści
-Dostępność
-Strona główna
-Procedury</t>
+          <t>Czy obywatel polski z podwójnym obywatelstwem może w Polsce posługiwać się amerykańskimi dokumentami? Jako obywatel jakiego kraju będzie traktowany po powrocie z emigracji? Czy obywatel polski z podwójnym obywatelstwem może w Polsce posługiwać się amerykańskimi dokumentami? Jako obywatel jakiego kraju będzie traktowany po powrocie? Przepisy prawa regulujące kwestie obywatelstwa polskiego zawarte są w Konstytucji Rzeczypospolitej Polskiej oraz w ustawie z dnia 2 kwietnia 2009 r. o obywatelstwie polskim . Prawo polskie nie zakazuje obywatelom polskim uzyskania obywatelstwa obcego, czy to poprzez urodzenie czy proces naturalizacji, polskie władze uznają jednak jedynie polskie obywatelstwo takiej osoby.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Jakie są wymagania językowe dotyczące uzyskania obywatelstwa w Dolnośląskiem?</t>
+          <t>Jak zgłosić pobyt czasowy w Polsce?</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.migrant.info.pl/pl/uznanie-za-obywatela</t>
+          <t>https://www.gov.pl/web/gov/zamelduj-sie-na-pobyt-staly-lub-czasowy-dluzszy-niz-3-miesiace</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Pragniemy zwrócić Państwa uwagę, że zamieszczone na niniejszej stronie informacje nie stanowią źródła prawa. Zapewniamy, że dołożyliśmy wszelkich starań, by były one zgodne z obowiązującymi regulacjami. Prosimy jednak pamiętać, że niniejsza strona służy wyłącznie celom informacyjnym, a informacje na niej zamieszczone nie mogą stanowić podstawy w sporach z organami administracji publicznej. W razie wątpliwości zalecamy skontaktowanie się z organem prowadzącym postępowanie administracyjne w danej sprawie oraz zapoznanie się z przepisami prawa, które mogą mieć decydujący wpływ na jej rozstrzygnięcie. Zapraszamy również do kontaktu z prowadzoną przez nas infolinią migrant.info - +48 22 490 20 44
-Pragniemy zwrócić Państwa uwagę, że zamieszczone na niniejszej stronie informacje nie stanowią źródła prawa. Zapewniamy, że dołożyliśmy wszelkich starań, by były one zgodne z obowiązującymi regulacjami. Prosimy jednak pamiętać, że niniejsza strona służy wyłącznie celom informacyjnym, a informacje na niej zamieszczone nie mogą stanowić podstawy w sporach z organami administracji publicznej. W razie wątpliwości zalecamy skontaktowanie się z organem prowadzącym postępowanie administracyjne w danej sprawie oraz zapoznanie się z przepisami prawa, które mogą mieć decydujący wpływ na jej rozstrzygnięcie. Zapraszamy również do kontaktu z prowadzoną przez nas infolinią migrant.info - +48 22 490 20 44</t>
+          <t>Zamelduj się na pobyt stały lub czasowy dłuższy niż 3 miesiące Zmieniasz miejsce zamieszkania? A może wracasz z zagranicy i nie masz meldunku w Polsce? Pamiętaj, żeby się zameldować. Możesz to zrobić przez internet albo w urzędzie gminy. Jeśli jesteś obywatelem Polski i twoje dziecko urodziło się w Polsce – kierownik urzędu stanu cywilnego, który sporządził akt urodzenia, z urzędu zamelduje twoje dziecko.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.dsw.edu.pl/strefa-studenta/aktualne-informacje-dla-studentow</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00210</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Szanowni Państwo,
-od 20 do 28 listopada 2024 r. ruszają elektroniczne zapisy na moduły kształcenia wybieralnego (specjalnościowego) poprzez system USOSWeb dla Studentów następujących kierunków:
-Geodezja i kartografia,
-Informatyka,</t>
+          <t>Procedura uzyskania zezwolenia na pobyt czasowy i pracę, czyli zezwolenie jednolite jest korzystna, bo wszystkie formalności legalizujące pobyt i zatrudnienie cudzoziemca odbywają się w ramach jednego postępowania administracyjnego - cudzoziemiec nie musi odrębnie ubiegać się o zezwolenie na pobyt , a pracodawca - o zezwolenie na pracę. Wojewoda, który udzielił jednolitego zezwolenia na pobyt czasowy i pracę na terytorium Polski, wydaje cudzoziemcowi z urzędu kartę pobytu. Karta pobytu, w okresie w którym jest ważna, potwierdza tożsamość cudzoziemca oraz uprawnia go, wraz z dokumentem podróży, do wielokrotnego przekraczania granicy bez konieczności uzyskania wizy.</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>http://www.przysiegly-niderlandzki-miw.pl/Blog%20Posts/jak-zostac-tlumaczem.html</t>
+          <t>https://www.gov.pl/web/uw-warminsko-mazurski/cudzoziemcy---zezwolenia-na-pobyt-czasowy-na-terytorium-rp</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-By zostać tłumaczem przysięgłym języka holenderskiego należy  przede wszystkim biegle posługiwać się językiem niderlandzkim oraz polskim, ale  nie tylko. Od 2006 roku należy również dodatkowo  zdać dwustopniowy egzamin w Ministerstwie Sprawiedliwości, składający się z  części pisemnej oraz ustnej. Niestety znajomość obu języków oraz pozytywne  przejście egzaminu nie uprawnia jeszcze tłumacza do wykonywania  tłumaczeń wierzytelnych.
-Zawód tłumacza przysięgłego jest zawodem zaufania  publicznego, dlatego też na podstawie Ustawy o Zawodzie Tłumacza Przysięgłego od  kandydatów wymaga się, by:
-Posiadali obywatelstwo polskie lub  obywatelstwo innego kraju UE lub EFTA, ewentualnie obywatelstwo kraju objętego „zasadą  wzajemności”,
-Nie byli karani za przestępstwa  umyślne, skarbowe oraz gospodarcze,</t>
+          <t>Szczegółowe informacje znajdziesz na stronie Urzędu do Spraw Cudzoziemców w Module Obsługi Spraw pod linkiem: https://www.mos.cudzoziemcy.gov.pl/potrzebuje-informacji/pobyt-czas https://mos.cudzoziemcy.gov.pl/potrzebuje-informacji/szczegolne-okol</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Czy mogę mieć podwójne obywatelstwo w Dolnośląskiem?</t>
+          <t>Co powinno być zawarte w mojej umowie o pracę w Polskim?</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://kancelariadso.pl/aktualnosci/czy-mozna-miec-podwojne-obywatelstwo</t>
+          <t>https://zielonalinia.gov.pl/-/umowa-o-prace-co-powinna-zawierac</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Start
-right-arrow_777</t>
+          <t>Przed rozpoczęciem zatrudnienia pracodawca powinien podpisać z Tobą umowę o pracę. Zgodnie z Kodeksem pracy, art. 29 §2 Umowę o pracę zawiera się na piśmie. Jeżeli umowa o pracę nie została zawarta z zachowaniem formy pisemnej, pracodawca przed dopuszczeniem pracownika do pracy potwierdza pracownikowi na piśmie ustalenia co do stron umowy, rodzaju umowy oraz jej warunków. Niedopuszczalnym jest świadczenie pracy bez podpisanej umowy lub ustalonych na piśmie warunków.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://czasopisma.uwm.edu.pl/index.php/sp/article/download/8796/7205/33470</t>
+          <t>https://zielonalinia.gov.pl/obowiazki-pracownika-i-pracodawcy-33373</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Start
-right-arrow_777</t>
+          <t>zaznajamianie pracowników podejmujących pracę z zakresem ich obowiązków, sposobem wykonywania pracy oraz ich podstawowymi uprawnieniami, zapewnienie bezpiecznych i higienicznych warunków pracy oraz systematyczne szkolenie pracowników w tym zakresie, ułatwianie pracownikom podnoszenia kwalifikacji zawodowych,</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.radiowroclaw.pl/articles/view/137528/J-Protasiewicz-o-wnioskach-cudzoziemcow-Przez-2-lata-nie-zdazylibysmy-ich-obsluzyc-Trzeba-to-usprawnic</t>
+          <t>https://zielonalinia.gov.pl/umowa-o-prace-33374</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Gościem Rozmowy Dnia Radia Wrocław był Jacek Protasiewicz, wicewojewoda dolnośląski.
-Chciałem powiedzieć na początek, że administracja rządowa to miejsce, w którym pan dotąd nie pracował, ale pan sprostował, że 34 lata temu był pan rzecznikiem wojewody dolnośląskiego.
-Tak. To była pierwsza praca, taka w okresie romantycznym, kiedy Polska przechodziła z systemu autorytarnego, PRL-owskiego, na ten demokratyczny. Rząd Tadeusza Mazowieckiego powołał pierwszych wojewodów, no nie PZPR-owskich i rzecznikiem pierwszego wojewody, pana Jarosława Muszyńskiego, byłem ja. Także praca na tym samym korytarzu, po przeciwnej stronie korytarza był mój gabinet.</t>
+          <t>na okres próbny do trzech miesięcy, w celu sprawdzenia kwalifikacji pracownika, minimalne wynagrodzenie , zakaz wypowiadania i rozwiązywania stosunku pracy w szczególnych przypadkach,</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Czy mogę otworzyć konto bankowe w Dolnośląskiem jako cudzoziemiec?</t>
+          <t>Jakie są składki na opiekę zdrowotną i ubezpieczenie społeczne dla cudzoziemców w Polskim?</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.pkobp.pl/klient-indywidualny/konta/jak-otworzyc-konto-osobiste?srsltid=AfmBOor8QFuVbvFvLpCHmHjqVDV1jKiWzNgsRO1j59LoGr1zEca6kGvy</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00291</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Otwórz konto bankowe przez internet i wybierz, jak podpisać umowę - potwierdź tożsamość online na selfie lub odbierz przesyłkę kurierską z umową
-Pobierz i uruchom aplikację IKO, a następnie wybierz Otwórz konto na selfie
-Podaj dane kontaktowe, udziel odpowiednie zgody oraz wybierz rodzaj konta i kartę płatniczą. Zrób zdjęcia swojego dowodu osobistego i twarzy, sprawdź poprawność danych, wskaż adres zamieszkania, zaakceptuj oświadczenia i złóż wniosek
-Podpisz umowę online i korzystaj ze swojego konta!Niektóre funkcje np. e-Urząd będą wymagały dodatkowego potwierdzenia tożsamości w oddziale1
-Jak szybko przenieść konto do PKO Banku Polskiego?</t>
+          <t>Kto może prowadzić działalność gospodarczą w Polsce Nawet gdy nie posiadasz polskiego obywatelstwa, masz prawo podejmować i wykonywać działalność gospodarczą w Polsce. Ponadto możesz oferować lub świadczyć czasowo swoje usługi albo założyć w Polsce oddział lub przedstawicielstwo swojej firmy.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.kontomaniak.pl/poradniki/konto-dla-obcokrajowca-gdzie-zalozyc</t>
+          <t>https://www.gov.pl/web/zdrowie/finansowanie-leczenia-cudzoziemcow-w-polsce</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Dane statystyczne wskazują na to, że w Polsce w 2024 roku mieszka około 2,5 miliona obcokrajowców. To spora liczba osób, z których wiele pracuje lub uczy się w naszym kraju. Posiadają również rachunki bankowe. W tym artykule sprawdzimy, czym powinno charakteryzować się konto dla obcokrajowca, w jaki sposób je założyć oraz gdzie to zrobić.
-Spis treści:
-Jak założyć konto dla obcokrajowca?
-Konto dla obcokrajowca – dokumenty
-Czy można założyć konto dla obcokrajowca bez karty pobytu?</t>
+          <t>Jeśli jesteś ubezpieczony w państwach członkowskich UE/EFTA Jeśli twój pobyt ma charakter czasowy możesz otrzymać tylko niezbędną opiekę medyczną. Poniższe świadczenia uzyskasz na takich samych zasadach, co osoby ubezpieczone w Polsce: zaopatrzenie w przedmioty ortopedyczne oraz środki pomocnicze,</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://polskabezgotowkowa.pl/dla-ciebie/artykuly/jak-zalozyc-konto-w-banku-bez-polskiego-obywatelstwa/</t>
+          <t>https://www.gov.pl/web/rodzina/pomoc-spoleczna-dla-cudzoziemcow-na-jakie-wsparcie-w-polsce-moga-liczyc</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About
-Necessary   6 Necessary cookies help make a website usable by enabling basic functions like page navigation and access to secure areas of the website. The website cannot function properly without these cookies.Cookiebot1Learn more about this providerCookieConsentStores the user's cookie consent state for the current domainMaximum Storage Duration: 1 yearType: HTTP CookieCriteo1Learn more about this provideroptoutIdentifies if the visitor has deselected any cookies, trackers or other audience targeting tools.Maximum Storage Duration: SessionType: HTTP CookieGoogle2Learn more about this providerSome of the data collected by this provider is for the purposes of personalization and measuring advertising effectiveness.ar_debugChecks whether a technical debugger-cookie is present. Maximum Storage Duration: 30 daysType: HTTP Cookietest_cookieUsed to check if the user's browser supports cookies.Maximum Storage Duration: 1 dayType: HTTP CookieID51Learn more about this providergdprDetermines whether the visitor has accepted the cookie consent box. This ensures that the cookie consent box will not be presented again upon re-entry.  Maximum Storage Duration: SessionType: HTTP CookieNativo1Learn more about this provideropt_outUsed to detect if the visitor has accepted the marketing category in the cookie banner. This cookie is necessary for GDPR-compliance of the website.  Maximum Storage Duration: 1 yearType: HTTP Cookie</t>
+          <t>Pomoc społeczna dla cudzoziemców. Na jakie wsparcie w Polsce mogą liczyć? Cudzoziemcy w Polsce nie są pozostawieni sami sobie. Na jakie wsparcie w ramach pomocy społecznej mogą liczyć? Jakie warunki muszą spełnić? Wyjaśniamy w praktycznym przewodniku. Osobami uprawnionymi do korzystania z pomocy społecznej – oprócz osób posiadających obywatelstwo polskie – są także cudzoziemcy, którzy mają miejsce zamieszkania i przebywają na terenie Polski m.in.:</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Jakie dokumenty są potrzebne do ubiegania się o kredyt lub hipotekę w Dolnośląskiem?</t>
+          <t>Jakie są wymagania dotyczące stałego pobytu w Polskim?</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.kingaburcan.pl/doradca-kredytowy-wroclaw/kredyt-hipoteczny-wroclaw/</t>
+          <t>https://powroty.gov.pl/zezwolenie-na-pobyt-staly-10025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About
-Necessary   6 Necessary cookies help make a website usable by enabling basic functions like page navigation and access to secure areas of the website. The website cannot function properly without these cookies.Google3Learn more about this providerSome of the data collected by this provider is for the purposes of personalization and measuring advertising effectiveness.test_cookiePendingMaximum Storage Duration: 1 dayType: HTTP Cookierc::aThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maximum Storage Duration: PersistentType: HTML Local Storagerc::cThis cookie is used to distinguish between humans and bots. Maximum Storage Duration: SessionType: HTML Local StorageUsercentrics GmbH2Learn more about this providerucDataStores the user's cookie consent state for the current domainMaximum Storage Duration: PersistentType: HTML Local StorageucStringNecessary for the correct implementation of the websites Consent Management Platform (CMP)Maximum Storage Duration: PersistentType: HTML Local Storagewww.kingaburcan.pl1CookieConsentStores the user's cookie consent state for the current domainMaximum Storage Duration: 1 yearType: HTTP Cookie</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>https://erif.pl/poradnik-konsumenta/jak-dostac-kredyt-na-mieszkanie-jakie-warunki-nalezy-spelnic/</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Strona główna  Poradnik konsumenta  Jak dostać kredyt na mieszkanie? Jakie warunki należy spełnić?
-Dla większości z nas realizacja marzenia o własnym domu lub mieszkaniu wiąże się z koniecznością zaciągnięcia kredytu hipotecznego. To długoterminowe zobowiązanie stanowi dla banków spore ryzyko, dlatego przed udzieleniem kredytu stawiają one przyszłemu kredytobiorcy szereg warunków do spełnienia. Z naszego artykułu dowiesz się, jak wziąć kredyt hipoteczny oraz jak zwiększyć swoje szanse na uzyskanie pozytywnej decyzji kredytowej.
-Kredyt hipoteczny to zobowiązanie finansowe, którego zabezpieczeniem jest hipoteka. To oznacza, że jeśli przestaniesz spłacać raty, bank może sprzedać zastawioną nieruchomość (za pośrednictwem komornika), aby w ten sposób odzyskać pożyczone pieniądze.
-Warto wiedzieć, że kredytodawca nie zyskuje takich uprawnień automatycznie. Hipoteka to ograniczone prawo do rzeczy i ustanawia ją właściciel nieruchomości, dokonując wpisu do ksiąg wieczystych już po przyznaniu kredytu. Wykreślenie wpisu następuje po spłacie zobowiązania.Hipoteka obciąża nieruchomość, a nie właściciela. Można więc zarówno sprzedać mieszkanie z hipoteką, jak i je kupić. Nowy właściciel będzie wówczas zobligowany do spłaty zobowiązania. Przed zakupem nieruchomości sprawdź księgi wieczyste, aby upewnić się, że na nieruchomości nie ciąży zadłużenie.</t>
-        </is>
-      </c>
+          <t>Legalizacja pobytu w Polsce małżonka/partnera cudzoziemca Informacje zgodne ze stanem prawnym na dzień: 2024-09-04 Małżonek obywatela polskiego, niebędący obywatelem jednego z państw EOG lub Szwajcarii, czyli obywatel tzw. kraju trzeciego, może się starać o zezwolenie na pobyt stały.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://grupaang.pl/kredyty-i-pozyczki/pozyczka-hipoteczna/</t>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/cudzoziemcy-18053962/art-195</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Zgoda
-Szczegóły
-[#IABV2SETTINGS#]
-O plikach cookies
-Niezbędne  12 Niezbędne pliki cookie są absolutnie niezbędne do prawidłowego funkcjonowania strony internetowej. Te pliki cookie anonimowo zapewniają podstawowe funkcje i zabezpieczenia strony internetowej.Google7Dowiedz się więcej na temat tego dostawcyNiektóre dane gromadzone przez tego dostawcę służą do personalizacji i pomiaru skuteczności reklamy.test_cookieW oczekiwaniuMaksymalny okres przechowywania: 1 dzieńRodzaj: Plik cookie HTTP_GRECAPTCHAThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maksymalny okres przechowywania: 180 dniRodzaj: Plik cookie HTTP_grecaptchaThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maksymalny okres przechowywania: StałeRodzaj: Lokalny magazyn HTMLrc::aThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maksymalny okres przechowywania: StałeRodzaj: Lokalny magazyn HTMLrc::bThis cookie is used to distinguish between humans and bots. Maksymalny okres przechowywania: SesyjneRodzaj: Lokalny magazyn HTMLrc::cThis cookie is used to distinguish between humans and bots. Maksymalny okres przechowywania: SesyjneRodzaj: Lokalny magazyn HTMLrc::fThis cookie is used to distinguish between humans and bots. Maksymalny okres przechowywania: StałeRodzaj: Lokalny magazyn HTMLangfinanse.pl1wpEmojiSettingsSupportsThis cookie is part of a bundle of cookies which serve the purpose of content delivery and presentation. The cookies keep the correct state of font, blog/picture sliders, color themes and other website settings.Maksymalny okres przechowywania: SesyjneRodzaj: Lokalny magazyn HTMLconsent.cookiebot.comporownywarkahipoteczna.angfinanse.pl2CookieConsent [x2]Stores the user's cookie consent state for the current domainMaksymalny okres przechowywania: 1 rokRodzaj: Plik cookie HTTPporownywarkahipoteczna.angfinanse.pl1tokenUsed to make live streaming of video content more efficient.Maksymalny okres przechowywania: StałeRodzaj: Lokalny magazyn HTMLwww.un.org.pl1PHPSESSIDPreserves user session state across page requests.Maksymalny okres przechowywania: SesyjneRodzaj: Plik cookie HTTP</t>
+          <t>Art. 195. - - Cudzoziemcy. Jeżeli chcesz mieć dostęp do wszystkich dokumentów powiązanych, zaloguj się do LEX-a Nie korzystasz jeszcze z programów LEX? Zamów dostęp testowy » W jaki sposób można zatrudnić cudzoziemca posiadającego zezwolenie na pobyt stały?</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Jak mogę zgłosić przestępstwo jako cudzoziemiec w Dolnośląskiem?</t>
+          <t>Jakie są zasady rejestracji zagranicznego pojazdu w Polskim?</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-staly/</t>
+          <t>https://samorzad.gov.pl/web/powiat-jasielski/rejestracja-pojazdu-sprowadzonego-z-zagranicy</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Kto składa wniosek?
-Kiedy powinienem / powinnam złożyć wniosek?
-Jak mogę złożyć wniosek?
-Jakie dokumenty muszę złożyć?
-Jakie są opłaty?</t>
+          <t>Rejestracja pojazdu używanego sprowadzonego z zagranicy I. Wniosek II. Załączniki do wniosku: 1) Dowód własności pojazdu, a w przypadku powierzenia pojazdu przez zagraniczną osobę prawną lub fizyczną podmiotowi polskiemu – dokument potwierdzający powierzenie pojazdu, 2) Oświadczenie o dacie sprowadzenia pojazdu z terytorium państwa członkowskiego Unii Europejskiej, jeżeli zostało dołączone do dowodu własności pojazdu, 3) Dowód rejestracyjny, jeżeli pojazd był zarejestrowany - stroną umowy o Europejskim Obszarze Gospodarczym, zamiast dowodu rejestracyjnego dopuszcza się przedstawienie innego dokumentu stwierdzającego rejestrację pojazdu, wydanego przez organ właściwy do rejestracji pojazdów w tym państwie), 4) Tablice rejestracyjne, jeżeli pojazd był zarejestrowany; w przypadku pojazdu sprowadzonego z zagranicy bez tablic rejestracyjnych albo konieczności zwrotu tych tablic organowi rejestrującemu państwa, z którego pojazd został sprowadzony, właściciel pojazdu zamiast tablic rejestracyjnych dołącza oświadczenie, że pojazd został sprowadzony z zagranicy bez tablic rejestracyjnych albo oświadczenie o konieczności zwrotu tych tablic organowi rejestrującemu państwa, z którego pojazd został sprowadzony; oświadczenie może być złożone na wniosku o rejestrację, w tym na jego odwrocie, 5) Dowód odprawy celnej przywozowej, jeżeli pojazd został sprowadzony z terytorium państwa niebędącego państwem członkowskim Unii Europejskiej i jest rejestrowany po raz pierwszy. W przypadku sprzedaży pojazdu przez przedsiębiorcę prowadzącego działalność w zakresie obrotu pojazdami dokument ten może być zastąpiony adnotacją na fakturze określającą datę i numer dowodu odprawy celnej przywozowej oraz nazwę organu, który dokonał odprawy celnej. 6) Dokument potwierdzający zapłatę akcyzy na terytorium kraju albo dokument potwierdzający brak obowiązku zapłaty akcyzy na terytorium kraju albo zaświadczenie stwierdzające zwolnienie od akcyzy, w rozumieniu przepisów o podatku akcyzowym, jeżeli samochód osobowy, pojazd rodzaju "samochodowy inny", podrodzaj "czterokołowiec" lub podrodzaj "czterokołowiec lekki" , samochód ciężarowy , podrodzaj "furgon", "furgon/podest", "ciężarowo-osobowy", "terenowy", "wielozadaniowy" lub "van" lub samochód specjalny , został sprowadzony z terytorium państwa członkowskiego Unii Europejskiej i jest rejestrowany po raz pierwszy.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.podlaski.strazgraniczna.pl/pod/cudzoziemcy/konsekwencje-nielegalne</t>
+          <t>https://powroty.gov.pl/-/rejestracja-samochodu-sprowadzonego-z-zagranicy-krok-po-kroku</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Przejdź do menu głównego
-Przejdź do treści
-Przejdź do wyszukiwarki
-Mapa strony
-Strona główna</t>
+          <t>W Polsce zakup samochodu sprowadzonego z zagranicy jest bardzo popularną formą nabycia dwuśladu. Dane statystyczne wskazują, że takich aut przybywa u nas około miliona rocznie. Nie brakuje też samochodów kupionych przez Polaków za granicą, używanych tam i sprowadzonych po powrocie do Polski. Zgodnie z Art.71 ust. 1. ustawy Prawo o ruchu drogowym: dokumentem stwierdzającym dopuszczenie do ruchu pojazdu samochodowego jest dowód rejestracyjny albo pozwolenie czasowe. W związku z tym każdy samochód, który nie był jeszcze zarejestrowany w Polsce, należy zarejestrować .</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://kancelaria-adwokacka-warszawa.pl/deportacja/</t>
+          <t>https://powroty.gov.pl/procedura-rejestracji-9531</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>W przypadku gdy cudzoziemiec nie posiada żadnego tytułu pobytowego w Polsce np. wizy lub zezwolenia na pobyt, jego pobyt tutaj jest nielegalne i grozi mu deportacja z Polski. Decyzja o zobowiązaniu do powrotu jest wydawana przez właściwego Komendanta Straży Granicznej. W decyzji deportacyjnej może zostać określony termin dobrowolnego powrotu od 15 do 30 dni. Jednak w przypadku, gdy istnieje prawdopodobieństwo, że cudzoziemiec dobrowolnie nie opuści Polski albo wymagają tego względy obronności lub bezpieczeństwa państw, terminu dobrowolnego powrotu nie określa się, a wykonanie decyzji jest natychmiastowe. Oznacza to, że deportacja imigranta następuje od razu bez względu na to, że przysługuje mu prawo złożenia odwołania od takiej decyzji.
-Należy pamiętać, że ustawa o cudzoziemcach przewiduje również możliwość deportacji cudzoziemca przebywającego legalnie w Polsce. Przyczynami deportacji są w takim przypadku m.in. wykonywanie pracy bez odpowiedniego zezwolenia, podjęcie działalności gospodarczej niezgodnie z przepisami, skazanie prawomocnym wyrokiem w Rzeczypospolitej Polskiej na karę pozbawienia wolności, uznanie przez organ że dalszy pobyt cudzoziemca stanowi zagrożenie dla porządku i bezpieczeństwa publicznego nawet bez skazania przez sąd wyrokiem karnym, czy też ustalenia przez organ że celu i warunki pobytu cudzoziemca w Polsce są niezgodne z deklarowanymi.
-Prawo przewiduje jednak sytuacje, gdy nawet w przypadku wystąpienia przesłanek deportacji w stosunku do cudzoziemca nie wydaje się decyzji zobowiązującej do powrotu.
-W decyzji o zobowiązaniu do powrotu organ może ustanowić okres zakazu ponownego wjazdu. W konsekwencji cudzoziemiec, który opuści Polskę na skutek takiej decyzji deportacyjnej, nie może od razu wrócić do Polski. Gdy w decyzji deportacyjnej nałożony został na cudzoziemca okres zakazu ponownego wjazdu do Polski, możliwe jest wystąpienie przez kancelarię o cofnięcie takiego zakazu i tym samym umożliwienie cudzoziemcom szybszego powrotu do Polski.
-Możliwe jest również uniknięcie w ogóle zakazu ponownego wjazdu.</t>
+          <t>Zarejestrowanie pojazdu używanego sprowadzonego z państwa, które nie należy do Unii Europejskiej Zarejestrowanie pojazdu używanego sprowadzonego z państwa, które nie należy do Unii Europejskiej Informacje zgodne ze stanem prawnym na dzień: 2024-09-06</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Gdzie mogę znaleźć darmową pomoc prawną w Dolnośląskiem?</t>
+          <t>Czy mogę prowadzić pojazd w Polskim na zagranicznym prawie jazdy?</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.kancelariakrs.pl/ile-kosztuje-porada-prawna-u-adwokata-prawnika-radcy-prawnego-notariusza/</t>
+          <t>http://bip.brpo.gov.pl/pl/content/rpo-polskie-prawo-jazdy-utrata-ue-kara-mc</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Strona główna » Blog » Ile kosztuje porada prawna u adwokata, prawnika, radcy prawnego, notariusza?
-Katarzyna Knapek
-Audyt prawny, Frankowicze, Pobyt cudzoziemców, Pomoc prawna dla firm, Prawo cywilne, Prawo dla branży budowlanej, Prawo gospodarcze, Prawo karne, Prawo nieruchomości, Prawo pracy, Prawo rodzinne, Prawo umów, Prawo w windykacji, Prawo w zamówieniach publicznych, RODO, Upadłość konsumencka, Znaki towarowe
-26 lutego, 2021
-Gdzie możliwe są darmowe porady prawne? Ile kosztuje pomoc prawna adwokata, radcy prawnego czy notariusza? Sprawdzamy cenniki usług prawniczych, wyjaśniamy, od czego zależy koszt porady prawnej w naszej i innych kancelariach adwokackich w Katowicach.</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
+          <t>Stracisz polskie prawo jazdy, a uzyskasz je gdzieś w UE? W Polsce będziesz ukarany za jego brak. Interwencja RPO Obywatel, który straci w Polsce prawo jazdy, a uzyska je w innym kraju Unii Europejskiej, w Polsce jest traktowany jako osoba kierująca pojazdem bez uprawnień, a za to grozi kara Ogranicza to także konstytucyjną swobodę poruszania się po terytorium Rzeczypospolitej Polskiej</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/prawo-jazdy-5285</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Informacje zgodne ze stanem prawnym na dzień: 2024-09-06 Każda osoba, która posiada prawo jazdy wydane za granicą, a mieszka w Polsce przynajmniej od 185 dni musi wymienić je na polskie prawo jazdy. Zagraniczne prawo jazdy przestaje być ważne po 6 miesiącach od momentu uzyskania stałego lub czasowego pobytu w Polsce. Dotyczy to także praw jazdy wydanych w Wielkiej Brytanii po dniu 31 grudnia 2020 r. Obowiązek wymiany prawa jazdy nie dotyczy jednak osób, które posiadają:</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.wroclaw.pl/dla-mieszkanca/pomoc-dla-cudzoziemcow-wroclaw</t>
+          <t>https://www.gov.pl/attachment/c7c9da8f-f437-4626-88a0-72e9d704a922</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Zgoda
-Szczegóły
-Ustawienia reklam
-O plikach cookies
-Gromadzić dane dotyczące Twojej lokalizacji geograficznej z dokładnością nawet do kilku metrów</t>
+          <t>Informacje zgodne ze stanem prawnym na dzień: 2024-09-06 Każda osoba, która posiada prawo jazdy wydane za granicą, a mieszka w Polsce przynajmniej od 185 dni musi wymienić je na polskie prawo jazdy. Zagraniczne prawo jazdy przestaje być ważne po 6 miesiącach od momentu uzyskania stałego lub czasowego pobytu w Polsce. Dotyczy to także praw jazdy wydanych w Wielkiej Brytanii po dniu 31 grudnia 2020 r. Obowiązek wymiany prawa jazdy nie dotyczy jednak osób, które posiadają:</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Co powinienem zrobić, jeśli zostanę aresztowany lub ukarany grzywną w Dolnośląskiem?</t>
+          <t>Jakie dokumenty są potrzebne do ubiegania się o kredyt lub hipotekę w Polskim?</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://gazetawroclawska.pl/tydzien-z-nowymi-mandatami-za-nami-na-dolnym-slasku-posypaly-sie-wysokie-kary/ar/c1-15987509</t>
+          <t>https://www.gov.pl/web/mieszkanie-dla-ciebie/program-pierwsze-mieszkanie</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>This website is using a security service to protect itself from online attacks. The action you just performed triggered the security solution. There are several actions that could trigger this block including submitting a certain word or phrase, a SQL command or malformed data.
-You can email the site owner to let them know you were blocked. Please include what you were doing when this page came up and the Cloudflare Ray ID found at the bottom of this page.
-Cloudflare Ray ID: 92f550bbbb4deec7
-•
-      Your IP:
-      Click to reveal
-83.27.101.111
-•
-Performance &amp; security by Cloudflare</t>
+          <t>10 powodów dla których warto wybrać Pierwsze Mieszkanie Jeśli jesteś gotów kupić pierwsze mieszkanie lub dom jednorodzinny – od 1 lipca 2023 r. możesz skorzystać z bezpiecznego kredytu 2%, czyli systemu dopłat do kredytu hipotecznego. Jeśli planujesz to w perspektywie następnych kilku lat – od tego samego momentu możesz oszczędzać na ich zakup na Koncie Mieszkaniowym. Przepisy, które umożliwiają ubieganie się o bezpieczny kredyt 2% i otworzenie Konta Mieszkaniowego, weszły w życie 1 lipca 2023 r.</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://tvn24.pl/wroclaw/172</t>
+          <t>https://www.gov.pl/web/mieszkanie-dla-ciebie/pytania-i-odpowiedzi</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>TVN24 na żywo
-TVN24 BiS na żywo
-TVN24 po ukraińsku
-TVN24NajnowszeŚwiatPolskaBiznesMeteoPremiumSportZdrowieTechnologiaKultura i stylCiekawostki
-FaktyZobacz FaktyFakty po FaktachFakty o ŚwiecieFakty po PołudniuLudzie Faktów</t>
+          <t>Odpowiedzi na poniższe pytania nie stanowią wykładni prawa w odniesieniu do indywidualnych przypadków, lecz ogólną interpretację przepisów ustawy z dnia 26 maja 2023 r. o pomocy państwa w oszczędzaniu na cele mieszkaniowe, zmieniającej ustawę z dnia z dnia 1 października 2021 r. o rodzinnym kredycie mieszkaniowym i bezpiecznym kredycie 2%. Ostateczna ocena spełnienia warunków programu „Pierwsze Mieszkanie” należy do banku biorącego udział w programie. W przypadku dokonania pozytywnej weryfikacji spełnienia kryteriów ustawowych to bank podejmie decyzję o możliwości udzielenia bezpiecznego kredytu 2% i założenia Konta Mieszkaniowego. Ministerstwo Rozwoju i Technologii nie bierze udziału w tym procesie. Stronami umowy o bezpieczny kredyt 2% lub prowadzenie Konta Mieszkaniowego są kredytobiorca/oszczędzający i bank udzielający kredytu lub prowadzący Konto. Ministerstwo Rozwoju i Technologii nie jest stroną takiej umowy, nie bierze udziału w procesie udzielenia kredytu lub otworzenia Konta. W związku z powyższym wszelkie pytania w sprawie zapisów umowy należy kierować do banku, z którym taka umowa została zawarta. Nie przewidziano ograniczenia ceny m2 lokalu mieszkalnego. Również w przypadku połączenia bezpiecznego kredytu 2% i gwarancji wkładu własnego kredytobiorcy.</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/PolicjaKG/?locale=gl_ES</t>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kredyt-hipoteczny-oraz-nadzor-nad-posrednikami-kredytu-18594631/roz-2</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>1m</t>
+          <t>Rozdział 2 - Obowiązki kredytodawcy, pośrednika kredytu hipotecznego i agenta przed zawarciem umowy o kredyt hipoteczny - Kredyt hipoteczny oraz nadzór nad pośrednikami kredytu hipotecznego i agentami. Obowiązki kredytodawcy, pośrednika kredytu hipotecznego i agenta przed zawarciem umowy o kredyt hipoteczny Kredytodawca, pośrednik kredytu hipotecznego oraz agent mogą przekazać konsumentowi przed zawarciem umowy o kredyt hipoteczny, na trwałym nośniku, dodatkowo inne dane niż określone w art. 11 ust. 1, łącznie z formularzem informacyjnym, o którym mowa w art. 11 ust. 2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Jak mogę uzyskać zezwolenie na pracę jako obywatel spoza UE w Polskim?</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/ou1611</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Wypełnij i wyślij elektroniczny wniosek na portalu praca.gov.pl. Podpiszesz go podpisem kwalifikowanym lub profilem zaufanym. Zezwolenie typu A lub B na pracę cudzoziemca na terytorium Polski Jesteś przedsiębiorcą, masz firmę w Polsce i chcesz zatrudnić cudzoziemca spoza UE, EOG lub Szwajcarii? Musisz najpierw uzyskać zezwolenie na wykonywanie przez niego pracy typu A lub B. Przeczytaj, czym różnią się te zezwolenia i jak je uzyskać.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00295</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Obywatele państw spoza Unii Europejskiej, Europejskiego Obszaru Gospodarczego lub Szwajcarii, mogą pracować w Polsce pod warunkiem, że: przedsiębiorca, który chce ich zatrudnić, uzyska dla nich odpowiednie zezwolenie na pracę albo cudzoziemiec posiada zezwolenie jednolite na pobyt czasowy i pracę.</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/004330</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Cudzoziemiec, który jest obywatelem państwa spoza Unii Europejskiej , Europejskiego Obszaru Gospodarczego lub Szwajcarii może legalnie pracować w Polsce, pod warunkiem że łącznie spełnia następujące warunki: legalnie przebywa na terytorium Polski, to znaczy posiada odpowiednie dokumenty pobytowe jeżeli nie jest zwolniony z obowiązku posiadania zezwolenia na pracę, to: uzyska zezwolenie na pobyt czasowy i pracę albo pracodawca uzyska dla niego zezwolenie na pracę, zezwolenie na pracę sezonową lub złoży oświadczenie o powierzeniu pracy cudzoziemcowi dokumenty pobytowe pozwalają mu na wykonywanie pracy jego praca odbywa się na warunkach oraz stanowisku, które zostały określone w zezwoleniu na pracę, oświadczeniu o powierzeniu pracy lub zezwoleniu na pobyt czasowy i pracę .</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Jak mogę zgłosić pracodawcę, który nie wypłaca mi wynagrodzenia w Polskim?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00199</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Przedmiotem skargi składanej do Państwowej Inspekcji Pracy może być naruszanie przepisów prawa pracy przez pracodawcę delegującego, w tym przepisów bezpieczeństwa i higieny pracy oraz przepisów dotyczących legalności zatrudnienia. W przypadku delegowania do 12 miesięcy pracownik delegowany do pracy w Polsce może złożyć skargę, jeżeli pracodawca nie zapewni mu warunków zatrudnienia dotyczących: norm i wymiaru czasu pracy oraz okresów odpoczynku dobowego i tygodniowego</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00197</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Pracownikom delegowanym do Polski przysługuje wynagrodzenie określone w ich umowach. Co do zasady za brak wypłaty wynagrodzenia pracownikowi delegowanemu na terytorium Polski odpowiedzialność ponosi pracodawca delegujący. Niewypłacenie pracownikowi delegowanemu wynagrodzenia za pracę stanowi wykroczenie przeciwko prawom osób wykonujących pracę zarobkową i jest zagrożone karą grzywny od 1000 zł do 30 000 zł.</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/finanse/stop-nielegalnemu-zatrudnieniu-i-placeniu-pod-stolem</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Stop nielegalnemu zatrudnieniu i płaceniu pod stołem Polski Ład to również działania mające ograniczyć pracę „na czarno” oraz wypłacanie wynagrodzeń „pod stołem”. Już od przyszłego roku, konsekwencje podatkowo-składkowe z tych tytułów ponosić będą nieuczciwi pracodawcy, a nie ich pracownicy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Jakie mam prawa jako najemca w Polskim?</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kodeks-cywilny-16785996/ks-3-tyt-17-dz-1</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Umowa najmu nieruchomości lub pomieszczenia na czas dłuższy niż rok powinna być zawarta na piśmie. W razie niezachowania tej formy poczytuje się umowę za zawartą na czas nieoznaczony. Jeżeli w czasie trwania najmu rzecz wymaga napraw, które obciążają wynajmującego, a bez których rzecz nie jest przydatna do umówionego użytku, najemca może wyznaczyć wynajmującemu odpowiedni termin do wykonania napraw. Po bezskutecznym upływie wyznaczonego terminu najemca może dokonać koniecznych napraw na koszt wynajmującego. Jeżeli osoba trzecia dochodzi przeciwko najemcy roszczeń dotyczących rzeczy najętej, najemca powinien niezwłocznie zawiadomić o tym wynajmującego.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>https://www.prawo.pl/biznes/najemca-obowiazany-jest-zwrocic-rzecz-w-stanie-niepogorszonym,151236.html</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Najemca ma usunąć uszkodzenia, kiedy wyprowadza się z mieszkania Najemca ma usunąć uszkodzenia, kiedy wyprowadza się z mieszkania Zgodnie z Kodeksem cywilnym najemca odpowiada za takie skutki używania lokalu, które przekraczają konsekwencje normalnego korzystania z niego. Z drugiej jednak strony przepisy prawa obligują najemcę np. do naprawy ścian i podłóg wynajmowanego lokalu. Słusznie wiele osób postrzega możliwość wynajmowania mieszkania jako dobry sposób na zabezpieczenie miesięcznego dochodu. Jednak nie zawsze relacje pomiędzy wynajmując a najemcą układają się bezproblemowo. Trudności pojawiają się zwłaszcza wówczas, gdy trzeba rozliczyć koszty napraw związanych z używaniem domu lub mieszkania. Trzeba pamiętać, że przepisy Kodeksu cywilnego nie zamykają zagadnienia, a niezbędne jest sięgnięcie po szczegółowe regulacje. Zgodnie z nimi większość drobnym remontów obciąża najemcę.</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kodeks-cywilny-16785996/art-673</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Art. 673. - - Kodeks cywilny. Jeżeli chcesz mieć dostęp do wszystkich dokumentów powiązanych, zaloguj się do LEX-a Nie korzystasz jeszcze z programów LEX? Zamów dostęp testowy » Jak wygląda sytuacja najemców lokali użytkowych w spółdzielniach mieszkaniowych w czasie koronawirusa?</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Jak uzyskać ubezpieczenie zdrowotne w Polsce?</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>http://pacjent.gov.pl/archiwum/2021/jak-ubezpieczyc-sie-dobrowolnie</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Jeśli mieszkasz w Polsce i nie obejmuje Cię powszechne ubezpieczenie zdrowotne ani nie masz prawa do świadczeń, możesz skorzystać z ubezpieczenia dobrowolnego Zgłoś się do oddziału wojewódzkiego NFZ właściwego ze względu na Twoje miejsce zamieszkania lub do jednej z delegatur tego oddziału. Wykaz aktualnych adresów oddziałów wojewódzkich znajdziesz na stronie NFZ. Wypełnij wniosek o objęcie dobrowolnym ubezpieczeniem zdrowotnym. Wniosek możesz wydrukować i wypełnić w domu lub na miejscu w oddziale. Wzór dokumentu znajdziesz na dole strony.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>https://www.nfz.gov.pl/dla-pacjenta/ubezpieczenia-w-nfz/</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Ubezpieczenie w NFZ eWUŚ Jak ubezpieczyć się dobrowolnie Pakiet onkologiczny otwiera się w nowej karcie Zaopatrzenie w wyroby medyczne Konstytucja gwarantuje Ci prawo do ochrony zdrowia, jednak nie zawsze możesz mieć prawo do bezpłatnych, czyli finansowanych ze środków publicznych, świadczeń opieki zdrowotnej. Ustawa z dnia 27 sierpnia 2004 r. o świadczeniach opieki zdrowotnej finansowanych ze środków publicznych ;</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>https://www.nfz.gov.pl/dla-pacjenta/ubezpieczenia-w-nfz/jak-sie-ubezpieczyc-dobrowolnie/</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Ubezpieczenie w NFZ eWUŚ Jak ubezpieczyć się dobrowolnie Pakiet onkologiczny otwiera się w nowej karcie Zaopatrzenie w wyroby medyczne Umowa zawarta z NFZ dobrowolnie uprawnia do: wszelkich świadczeń opieki zdrowotnej finansowanych ze środków publicznych na takich samych zasadach, jak w przypadku pozostałych ubezpieczonych w ramach publicznego systemu opieki zdrowotnej,</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Jak mogę zarejestrować firmę w Polskim?</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00120</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Sprawdź, czy możesz prowadzić działalność gospodarczą w Polsce Możesz prowadzić firmę jednoosobową samodzielnie, jeśli jesteś osobą pełnoletnią, bo tylko wtedy ponosisz pełną odpowiedzialność za swoje działania i masz pełną zdolność do podejmowania decyzji. Osoby niepełnoletnie, które chcą prowadzić własny biznes, w wielu sytuacjach będą musiały korzystać z pomocy swoich ustawowych przedstawicieli. Najczęściej będą to rodzice.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00119</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Polska Klasyfikacja Działalności to systematyka działalności gospodarczych stosowana w statystyce publicznej, ewidencji oraz rachunkowości. Od 1 stycznia 2025 roku obowiązuje nowa Polska Klasyfikacja Działalności - PKD 2025, która zastąpiła dotychczasową - PKD 2007. PKD 2025 została dostosowana do zmian dokonanych w klasyfikacji Unii Europejskiej , aktualnych realiów rynku, technologii i społecznych. Ujęto w niej rodzaje działalności, które pojawiły się w gospodarce w ostatnich latach, związane na przykład z gospodarką cyfrowa, gospodarką cyrkulacyjną czy bio-gospodarką. Doprecyzowano również opisy tradycyjnych branż.</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00172</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>W przepisach regulujących prowadzenie działalności gospodarczej występują różne definicje działalności gospodarczej. Prowadząc biznes należy brać pod uwagę czy konkretna aktywność stanowi działalność gospodarczą w rozumieniu właściwych przepisów. Dla celów podatku dochodowego działalnością gospodarczą jest zarobkowa działalność: polegająca na poszukiwaniu, rozpoznawaniu i wydobywaniu kopalin ze złóż</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Jak złożyć wniosek o kartę pobytu w Polsce?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/uw-podlaski/zasady-skladania-wnioskow-i-odbioru-kart-pobytu</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Założyć konto w Module Obsługi Spraw - mos.cudzoziemcy.gov.pl – wniosek o pobyt czasowy lub pobyt stały wypełnić elektronicznie, wydrukować z kodem kreskowym, własnoręcznie podpisać i wraz z wymaganymi dokumentami wysyłać do Urzędu za pośrednictwem operatora pocztowego lub złożyć - za pokwitowaniem – w Punkcie Obsługi Klienta Podlaskiego Urzędu Wojewódzkiego w Białymstoku przy ul. Mickiewicza 3 . Wnioski wypełnione elektroniczne w MOS będą bezpośrednio przekazywane do realizacji po wpływie do Urzędu, a cudzoziemiec otrzyma pisemne wezwanie do osobistego stawiennictwa celem pobrania odcisków palców w określonym dniu i godzinie. Priorytetowo obsługiwane będą również wnioski o udzielenie zezwolenia na pobyt rezydenta długoterminowego wypełnione w formie papierowej, wysyłane pocztą lub składane w Punkcie Obsługi Urzędu, z uwagi na brak usługi elektronicznego wypełnienia w MOS. Film instruktażowy na temat wypełniania wniosków o udzielenie zezwolenia na pobyt czasowy za pomocą formularza elektronicznego w MOS znajduje się pod adresem: https://www.youtube.com/watch?v=CQwDzLXejjo&amp;t=8s Wypełnić wniosek o pobyt czasowy lub pobyt stały w formie tradycyjnej i wraz z wymaganymi dokumentami wysyłać do Urzędu za pośrednictwem operatora pocztowego lub złożyć - za pokwitowaniem w Punkcie Obsługi Klienta w siedzibie Urzędu. Wnioski wypełnione tradycyjnie, poza MOS, będą przekazywane do realizacji nie wcześniej niż po upływie 6 miesięcy od dnia ich wpływu do Urzędu. Po tym terminie cudzoziemiec otrzyma pisemne wezwanie do osobistego stawiennictwa celem pobrania odcisków palców w określonym dniu i godzinie. Złożenie wniosków o wymianę karty pobytu, wydanie polskiego dokumentu podróży dla cudzoziemca, odbiór karty pobytu oraz polskiego dokumentu podróży dla cudzoziemca odbywa się bez pobierania biletu z biletomatu: na Sali Obsługi Cudzoziemców – stanowisko nr 5 poniedziałek 7:15 – 17:45 wtorek, czwartek, piątek 8:00 – 15:00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00210</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Procedura uzyskania zezwolenia na pobyt czasowy i pracę, czyli zezwolenie jednolite jest korzystna, bo wszystkie formalności legalizujące pobyt i zatrudnienie cudzoziemca odbywają się w ramach jednego postępowania administracyjnego - cudzoziemiec nie musi odrębnie ubiegać się o zezwolenie na pobyt , a pracodawca - o zezwolenie na pracę. Wojewoda, który udzielił jednolitego zezwolenia na pobyt czasowy i pracę na terytorium Polski, wydaje cudzoziemcowi z urzędu kartę pobytu. Karta pobytu, w okresie w którym jest ważna, potwierdza tożsamość cudzoziemca oraz uprawnia go, wraz z dokumentem podróży, do wielokrotnego przekraczania granicy bez konieczności uzyskania wizy.</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00210#2</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Procedura uzyskania zezwolenia na pobyt czasowy i pracę, czyli zezwolenie jednolite jest korzystna, bo wszystkie formalności legalizujące pobyt i zatrudnienie cudzoziemca odbywają się w ramach jednego postępowania administracyjnego - cudzoziemiec nie musi odrębnie ubiegać się o zezwolenie na pobyt , a pracodawca - o zezwolenie na pracę. Wojewoda, który udzielił jednolitego zezwolenia na pobyt czasowy i pracę na terytorium Polski, wydaje cudzoziemcowi z urzędu kartę pobytu. Karta pobytu, w okresie w którym jest ważna, potwierdza tożsamość cudzoziemca oraz uprawnia go, wraz z dokumentem podróży, do wielokrotnego przekraczania granicy bez konieczności uzyskania wizy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Jak uzyskać prawo jazdy w Polsce?</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/uzyskaj-prawo-jazdy</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Chcesz uzyskać prawo jazdy? Masz prawo jazdy i chcesz mieć kolejną kategorię? Sprawdź, jak to zrobić. Rozwiń tekst Kto może uzyskać Prawo jazdy może uzyskać każdy, kto mieszka w Polsce przynajmniej od 185 dni i: po raz pierwszy chce dostać prawo jazdy – jeśli jest w odpowiednim wieku, ma już prawo jazdy i chce uzyskać kolejną kategorię – jeśli jest w odpowiednim wieku. Sprawdź, jaki jest minimalny wymagany wiek dla poszczególnych kategorii prawa jazdy. Wniosek możesz złożyć przez pełnomocnika. Dowiedz się w urzędzie, jak to zrobić. Prawo jazdy może uzyskać każdy, kto mieszka w Polsce przynajmniej od 185 dni i:</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/infrastruktura/jak-uzyskac-prawo-jazdy-</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Chcesz uzyskać prawo jazdy? A może już je masz i chcesz uzyskać pozwolenie na kolejną kategorię? Dowiedz się, jak wygląda cały proces - od złożenia wniosku, przez kurs i egzamin, po odbiór dokumentu. Jeśli chcesz złożyć wniosek o prawo jazdy przez Internet, kliknij na link "Przez Internet". każdy obywatel Polski, który po raz pierwszy chce dostać prawo jazdy - jeśli jest w wieku wymaganym dla danej kategorii. Sprawdź, jaki jest minimalny wymagany wiek dla poszczególnych kategorii prawa jazdy, każdy pełnoletni obywatel Polski, który ma już prawo jazdy i chce uzyskać pozwolenie na inną kategorię ,</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/kategorie-prawa-jazdy</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Chcesz uzyskać prawo jazdy? Sprawdź, jakie pojazdy możesz prowadzić w poszczególnych kategoriach oraz w jakim musisz być wieku, żeby móc zdać egzamin, by je prowadzić. Rozwiń tekst Kategorie prawa jazdy Nazwa kategorii Jakimi pojazdami możesz kierować Ile musisz mieć lat, żeby uzyskać prawo jazdy AM motorower czterokołowiec lekki zespół pojazdów – powyższe pojazdy połączone z przyczepą – tylko w Polsce 14 lat A1 motocykl o pojemności skokowej silnika do 125 cm3, mocy do 11 kW i stosunku mocy do masy własnej do 0,1 kW/kg motocykl trójkołowy o mocy do 15 kW pojazdy z kategorii AM zespół pojazdów – powyższe pojazdy połączone z przyczepą - tylko w Polsce 16 lat A2 motocykl, który spełnia wszystkie poniższe warunki: moc do 35 kW stosunek mocy do masy własnej do 0,2 kW/kg nie może on powstać w wyniku wprowadzenia zmian w pojeździe, którego moc przekracza dwukrotność mocy tego motocykla motocykl trójkołowy o mocy do 15 kW pojazdy z kategorii AM zespół pojazdów – powyższe pojazdy połączone z przyczepą – tylko w Polsce 18 lat A każdy motocykl pojazd z kategorii AM zespół pojazdów – powyższe pojazdy połączone z przyczepą – tylko w Polsce 20 lat - jeśli masz już od co najmniej 2 lat prawo jazdy kategorii A2 24 lata - jeśli nie maszod co najmniej 2 lat prawa jazdy kategorii A2 B1 czterokołowiec pojazd z kategorii AM 16 lat B pojazd samochodowy o dopuszczalnej masie całkowitej do 3,5 t , z wyjątkiem autobusu i motocykla zespół pojazdów – powyższy pojazd połączony z lekką przyczepą pojazd z kategorii AM zespół pojazdów – złożony z pojazdu samochodowego o dopuszczalnej masie całkowitej do 3,5 t oraz przyczepy. Jednak łączna dopuszczalna masa całkowita całego zespołu nie może przekroczyć 3500 kg, jeśli zdasz dodatkowy egzamin praktyczny i masz dodatkowy wpis w prawie jazdy – zespół pojazdów złożony z pojazdu samochodowego o dopuszczalnej masie całkowitej do 3,5 t oraz przyczepy. Jednak łączna dopuszczalna masa całkowita całego zespołu nie może przekroczyć 4250 kg ciągnik rolniczy – tylko w Polsce pojazd wolnobieżny – tylko w Polsce zespół pojazdów złożony z ciągnika rolniczego oraz lekkiej przyczepy – tylko w Polsce zespół pojazdów złożony z pojazdu wolnobieżnego oraz lekkiej przyczepy – tylko w Polsce jeśli masz prawo jazdy kategorii B od co najmniej 3 lat - motocykl o pojemności skokowej silnika do 125 cm3, mocy do 11 kW i stosunku mocy do masy własnej do 0,1 kW/kg – tylko w Polsce 18 lat B+E zespół pojazdów złożony z pojazdu z kategorii B i przyczepy o dopuszczalnej masie całkowitej do 3,5 tony zespół pojazdów złożony z ciągnika rolniczego i przyczepy lub przyczep – tylko w Polsce zespół pojazdów złożony z pojazdu wolnobieżnego i przyczepy lub przyczep – tylko w Polsce 18 lat C pojazd samochodowy o dopuszczalnej masie całkowitej ponad 3,5 t, z wyjątkiem autobus zespół pojazdów – powyższy pojazd i lekka przyczepa pojazd z kategorii AM ciągnik rolniczy – tylko w Polsce pojazd wolnobieżny – tylko w Polsce zespół pojazdów złożony z ciągnika rolniczego oraz lekkiej przyczepy – tylko w Polsce zespół pojazdów złożony z pojazdu wolnobieżnego oraz lekkiej przyczepy – tylko w Polsce 21 lat C1 pojazd samochodowy o dopuszczalnej masie całkowitej ponad 3,5 t do 7,5 t, z wyjątkiem autobus zespół pojazdów – powyższy pojazd i lekka przyczepa pojazd z kategorii AM ciągnik rolniczy – tylko w Polsce, pojazd wolnobieżny – tylko w Polsce zespół pojazdów złożony z ciągnika rolniczego oraz lekkiej przyczepy – tylko w Polsce zespół pojazdów złożony z pojazdu wolnobieżnego oraz lekkiej przyczepy – tylko w Polsce 18 lat C1+E zespół pojazdów o dopuszczalnej masie całkowitej do 12 ton, który składa się z: pojazdu, który ciągnie – pojazdy z kategorii C1 przyczepy zespół pojazdów złożony z ciągnika rolniczego oraz przyczepy lub przyczep – tylko w Polsce zespół pojazdów złożony z pojazdu wolnobieżnego oraz przyczepy lub przyczep – tylko w Polsce 18 lat C+E zespół pojazdów złożony z pojazdu z kategorii C i przyczepy, zespół pojazdów złożony z ciągnika rolniczego oraz przyczepy lub przyczep – tylko w Polsce zespół pojazdów złożony z pojazdu wolnobieżnego oraz przyczepy lub przyczep – tylko w Polsce 21 lat D autobus zespół pojazdów złożony z autobusu oraz z lekkiej przyczepy pojazd z kategorii AM ciągnik rolniczy – tylko w Polsce pojazd wolnobieżny – tylko w Polsce zespół pojazdów złożony z ciągnika rolniczego oraz lekkiej przyczepy – tylko w Polsce zespół pojazdów złożony z pojazdu wolnobieżnego oraz lekkiej przyczepy – tylko w Polsce 24 lata D1 autobus przeznaczony konstrukcyjnie do przewozu do 17 osób łącznie z kierowcą, o długości do 8 m zespół pojazdów złożony z pojazdu, o którym mowa powyżej, oraz z lekkiej przyczepy pojazd z kategorii AM ciągnik rolniczy – tylko w Polsce pojazd wolnobieżny – tylko w Polsce zespół pojazdów złożony z ciągnika rolniczego oraz lekkiej przyczepy – tylko w Polsce zespół pojazdów złożony z pojazdu wolnobieżnego oraz lekkiej przyczepy – tylko w Polsce 21 lat D1+E zespół pojazdów złożony z pojazdu kategorii D1 i przyczepy zespół pojazdów złożony z ciągnika rolniczego oraz przyczepy lub przyczep – tylko w Polsce zespół pojazdów złożony z pojazdu wolnobieżnego oraz przyczepy lub przyczep – tylko w Polsce 21 lat D+E zespół pojazdów złożony z pojazdu z kategorii D i przyczepy zespół pojazdów złożony z ciągnika rolniczego oraz przyczepy lub przyczep – tylko w Polsce zespół pojazdów złożony z pojazdu wolnobieżnego oraz przyczepy lub przyczep – tylko w Polsce 24 lata T ciągnik rolniczy pojazd wolnobieżny zespół pojazdów złożony z ciągnika rolniczego i przyczepy lub przyczep zespół pojazdów złożony z pojazdu wolnobieżnego i przyczepy lub przyczep pojazd z kategorii AM 16 lat Tramwaj tramwaj 21 lat Możesz rozpocząć kurs i zdać egzamin na prawo jazdy dla określonej kategorii jeszcze zanim ukończysz wskazany powyżej wiek – jednak nie wcześniej niż 3 miesiące przed jego ukończeniem. Dlatego wniosek o prawo jazdy złóż nie wcześniej niż 3 miesiące przed ukończeniem tego wieku. Informacje, które znajdują się w tej karcie nie dotyczą prowadzenia pojazdów Sił Zbrojnych RP, Państwowej Straży Pożarnej, Policji, Służby Granicznej. zespół pojazdów – powyższe pojazdy połączone z przyczepą – tylko w Polsce</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Czy istnieją ograniczenia prawne dotyczące wynajmu mieszkania przez cudzoziemca w Polskim?</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/attachment/727a25ae-43bf-461a-8d45-c35e444e5c64</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Druk nr 950 - o zmianie ustawy o cudzoziemcach oraz ... o zmianie ustawy o udzielaniu cudzoziemcom ochrony na ...</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/ou209</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Uzyskaj zezwolenie na nabycie nieruchomości przez cudzoziemca Jesteś cudzoziemcem spoza Unii Europejskiej, Szwajcarii, Norwegii, Islandii i Lichtensteinu i zamierzasz nabyć w Polsce nieruchomość? Musisz uzyskać zezwolenie ministra. Sprawdź, jak to zrobić. Co powinieneś wiedzieć i kto może skorzystać z usługi</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>https://www.malopolska.uw.gov.pl/doc/pouczenie_dla_cudzoziemcow.doc</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Uzyskaj zezwolenie na nabycie nieruchomości przez cudzoziemca Jesteś cudzoziemcem spoza Unii Europejskiej, Szwajcarii, Norwegii, Islandii i Lichtensteinu i zamierzasz nabyć w Polsce nieruchomość? Musisz uzyskać zezwolenie ministra. Sprawdź, jak to zrobić. Co powinieneś wiedzieć i kto może skorzystać z usługi</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Jak mogę zgłosić przestępstwo jako cudzoziemiec w Polskim?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://bip.brpo.gov.pl/pl/content/rpo-cudzoziemcy-przestepstwa-zawiadomienia-kgp-odpowiedz</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Sprawa składania przez cudzoziemców nieznających jęz. polskiego ustnych zawiadomień o przestępstwie. Odpowiedź KGP Zastępca RPO Stanisław Trociuk zwrócił się do Komendanta Głównego Policji insp. Marka Boronia w sprawie zapewnienia pomocy tłumacza cudzoziemcom, którzy zgłaszają przestępstwo na swoją szkodę Obowiązek wezwania tłumacza zachodzi, gdy przesłuchiwana osoba językiem polskim nie włada, nawet, jeżeli przesłuchujący policjant zna język obcy, którym ona się posługuje. Co istotne, osoby przesłuchiwane nie ponoszą kosztów udziału tłumacza - wyjaśnia KGP</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>https://lublin.policja.gov.pl/llu/prewencja/dla-cudzoziemcow/64544,Jak-zlozyc-zawiadomienie-o-popelnionym-przestepstwie.html</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Jak złożyć zawiadomienie o popełnionym przestępstwie Jeśli zostałeś pokrzywdzony przestępstwem - , lub byłeś bezpośrednim świadkiem takiego zdarzenia ZŁÓŻ ZAWIADOMIENIE O POPEŁNIENIU PRZESTĘPSTWA W tym celu najlepiej udaj się do najbliższego komisariatu Policji lub jednostki prokuratury. Zawiadomienie możesz złożyć ustnie lub pisemnie. Ustne złożenie zawiadomienia polega na opowiedzeniu policjantowi/prokuratorowi o całym wydarzeniu. Po złożeniu ustnego zawiadomienia możesz zostać od razu przesłuchany w charakterze świadka. Zarówno zawiadomienie, jak i przesłuchanie zostaną zapisane w protokole, który wypełni policjant/prokurator. Na koniec protokół musi zostać podpisany przez Ciebie. Jeżeli pragniesz złożyć zawiadomienie pisemnie, pismo zawierające informacje, jakie chciałbyś przekazać organom ścigania, zostaw na komisariacie Policji lub w prokuraturze albo wyślij je drogą listowną .</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>https://ksp.policja.gov.pl/download/168/25021/Jakpowinienpostepowapolicjantwykonujacyczynnoscizudzialemcudzoziemca.pdf</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Jak złożyć zawiadomienie o popełnionym przestępstwie Jeśli zostałeś pokrzywdzony przestępstwem - , lub byłeś bezpośrednim świadkiem takiego zdarzenia ZŁÓŻ ZAWIADOMIENIE O POPEŁNIENIU PRZESTĘPSTWA W tym celu najlepiej udaj się do najbliższego komisariatu Policji lub jednostki prokuratury. Zawiadomienie możesz złożyć ustnie lub pisemnie. Ustne złożenie zawiadomienia polega na opowiedzeniu policjantowi/prokuratorowi o całym wydarzeniu. Po złożeniu ustnego zawiadomienia możesz zostać od razu przesłuchany w charakterze świadka. Zarówno zawiadomienie, jak i przesłuchanie zostaną zapisane w protokole, który wypełni policjant/prokurator. Na koniec protokół musi zostać podpisany przez Ciebie. Jeżeli pragniesz złożyć zawiadomienie pisemnie, pismo zawierające informacje, jakie chciałbyś przekazać organom ścigania, zostaw na komisariacie Policji lub w prokuraturze albo wyślij je drogą listowną .</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Jak zapisać dziecko do szkoły w Polsce?</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://www.prawo.pl/oswiata/jak-zapisac-dziecko-do-szkoly-jakie-dokumenty-potrzebne-czym-jest-rejonizacja-szkol-podstawowych,374408.html</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Kryteria naboru do szkół podstawowych - decyduje ustawa i przepisy samorządowe Kryteria naboru do szkół podstawowych - decyduje ustawa i przepisy samorządowe Podstawę prawną rekrutacji do szkół podstawowych stanowią przepisy ustawy Prawo oświatowe oraz przepisy rozporządzenia Ministra Edukacji Narodowej w sprawie przeprowadzania postępowania rekrutacyjnego oraz postępowania uzupełniającego do publicznych przedszkoli, szkół, placówek i centrów.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/-/wracamy-do-polskiej-szkoly</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Świadectwa, zaświadczenia, certyfikaty, czyli jakie dokumenty będą potrzebne Powrót z emigracji jest na pewno wyzwaniem logistycznym. Formalności, dokumenty, pakowanie zgromadzonego dobytku, a jeszcze świadomość wszystkich formalności czekających na was po powrocie. Pośród wszystkich tych kwestii są jeszcze dzieci – ich przygotowanie: mentalne, ale też sprawy praktyczne, takie jak edukacja. Pojawia się też pytanie: jakie dokumenty dziecka będą wymagane w polskiej szkole? Dokumenty standardowo wymagane ze szkoły lokalnej to świadectwa, jeśli w systemie szkolnym danego państwa są one wydawane albo zaświadczenie wystawione przez dyrekcję szkoły, w której dziecko uczyło się. Dodatkowo, jeśli dziecko uczęszczało również do szkoły polskiej, tzw. sobotniej – potrzebne będą świadectwa z kolejno ukończonych klas. Wszystkie te dokumenty, dotyczące edukacji dziecka za granicą, pozwolą potwierdzić spełnienie obowiązku szkolnego oraz będą informacją na temat uzyskanych przez dziecko ocen. Na podstawie wspomnianych dokumentów dyrektor szkoły będzie mógł zadecydować, do której klasy dziecko powinno zostać przyjęte.</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/na-jakich-warunkach-moje-dzieci-moga-zostac-przyjete-do-polskiej-szkoly-12138</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Na jakich warunkach moje dzieci mogą zostać przyjęte do polskiej szkoły? Wracamy z dziećmi z Islandii po 3 latach pobytu. Czy będziemy mieć problemy z zapisaniem ich do szkoły po rozpoczęciu roku szkolnego? Bardzo słabo mówią po polsku i boimy się, że trafią do klas z dużo młodszymi dziećmi. Każdego ucznia przybywającego/powracającego z zagranicy przyjmuje się do szkoły w Polsce na podstawie:</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Jakie są warunki otrzymania obywatelstwa polskiego?</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/nabycie-obywatelstwa-polskiego-10000</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Informacje zgodne ze stanem prawnym na dzień: 2024-09-11 Zagadnienia nabycia obywatelstwa polskiego i jego utraty reguluje ustawa z 2 kwietnia 2009 r. o obywatelstwie polskim. 1. Urodzenie z rodziców, z których co najmniej jedno ma obywatelstwo polskie – zasada krwi/Ius Sanguinis</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>https://archiwum.mswia.gov.pl/pl/bezpieczenstwo/obywatelstwo-i-repatri/cudzoziemcy/10169,SPOSOBY-NABYCIA-OBYWATELSTWA-POLSKIEGO.html</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Zagadnienia nabycia obywatelstwa polskiego i jego utraty reguluje ustawa z dnia 2 kwietnia 2009 roku o obywatelstwie polskim . Ustawa zawiera dwie podstawowe zasady dotyczące obywatelstwa polskiego. Wyrażona w art. 2 ustawy zasada ciągłości obywatelstwa polskiego gwarantuje trwałość obywatelstwa w czasie, począwszy od momentu jego nabycia, zgodnie z obowiązującymi w tym czasie przepisami, niezależnie od zmian, jakim podlega ustawodawstwo dotyczące obywatelstwa. Oznacza to, iż osoby, które nabyły obywatelstwo polskie na podstawie dawnych przepisów, następnie uchylonych lub zmienionych, jeśli obywatelstwa polskiego nie utraciły, zachowują je zgodnie z przepisami obowiązującymi w dacie jego nabycia. Zasada ta jest równocześnie dyrektywą dla właściwych organów administracji publicznej w postępowaniu o potwierdzenie posiadania lub utraty obywatelstwa polskiego. Natomiast wprowadzona przepisem art. 3 ustawy, zasada wyłączności obywatelstwa polskiego wiąże się ściśle z problemem podwójnego obywatelstwa, tworzy bowiem jasną dyrektywę kolizyjną w przypadku jego zaistnienia i pozwala na usuwanie jego niekorzystnych skutków. Projekt ustawy przyjmuje zasadę dopuszczalności wielości obywatelstw przy utrzymaniu bezwzględnego priorytetu obywatelstwa polskiego. Obywatel polski może posiadać równocześnie obywatelstwo polskie i obywatelstwo państwa obcego, ale nawet wówczas posiada wobec Rzeczypospolitej Polskiej takie same prawa i obowiązki, jak osoba posiadająca wyłącznie obywatelstwo polskie, tj. nie może wobec władz polskich powoływać się ze skutkiem prawnym na posiadane równocześnie obywatelstwo obce lub na wynikające z niego prawa i obowiązki. Urodzenie z rodziców, z których co najmniej jedno posiada obywatelstwo polskie – Zasada krwi/Ius Sanguinis</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/mswia/uzyskaj-polskie-obywatelstwo</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Potwierdzenie posiadania lub utraty obywatelstwa polskiego Chcesz dostać polskie obywatelstwo? Utraciłeś polskie obywatelstwo i chcesz je odzyskać? Potrzebujesz urzędowego potwierdzenia, że masz polskie obywatelstwo? Tutaj znajdziesz wszystkie potrzebne informacje. Złóż wniosek do Prezydenta o nadanie polskiego obywatelstwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Czy potrzebuję zezwolenia na pracę w Polskim?</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/uw-lodzki/kiedy-cudzoziemiec-nie-potrzebuje-zezwolenia-na-prace</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Kiedy cudzoziemiec nie potrzebuje zezwolenia na pracę? Cudzoziemiec może pracować na terytorium Polski, jeżeli: posiada status uchodźcy nadany w Rzeczypospolitej Polskiej;</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/ou1611</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Wypełnij i wyślij elektroniczny wniosek na portalu praca.gov.pl. Podpiszesz go podpisem kwalifikowanym lub profilem zaufanym. Zezwolenie typu A lub B na pracę cudzoziemca na terytorium Polski Jesteś przedsiębiorcą, masz firmę w Polsce i chcesz zatrudnić cudzoziemca spoza UE, EOG lub Szwajcarii? Musisz najpierw uzyskać zezwolenie na wykonywanie przez niego pracy typu A lub B. Przeczytaj, czym różnią się te zezwolenia i jak je uzyskać.</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://zielonalinia.gov.pl/-/cudzoziemcy-zwolnieni-z-obowiazku-posiadania-zezwolenia-na-prace-cz-1-</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Gdy szukamy przepisów, określających cudzoziemców, którzy są uprawnieni do wykonywania pracy na terytorium Polski bez konieczności posiadania zezwolenia na pracę sięgamy do ustawy z dnia 20 kwietnia 2004 r. o promocji zatrudnienia i instytucjach rynku pracy oraz do rozporządzenia Ministra Pracy i Polityki Społecznej z dnia 21 kwietnia 2015 r. w sprawie przypadków, w których powierzenie wykonywania pracy cudzoziemcowi na terytorium Rzeczypospolitej Polskiej jest dopuszczalne bez konieczności uzyskania zezwolenia na pracę. Dodatkowo przydatna jest także ustawa z dnia 12 grudnia 2013 r. o cudzoziemcach. W pierwszej części tego artykułu przedstawimy przypadki opisane w ustawie o promocji zatrudnienia i instytucjach rynku pracy. Zgodnie z art. 87 ust. 1 ustawy o promocji zatrudnienia i instytucjach rynku pracy cudzoziemiec jest uprawniony do wykonywania pracy na terytorium Polski, m.in. jeżeli: 1) posiada status uchodźcy nadany w Rzeczypospolitej Polskiej;</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Jakie są zasady łączenia rodzin w Polsce?</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/attachment/59d481b9-ee0d-449a-b03f-9f0b8f114669</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Zezwolenie na pobyt czasowy w celu połączenia się z ... Zezwolenie na pobyt czasowy w celu połączenia się z ... Połączenie z rodziną - Podlaski Urząd Wojewódzki w ...</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>https://www.mos.cudzoziemcy.gov.pl/informacje/zwiazek-mal</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Zezwolenie na pobyt czasowy w celu połączenia się z rodziną - związek małżeński uznawany przez prawo RP Wybierz interesujące Cię zagadnienie lub poznaj pełną informację o zezwoleniu Przepisy migracyjne zapewniają możliwość wykonywania prawa do łączenia rodzin określonym członkom rodziny rozdzielonej, będącym obywatelami państw trzecich lub będącym bezpaństwowcami, w tym także:</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://mos.cudzoziemcy.gov.pl/informacje/maloletni-benef/wymogi</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Zezwolenie na pobyt czasowy w celu połączenia się z rodziną - rodzic lub opiekun małoletniego beneficjenta ochrony międzynarodowej pozostającego bez opieki Wybierz interesujące Cię zagadnienie lub poznaj pełną informację o zezwoleniu Aby cudzoziemiec mógł uzyskać zezwolenie na pobyt czasowy w celu połączenia się z rodziną konieczne jest spełnienie przez niego w sposób łączny następujących wymogów:</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Jak wynająć mieszkanie w Polsce legalnie?</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://www.prawo.pl/student/jak-bezpiecznie-wynajac-mieszkanie-bedac-studentem,520206.html</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Zasady najmu mieszkania reguluje kodeks cywilny oraz ustawa o ochronie praw lokatorów, mieszkaniowym zasobie gminy i o zmianie Kodeksu cywilnego . Zgodnie z art. 659 k.c. przez umowę najmu wynajmujący zobowiązuje się oddać najemcy rzecz do używania przez czas oznaczony lub nieoznaczony, a najemca zobowiązuje się płacić wynajmującemu umówiony czynsz. Czynsz może być oznaczony w pieniądzach lub w świadczeniach innego rodzaju. Umowa najmu nieruchomości lub pomieszczenia na czas dłuższy niż rok powinna być zawarta na piśmie. W razie niezachowania tej formy poczytuje się umowę za zawartą na czas nieoznaczony . Wskazanie w zawieranej umowie terminu ma ogromne znaczenie w kontekście ustalenia okresu wypowiedzenia. W tym przypadku, zgodnie z art. 673 k.c., który zawiera terminy wypowiedzenia najmu przyjmuje się, że jeżeli czas trwania najmu nie jest oznaczony, zarówno wynajmujący, jak i najemca mogą wypowiedzieć najem z zachowaniem terminów umownych, a w ich braku z zachowaniem terminów ustawowych.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kodeks-cywilny-16785996/ks-3-tyt-17-dz-1</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Umowa najmu nieruchomości lub pomieszczenia na czas dłuższy niż rok powinna być zawarta na piśmie. W razie niezachowania tej formy poczytuje się umowę za zawartą na czas nieoznaczony. Jeżeli w czasie trwania najmu rzecz wymaga napraw, które obciążają wynajmującego, a bez których rzecz nie jest przydatna do umówionego użytku, najemca może wyznaczyć wynajmującemu odpowiedni termin do wykonania napraw. Po bezskutecznym upływie wyznaczonego terminu najemca może dokonać koniecznych napraw na koszt wynajmującego. Jeżeli osoba trzecia dochodzi przeciwko najemcy roszczeń dotyczących rzeczy najętej, najemca powinien niezwłocznie zawiadomić o tym wynajmującego.</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/rozwoj-technologia/spoleczne-agencje-najmu3</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Społeczna agencja najmu to podmiot współpracujący z gminą, który pośredniczy między właścicielami mieszkań na wynajem i osobami, którym dochody lub sytuacja życiowa utrudniają najem mieszkania w warunkach rynkowych. zwiększenie oferty mieszkaniowej dla osób o średnich i niższych dochodach, rozszerzenie narzędzi dostępnych gminom w ramach realizacji lokalnej polityki mieszkaniowej o formułę, która może stanowić alternatywę dla budownictwa komunalnego,</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Co powinienem zrobić, jeśli zostanę aresztowany lub ukarany grzywną w Polskim?</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://mazowiecka.policja.gov.pl/wsi/aktualnosci/78630,Areszt-za-niezaplacona-grzywne-Jak-i-kiedy.html</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Nie przyjąłeś mandatu karnego lub nie zapłaciłeś grzywny i myślisz, że przejdzie ci to płazem? Nic bardziej mylnego. Niezapłacona grzywna skutkuje zamianą na karę aresztu od kilku dni do nawet 6 miesięcy w tej samej sprawie. Jak się przed tym uchronić? Ile dni aresztu za jaką kwotę grzywny? Tego dowiesz się poniżej. W przypadku odmowy przyjęcia mandatu karnego, Policja kieruje wniosek o ukaranie do Sądu Rejonowego. Sąd orzeka czy dana osoba jest winna lub niewinna. W przypadku stwierdzonej winy w sprawach mniejszej wagi orzekana jest grzywna, orzekając jednocześnie - na wypadek niezapłacenia - zamianę grzywny na areszt, licząc jeden dzień aresztu od 50zł do 1.500zł grzywny. Ogólny czas trwania aresztu nie może w tej samej sprawie przekroczyć 6 miesięcy. Taki wyrok jest przesyłany do osoby skazanej. Jest w nim zapis o wysokości grzywny, numerze konta oraz terminie zapłaty po uprawomocnieniu się wyroku. Jeżeli osoba bagatelizuje otrzymane pismo i nie płaci kary grzywny, sprawa ponownie wraca do sądu, gdzie kara pieniężna jest zamieniana na karę aresztu. Zamieniając grzywnę na zastępczą karę pozbawienia wolności sąd przyjmuje, że jeden dzień pozbawienia wolności równa się dwie stawki dzienne grzywny. Jeśli zatem do zapłacenia jest 100 stawek dziennych grzywny po 20 zł każda, to sąd wymierzy 50 dni kary zastępczej. Jeżeli osoba nie stawia się w areszcie i w dalszym ciągu nie płaci orzeczonej grzywny wówczas sąd wydaje Polecenie zatrzymania i doprowadzenia wraz z zarządzeniem o wszczęciu poszukiwań ogólnokrajowych i przesyła je do Policji. Zgodnie z ustawą o Policji wykonujemy polecenia sądu i prokuratury. Mundurowi mają miesiąc czasu na zatrzymanie i doprowadzenie takiej osoby do aresztu, w innym przypadku sąd może wydać za taką osobą list gończy, który można opublikować na stronach internetowych, w prasie i mediach.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/procedury/ukaranie-kara-porzadkowa-grzywny-lub-pozbawienia-wolnosci-za-naruszenie-powagi-sadu-1610615575</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Stefański Ryszard A., Ukaranie karą porządkową grzywny lub pozbawienia wolności za naruszenie powagi sądu Ukaranie karą porządkową grzywny lub pozbawienia wolności za naruszenie powagi sądu Ukaranie karą porządkową grzywny lub pozbawienia wolności za naruszenie powagi sądu</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kodeks-karny-wykonawczy-16798687/CZ-.sz</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Część szczególna - Grzywna - Kodeks karny wykonawczy. W posiedzeniu w przedmiocie zarządzenia wykonania zastępczej kary pozbawienia wolności ma prawo wziąć udział prokurator, skazany oraz jego obrońca, a gdy skazany pozostaje pod dozorem - również sądowy kurator zawodowy, osoba godna zaufania lub przedstawiciel stowarzyszenia, instytucji albo organizacji społecznej, o której mowa w art. 73 § 1 Kodeksu karnego. Udzielając skazanemu warunkowego przedterminowego zwolnienia z odbycia reszty kary pozbawienia wolności, sąd penitencjarny może, jeżeli istnieją podstawy do przyjęcia, że skazany uiści grzywnę dobrowolnie, wstrzymać uprzednio zarządzone wykonanie zastępczej kary pozbawienia wolności, stosując jednocześnie art. 49; wówczas okres rozłożenia grzywny na raty biegnie od dnia wydania postanowienia o warunkowym przedterminowym zwolnieniu.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Jak mogę wymienić moje prawo jazdy na polskie w Polskim?</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/wymien-zagraniczne-prawo-jazdy-na-polskie</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Kraje członkowiskie Unii Europejskiej: Austria / Austria Belgia / Belgium Bułgaria / Bulgaria Chorwacja / Croatia Cypr / Cyprus Czechy / Czechia Dania / Denmark Estonia / Estonia Finlandia / Finland Francja / France Grecja / Greece Hiszpania / Spain Holandia / Netherlands Irlandia / Ireland Litwa / Lithuania Luksemburg / Luxembourg Łotwa / Latvia Malta / Malta Niemcy / Germany Portugalia / Portugal Rumunia / Romania Słowacja / Slovakia Słowenia / Slovenia Szwecja / Sweden Węgry /Hungary Włochy / Italy Masz zagraniczne prawo jazdy i mieszkasz w Polsce już od minimum 185 dni? Wymień je na polskie prawo jazdy. Sprawdź, jak to zrobić. Jeśli masz ważne prawo jazdy z kraju Unii Europejskiej – nie musisz wymieniać go na polskie prawo jazdy. Prawo jazdy z kraju UE jest ważne w Polsce.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/prawo-jazdy-5285</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Informacje zgodne ze stanem prawnym na dzień: 2024-09-06 Każda osoba, która posiada prawo jazdy wydane za granicą, a mieszka w Polsce przynajmniej od 185 dni musi wymienić je na polskie prawo jazdy. Zagraniczne prawo jazdy przestaje być ważne po 6 miesiącach od momentu uzyskania stałego lub czasowego pobytu w Polsce. Dotyczy to także praw jazdy wydanych w Wielkiej Brytanii po dniu 31 grudnia 2020 r. Obowiązek wymiany prawa jazdy nie dotyczy jednak osób, które posiadają:</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/wymien-prawo-jazdy</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Przeprowadzasz się lub zmieniasz nazwisko i twoje prawo jazdy jest nieważne? Wymień je. Sprawdź, jak to zrobić. Rozwiń tekst Kto musi wymienić Każdy, kto zmienił: imię lub nazwisko. Każdy, kogo: prawo jazdy straciło ważność, kategoria prawa jazdy straciła ważność. Sprawę można też załatwić przez pełnomocnika. Dowiedz się w urzędzie, jak to zrobić. Sprawę można też załatwić przez pełnomocnika. Dowiedz się w urzędzie, jak to zrobić.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Jakie są wymagania językowe dotyczące uzyskania obywatelstwa w Polskim?</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://archiwum.mswia.gov.pl/pl/bezpieczenstwo/obywatelstwo-i-repatri/cudzoziemcy/10169,SPOSOBY-NABYCIA-OBYWATELSTWA-POLSKIEGO.html</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Zagadnienia nabycia obywatelstwa polskiego i jego utraty reguluje ustawa z dnia 2 kwietnia 2009 roku o obywatelstwie polskim . Ustawa zawiera dwie podstawowe zasady dotyczące obywatelstwa polskiego. Wyrażona w art. 2 ustawy zasada ciągłości obywatelstwa polskiego gwarantuje trwałość obywatelstwa w czasie, począwszy od momentu jego nabycia, zgodnie z obowiązującymi w tym czasie przepisami, niezależnie od zmian, jakim podlega ustawodawstwo dotyczące obywatelstwa. Oznacza to, iż osoby, które nabyły obywatelstwo polskie na podstawie dawnych przepisów, następnie uchylonych lub zmienionych, jeśli obywatelstwa polskiego nie utraciły, zachowują je zgodnie z przepisami obowiązującymi w dacie jego nabycia. Zasada ta jest równocześnie dyrektywą dla właściwych organów administracji publicznej w postępowaniu o potwierdzenie posiadania lub utraty obywatelstwa polskiego. Natomiast wprowadzona przepisem art. 3 ustawy, zasada wyłączności obywatelstwa polskiego wiąże się ściśle z problemem podwójnego obywatelstwa, tworzy bowiem jasną dyrektywę kolizyjną w przypadku jego zaistnienia i pozwala na usuwanie jego niekorzystnych skutków. Projekt ustawy przyjmuje zasadę dopuszczalności wielości obywatelstw przy utrzymaniu bezwzględnego priorytetu obywatelstwa polskiego. Obywatel polski może posiadać równocześnie obywatelstwo polskie i obywatelstwo państwa obcego, ale nawet wówczas posiada wobec Rzeczypospolitej Polskiej takie same prawa i obowiązki, jak osoba posiadająca wyłącznie obywatelstwo polskie, tj. nie może wobec władz polskich powoływać się ze skutkiem prawnym na posiadane równocześnie obywatelstwo obce lub na wynikające z niego prawa i obowiązki. Urodzenie z rodziców, z których co najmniej jedno posiada obywatelstwo polskie – Zasada krwi/Ius Sanguinis</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/mswia/uzyskaj-polskie-obywatelstwo</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Potwierdzenie posiadania lub utraty obywatelstwa polskiego Chcesz dostać polskie obywatelstwo? Utraciłeś polskie obywatelstwo i chcesz je odzyskać? Potrzebujesz urzędowego potwierdzenia, że masz polskie obywatelstwo? Tutaj znajdziesz wszystkie potrzebne informacje. Złóż wniosek do Prezydenta o nadanie polskiego obywatelstwa</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/dolnoslaski-uw/uznanie-za-obywatela-polskiego</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Uzyskać polskie obywatelstwo w trybie decyzji administracyjnej wydanej przez Wojewodę Dolnośląskiego. cudzoziemca przebywającego nieprzerwanie na terytorium Rzeczypospolitej Polskiej co najmniej od 3 lat na podstawie zezwolenia na pobyt stały, zezwolenia na pobyt rezydenta długoterminowego Unii Europejskiej lub prawa stałego pobytu, który posiada w Rzeczypospolitej Polskiej stabilne i regularne źródło dochodu oraz tytuł prawny do zajmowania lokalu mieszkalnego lub cudzoziemca przebywającego nieprzerwanie na terytorium Rzeczypospolitej Polskiej co najmniej od 2 lat na podstawie zezwolenia na pobyt stały, zezwolenia na pobyt rezydenta długoterminowego Unii Europejskiej lub prawa stałego pobytu, który: pozostaje co najmniej od 3 lat w związku małżeńskim zawartym z obywatelem polskim lub nie posiada żadnego obywatelstwa, lub</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Jak założyć firmę w Polsce jako cudzoziemiec?</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00806</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Kto może prowadzić działalność gospodarczą w Polsce Obywatele państw członkowskich Unii Europejskiej oraz Europejskiego Obszaru Gospodarczego, którzy chcą wykonywać w Polsce działalność gospodarczą, mogą: założyć własną firmę jednoosobową lub dowolną spółkę handlową</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00806#2</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Kto może prowadzić działalność gospodarczą w Polsce Obywatele państw członkowskich Unii Europejskiej oraz Europejskiego Obszaru Gospodarczego, którzy chcą wykonywać w Polsce działalność gospodarczą, mogą: założyć własną firmę jednoosobową lub dowolną spółkę handlową</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00806#4</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Kto może prowadzić działalność gospodarczą w Polsce Obywatele państw członkowskich Unii Europejskiej oraz Europejskiego Obszaru Gospodarczego, którzy chcą wykonywać w Polsce działalność gospodarczą, mogą: założyć własną firmę jednoosobową lub dowolną spółkę handlową</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Jak mogę odzyskać kaucję za wynajem w Polskim?</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/ochrona-praw-lokatorow-mieszkaniowy-zasob-gminy-i-zmiana-kodeksu-16903658/art-6</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Art. 6. - - Ochrona praw lokatorów, mieszkaniowy zasób gminy i zmiana Kodeksu cywilnego. Jeżeli chcesz mieć dostęp do wszystkich dokumentów powiązanych, zaloguj się do LEX-a Nie korzystasz jeszcze z programów LEX? Zamów dostęp testowy » Czy kwotę kaucji należy zwrócić na konto bankowe najemcy, jeżeli ma on zaległości z tytułu najmu lokalu, w tym zaległości z tytułu należności czynszowych?</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/kaucja-8433</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Informacje zgodne ze stanem prawnym na dzień: 2023-10-11 W przypadku umowy najmu w Wielkiej Brytanii obowiązuje zazwyczaj zwrotna kaucja/depozyt , którą otrzymujemy, zwracając klucze do mieszkania. Zazwyczaj jest ona równa trzymiesięcznej wysokości najmu, choć zdarzają się i jedno- lub dwumiesięczne. Depozyt, który wpłacaliśmy, podpisując umowę, znacznie łatwiej odzyskać w całości w przypadku wynajmowania mieszkania prywatnie. Nieco trudniejsze jest odzyskanie 100 proc. wpłaconej sumy w przypadku wynajmowania mieszkania bądź pokoju przez agencję. Właściciel bądź agencja mają prawo odliczyć sobie z depozytu koszta zniszczeń dokonanych przez wynajmujących bądź niepokrytych przez nich rachunków. W wielu wypadkach dochodzi wręcz do liczenia każdej usterki, która nie jest zawarta w protokole dołączanym zazwyczaj do umowy najmu.</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>https://www.prawo.pl/prawo/problemy-z-najmem-okazjonalnym,513120.html</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Najem okazjonalny - niezapłacone rachunki można pokryć z kaucji Najem okazjonalny - niezapłacone rachunki można pokryć z kaucji Umowa najmu okazjonalnego wydaje się być rozwiązaniem odpowiednim dla wielu stron takich kontraktów. Jawi się jako rozwiązanie bezpieczne szczególnie dla wynajmujących, który mogą liczyć na to, że najemca w razie problemów dobrowolnie opuści zajmowany lokal, skoro powinien on wskazać inny adres, pod który może się wyprowadzić z najmowanego mieszkania.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Gdzie mogę znaleźć darmową pomoc prawną w Polskim?</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/skorzystaj-z-darmowej-pomocy-prawnej</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Skorzystaj z nieodpłatnych porad prawnych, obywatelskich i mediacji Potrzebujesz pomocy prawnika, doradcy obywatelskiego, mediatora? Jesteś w trudnej życiowej sytuacji, na przykład potrzebujesz pomocy w rozłożeniu długu na raty, w spłacie pożyczek „chwilówek”, masz kłopoty mieszkaniowe, napotkałeś trudności ze znalezieniem pracy, nie wiesz do jakiego urzędu pójść po pomoc, masz inne problemy związane ze sprawami życia codziennego? Udaj się po poradę obywatelską.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/nieodplatna-pomoc</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Nieodpłatna pomoc prawna, porady obywatelskie i mediacja są świadczone w około 1500 punktach w Polsce - w każdym powiecie Osoby ze szczególnymi potrzebami Dowiedz się więcej</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/nieodplatna-pomoc/dyzury-specjalistyczne</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Z początkiem 2022 roku w wybranych punktach nieodpłatnej pomocy prawnej i nieodpłatnego poradnictwa obywatelskiego zostały uruchomione dyżury o określonej specjalizacji. Specjalizacją jest wskazanie dziedziny prawa lub innej problematyki, której dotyczy porada albo grupy osób uprawnionych do pomocy. Dyżury specjalistyczne to wyodrębnione dyżury w istniejących punktach z dodatkowo określoną specjalizacją. Wprowadzenie punktów specjalistycznych umożliwia zaoferowanie i wykorzystanie wiedzy i doświadczenia prawników nieodpłatnej pomocy oraz doradców obywatelskich ze wskazaniem ich specjalizacji. Beneficjent pomocy może odnaleźć specjalistę w interesującej go dziedzinie. Analiza tematyki porad przeprowadzonych w poprzednich latach pozwoliła na zidentyfikowanie najistotniejszych dla beneficjentów nieodpłatnej pomocy dziedzin prawa. Należą do nich m.in. pomoc rodzinom wychowującym dzieci z niepełnosprawnością oraz pomoc ofiarom przemocy wobec kobiet i dzieci. Punkty o takich właśnie specjalizacjach zostały utworzone obok punktów specjalizujących się w prawie spadkowym, kredytach frankowych, ubezpieczeniach, podatkach czy upadłości konsumenckiej.</t>
         </is>
       </c>
     </row>

</xml_diff>